<commit_message>
Did First Three questions of Getting_Started
</commit_message>
<xml_diff>
--- a/Level_1/First Job Program With Web Development.xlsx
+++ b/Level_1/First Job Program With Web Development.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aryan\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\Nados\LearnDSA\Level_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1937B11F-4321-4D1C-9000-78FE202EB15A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{835ACE8E-6FAB-411F-83F0-C00F8E17CB96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,12 +20,21 @@
     <sheet name="Puzzles" sheetId="5" r:id="rId5"/>
     <sheet name="Guesstimates" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1213" uniqueCount="1122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1214" uniqueCount="1123">
   <si>
     <t>Print Z</t>
   </si>
@@ -3410,11 +3419,17 @@
   <si>
     <t>Easy</t>
   </si>
+  <si>
+    <t>Done</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+  </numFmts>
   <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -3514,7 +3529,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3599,6 +3614,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -3664,7 +3697,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -3719,21 +3752,24 @@
     <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3745,9 +3781,11 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3968,13 +4006,14 @@
   </sheetPr>
   <dimension ref="A1:D566"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="69" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="26" customFormat="1" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -3992,7 +4031,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="32" t="s">
         <v>1119</v>
       </c>
     </row>
@@ -4000,15 +4039,22 @@
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="49" t="s">
         <v>1121</v>
+      </c>
+      <c r="C3" s="48">
+        <f>DATE(2022,2,6)</f>
+        <v>44598</v>
+      </c>
+      <c r="D3" s="47" t="s">
+        <v>1122</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="46" t="s">
+      <c r="B4" s="34" t="s">
         <v>1121</v>
       </c>
     </row>
@@ -4016,7 +4062,7 @@
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="46" t="s">
+      <c r="B5" s="34" t="s">
         <v>1121</v>
       </c>
     </row>
@@ -4024,7 +4070,7 @@
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="46" t="s">
+      <c r="B6" s="50" t="s">
         <v>1121</v>
       </c>
     </row>
@@ -4032,7 +4078,7 @@
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="46" t="s">
+      <c r="B7" s="51" t="s">
         <v>1121</v>
       </c>
     </row>
@@ -4040,7 +4086,7 @@
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="46" t="s">
+      <c r="B8" s="34" t="s">
         <v>1121</v>
       </c>
     </row>
@@ -4048,7 +4094,7 @@
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="46" t="s">
+      <c r="B9" s="34" t="s">
         <v>1121</v>
       </c>
     </row>
@@ -4056,7 +4102,7 @@
       <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="46" t="s">
+      <c r="B10" s="34" t="s">
         <v>1121</v>
       </c>
     </row>
@@ -4064,7 +4110,7 @@
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="46" t="s">
+      <c r="B11" s="34" t="s">
         <v>1121</v>
       </c>
     </row>
@@ -4072,7 +4118,7 @@
       <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="46" t="s">
+      <c r="B12" s="34" t="s">
         <v>1121</v>
       </c>
     </row>
@@ -4080,7 +4126,7 @@
       <c r="A13" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="46" t="s">
+      <c r="B13" s="34" t="s">
         <v>1121</v>
       </c>
     </row>
@@ -4088,7 +4134,7 @@
       <c r="A14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="46" t="s">
+      <c r="B14" s="34" t="s">
         <v>1121</v>
       </c>
     </row>
@@ -4096,7 +4142,7 @@
       <c r="A15" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="46" t="s">
+      <c r="B15" s="34" t="s">
         <v>1121</v>
       </c>
     </row>
@@ -4104,7 +4150,7 @@
       <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="46" t="s">
+      <c r="B16" s="34" t="s">
         <v>1121</v>
       </c>
     </row>
@@ -4112,12 +4158,12 @@
       <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="46" t="s">
+      <c r="B17" s="34" t="s">
         <v>1121</v>
       </c>
     </row>
     <row r="18" spans="1:2" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A18" s="45" t="s">
+      <c r="A18" s="33" t="s">
         <v>1120</v>
       </c>
     </row>
@@ -6851,7 +6897,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="43" t="s">
         <v>544</v>
       </c>
       <c r="B1" s="4" t="s">
@@ -6863,7 +6909,7 @@
       <c r="D1" s="2"/>
     </row>
     <row r="2" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A2" s="33"/>
+      <c r="A2" s="36"/>
       <c r="B2" s="6" t="s">
         <v>547</v>
       </c>
@@ -6873,7 +6919,7 @@
       <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A3" s="33"/>
+      <c r="A3" s="36"/>
       <c r="B3" s="6" t="s">
         <v>547</v>
       </c>
@@ -6883,7 +6929,7 @@
       <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A4" s="33"/>
+      <c r="A4" s="36"/>
       <c r="B4" s="6" t="s">
         <v>547</v>
       </c>
@@ -6893,29 +6939,29 @@
       <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A5" s="33"/>
+      <c r="A5" s="36"/>
       <c r="B5" s="6" t="s">
         <v>551</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>552</v>
       </c>
-      <c r="D5" s="34" t="s">
+      <c r="D5" s="35" t="s">
         <v>553</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A6" s="33"/>
+      <c r="A6" s="36"/>
       <c r="B6" s="6" t="s">
         <v>551</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>554</v>
       </c>
-      <c r="D6" s="33"/>
+      <c r="D6" s="36"/>
     </row>
     <row r="7" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A7" s="33"/>
+      <c r="A7" s="36"/>
       <c r="B7" s="9" t="s">
         <v>555</v>
       </c>
@@ -6925,7 +6971,7 @@
       <c r="D7" s="10"/>
     </row>
     <row r="8" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A8" s="33"/>
+      <c r="A8" s="36"/>
       <c r="B8" s="2" t="s">
         <v>557</v>
       </c>
@@ -6935,39 +6981,39 @@
       <c r="D8" s="10"/>
     </row>
     <row r="9" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A9" s="33"/>
+      <c r="A9" s="36"/>
       <c r="B9" s="6" t="s">
         <v>559</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>560</v>
       </c>
-      <c r="D9" s="34" t="s">
+      <c r="D9" s="35" t="s">
         <v>561</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A10" s="33"/>
+      <c r="A10" s="36"/>
       <c r="B10" s="6" t="s">
         <v>559</v>
       </c>
       <c r="C10" s="12" t="s">
         <v>562</v>
       </c>
-      <c r="D10" s="33"/>
+      <c r="D10" s="36"/>
     </row>
     <row r="11" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A11" s="33"/>
+      <c r="A11" s="36"/>
       <c r="B11" s="6" t="s">
         <v>559</v>
       </c>
       <c r="C11" s="12" t="s">
         <v>563</v>
       </c>
-      <c r="D11" s="33"/>
+      <c r="D11" s="36"/>
     </row>
     <row r="12" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A12" s="33"/>
+      <c r="A12" s="36"/>
       <c r="B12" s="9" t="s">
         <v>564</v>
       </c>
@@ -6977,39 +7023,39 @@
       <c r="D12" s="10"/>
     </row>
     <row r="13" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A13" s="33"/>
+      <c r="A13" s="36"/>
       <c r="B13" s="6" t="s">
         <v>566</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>567</v>
       </c>
-      <c r="D13" s="34" t="s">
+      <c r="D13" s="35" t="s">
         <v>568</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A14" s="33"/>
+      <c r="A14" s="36"/>
       <c r="B14" s="6" t="s">
         <v>566</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>569</v>
       </c>
-      <c r="D14" s="33"/>
+      <c r="D14" s="36"/>
     </row>
     <row r="15" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A15" s="33"/>
+      <c r="A15" s="36"/>
       <c r="B15" s="6" t="s">
         <v>566</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>569</v>
       </c>
-      <c r="D15" s="33"/>
+      <c r="D15" s="36"/>
     </row>
     <row r="16" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A16" s="33"/>
+      <c r="A16" s="36"/>
       <c r="B16" s="9" t="s">
         <v>570</v>
       </c>
@@ -7019,7 +7065,7 @@
       <c r="D16" s="2"/>
     </row>
     <row r="17" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A17" s="33"/>
+      <c r="A17" s="36"/>
       <c r="B17" s="6" t="s">
         <v>566</v>
       </c>
@@ -7029,7 +7075,7 @@
       <c r="D17" s="10"/>
     </row>
     <row r="18" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A18" s="33"/>
+      <c r="A18" s="36"/>
       <c r="B18" s="6" t="s">
         <v>566</v>
       </c>
@@ -7039,7 +7085,7 @@
       <c r="D18" s="10"/>
     </row>
     <row r="19" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A19" s="33"/>
+      <c r="A19" s="36"/>
       <c r="B19" s="9" t="s">
         <v>574</v>
       </c>
@@ -7049,7 +7095,7 @@
       <c r="D19" s="10"/>
     </row>
     <row r="20" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A20" s="33"/>
+      <c r="A20" s="36"/>
       <c r="B20" s="2" t="s">
         <v>557</v>
       </c>
@@ -7059,7 +7105,7 @@
       <c r="D20" s="10"/>
     </row>
     <row r="21" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A21" s="32" t="s">
+      <c r="A21" s="40" t="s">
         <v>577</v>
       </c>
       <c r="B21" s="6" t="s">
@@ -7071,7 +7117,7 @@
       <c r="D21" s="2"/>
     </row>
     <row r="22" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A22" s="33"/>
+      <c r="A22" s="36"/>
       <c r="B22" s="6" t="s">
         <v>578</v>
       </c>
@@ -7081,7 +7127,7 @@
       <c r="D22" s="2"/>
     </row>
     <row r="23" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A23" s="33"/>
+      <c r="A23" s="36"/>
       <c r="B23" s="6" t="s">
         <v>578</v>
       </c>
@@ -7091,7 +7137,7 @@
       <c r="D23" s="2"/>
     </row>
     <row r="24" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A24" s="33"/>
+      <c r="A24" s="36"/>
       <c r="B24" s="10" t="s">
         <v>582</v>
       </c>
@@ -7101,37 +7147,37 @@
       <c r="D24" s="2"/>
     </row>
     <row r="25" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A25" s="33"/>
+      <c r="A25" s="36"/>
       <c r="B25" s="13" t="s">
         <v>584</v>
       </c>
       <c r="C25" s="7"/>
-      <c r="D25" s="35" t="s">
+      <c r="D25" s="37" t="s">
         <v>585</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A26" s="33"/>
+      <c r="A26" s="36"/>
       <c r="B26" s="6" t="s">
         <v>584</v>
       </c>
       <c r="C26" s="7" t="s">
         <v>586</v>
       </c>
-      <c r="D26" s="36"/>
+      <c r="D26" s="38"/>
     </row>
     <row r="27" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A27" s="33"/>
+      <c r="A27" s="36"/>
       <c r="B27" s="6" t="s">
         <v>584</v>
       </c>
       <c r="C27" s="7" t="s">
         <v>587</v>
       </c>
-      <c r="D27" s="37"/>
+      <c r="D27" s="39"/>
     </row>
     <row r="28" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A28" s="33"/>
+      <c r="A28" s="36"/>
       <c r="B28" s="2" t="s">
         <v>582</v>
       </c>
@@ -7141,39 +7187,39 @@
       <c r="D28" s="2"/>
     </row>
     <row r="29" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A29" s="33"/>
+      <c r="A29" s="36"/>
       <c r="B29" s="6" t="s">
         <v>589</v>
       </c>
       <c r="C29" s="7" t="s">
         <v>590</v>
       </c>
-      <c r="D29" s="34" t="s">
+      <c r="D29" s="35" t="s">
         <v>591</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A30" s="33"/>
+      <c r="A30" s="36"/>
       <c r="B30" s="6" t="s">
         <v>589</v>
       </c>
       <c r="C30" s="7" t="s">
         <v>592</v>
       </c>
-      <c r="D30" s="33"/>
+      <c r="D30" s="36"/>
     </row>
     <row r="31" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A31" s="33"/>
+      <c r="A31" s="36"/>
       <c r="B31" s="6" t="s">
         <v>589</v>
       </c>
       <c r="C31" s="7" t="s">
         <v>593</v>
       </c>
-      <c r="D31" s="33"/>
+      <c r="D31" s="36"/>
     </row>
     <row r="32" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A32" s="33"/>
+      <c r="A32" s="36"/>
       <c r="B32" s="6" t="s">
         <v>594</v>
       </c>
@@ -7183,7 +7229,7 @@
       <c r="D32" s="2"/>
     </row>
     <row r="33" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A33" s="33"/>
+      <c r="A33" s="36"/>
       <c r="B33" s="2" t="s">
         <v>596</v>
       </c>
@@ -7193,39 +7239,39 @@
       <c r="D33" s="2"/>
     </row>
     <row r="34" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A34" s="33"/>
+      <c r="A34" s="36"/>
       <c r="B34" s="6" t="s">
         <v>598</v>
       </c>
       <c r="C34" s="7" t="s">
         <v>599</v>
       </c>
-      <c r="D34" s="35" t="s">
+      <c r="D34" s="37" t="s">
         <v>600</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A35" s="33"/>
+      <c r="A35" s="36"/>
       <c r="B35" s="6" t="s">
         <v>598</v>
       </c>
       <c r="C35" s="7" t="s">
         <v>601</v>
       </c>
-      <c r="D35" s="36"/>
+      <c r="D35" s="38"/>
     </row>
     <row r="36" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A36" s="33"/>
+      <c r="A36" s="36"/>
       <c r="B36" s="6" t="s">
         <v>598</v>
       </c>
       <c r="C36" s="7" t="s">
         <v>602</v>
       </c>
-      <c r="D36" s="37"/>
+      <c r="D36" s="39"/>
     </row>
     <row r="37" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A37" s="33"/>
+      <c r="A37" s="36"/>
       <c r="B37" s="6" t="s">
         <v>598</v>
       </c>
@@ -7235,7 +7281,7 @@
       <c r="D37" s="2"/>
     </row>
     <row r="38" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A38" s="33"/>
+      <c r="A38" s="36"/>
       <c r="B38" s="2" t="s">
         <v>582</v>
       </c>
@@ -7245,7 +7291,7 @@
       <c r="D38" s="2"/>
     </row>
     <row r="39" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A39" s="33"/>
+      <c r="A39" s="36"/>
       <c r="B39" s="9" t="s">
         <v>605</v>
       </c>
@@ -7255,7 +7301,7 @@
       <c r="D39" s="2"/>
     </row>
     <row r="40" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A40" s="39" t="s">
+      <c r="A40" s="41" t="s">
         <v>607</v>
       </c>
       <c r="B40" s="6" t="s">
@@ -7267,7 +7313,7 @@
       <c r="D40" s="2"/>
     </row>
     <row r="41" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A41" s="33"/>
+      <c r="A41" s="36"/>
       <c r="B41" s="6" t="s">
         <v>608</v>
       </c>
@@ -7277,7 +7323,7 @@
       <c r="D41" s="2"/>
     </row>
     <row r="42" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A42" s="33"/>
+      <c r="A42" s="36"/>
       <c r="B42" s="6" t="s">
         <v>608</v>
       </c>
@@ -7287,51 +7333,51 @@
       <c r="D42" s="2"/>
     </row>
     <row r="43" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A43" s="33"/>
+      <c r="A43" s="36"/>
       <c r="B43" s="6" t="s">
         <v>612</v>
       </c>
       <c r="C43" s="7"/>
-      <c r="D43" s="34" t="s">
+      <c r="D43" s="35" t="s">
         <v>613</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A44" s="33"/>
+      <c r="A44" s="36"/>
       <c r="B44" s="6" t="s">
         <v>612</v>
       </c>
       <c r="C44" s="7"/>
-      <c r="D44" s="33"/>
+      <c r="D44" s="36"/>
     </row>
     <row r="45" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A45" s="33"/>
+      <c r="A45" s="36"/>
       <c r="B45" s="6" t="s">
         <v>612</v>
       </c>
       <c r="C45" s="7"/>
-      <c r="D45" s="33"/>
+      <c r="D45" s="36"/>
     </row>
     <row r="46" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A46" s="33"/>
+      <c r="A46" s="36"/>
       <c r="B46" s="6" t="s">
         <v>612</v>
       </c>
       <c r="C46" s="7"/>
-      <c r="D46" s="33"/>
+      <c r="D46" s="36"/>
     </row>
     <row r="47" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A47" s="33"/>
+      <c r="A47" s="36"/>
       <c r="B47" s="6" t="s">
         <v>614</v>
       </c>
       <c r="C47" s="7" t="s">
         <v>615</v>
       </c>
-      <c r="D47" s="33"/>
+      <c r="D47" s="36"/>
     </row>
     <row r="48" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A48" s="33"/>
+      <c r="A48" s="36"/>
       <c r="B48" s="6" t="s">
         <v>614</v>
       </c>
@@ -7341,7 +7387,7 @@
       <c r="D48" s="2"/>
     </row>
     <row r="49" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A49" s="33"/>
+      <c r="A49" s="36"/>
       <c r="B49" s="6" t="s">
         <v>614</v>
       </c>
@@ -7351,7 +7397,7 @@
       <c r="D49" s="2"/>
     </row>
     <row r="50" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A50" s="33"/>
+      <c r="A50" s="36"/>
       <c r="B50" s="2" t="s">
         <v>618</v>
       </c>
@@ -7359,57 +7405,57 @@
       <c r="D50" s="2"/>
     </row>
     <row r="51" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A51" s="33"/>
+      <c r="A51" s="36"/>
       <c r="B51" s="6" t="s">
         <v>619</v>
       </c>
       <c r="C51" s="7"/>
-      <c r="D51" s="35" t="s">
+      <c r="D51" s="37" t="s">
         <v>620</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A52" s="33"/>
+      <c r="A52" s="36"/>
       <c r="B52" s="6" t="s">
         <v>619</v>
       </c>
       <c r="C52" s="7"/>
-      <c r="D52" s="36"/>
+      <c r="D52" s="38"/>
     </row>
     <row r="53" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A53" s="33"/>
+      <c r="A53" s="36"/>
       <c r="B53" s="6" t="s">
         <v>619</v>
       </c>
       <c r="C53" s="7"/>
-      <c r="D53" s="36"/>
+      <c r="D53" s="38"/>
     </row>
     <row r="54" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A54" s="33"/>
+      <c r="A54" s="36"/>
       <c r="B54" s="6" t="s">
         <v>619</v>
       </c>
       <c r="C54" s="7"/>
-      <c r="D54" s="36"/>
+      <c r="D54" s="38"/>
     </row>
     <row r="55" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A55" s="33"/>
+      <c r="A55" s="36"/>
       <c r="B55" s="6" t="s">
         <v>619</v>
       </c>
       <c r="C55" s="7"/>
-      <c r="D55" s="36"/>
+      <c r="D55" s="38"/>
     </row>
     <row r="56" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A56" s="33"/>
+      <c r="A56" s="36"/>
       <c r="B56" s="6" t="s">
         <v>619</v>
       </c>
       <c r="C56" s="7"/>
-      <c r="D56" s="37"/>
+      <c r="D56" s="39"/>
     </row>
     <row r="57" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A57" s="33"/>
+      <c r="A57" s="36"/>
       <c r="B57" s="6" t="s">
         <v>621</v>
       </c>
@@ -7419,7 +7465,7 @@
       <c r="D57" s="2"/>
     </row>
     <row r="58" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A58" s="33"/>
+      <c r="A58" s="36"/>
       <c r="B58" s="6" t="s">
         <v>621</v>
       </c>
@@ -7429,7 +7475,7 @@
       <c r="D58" s="2"/>
     </row>
     <row r="59" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A59" s="33"/>
+      <c r="A59" s="36"/>
       <c r="B59" s="6" t="s">
         <v>621</v>
       </c>
@@ -7441,33 +7487,33 @@
       </c>
     </row>
     <row r="60" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A60" s="33"/>
+      <c r="A60" s="36"/>
       <c r="B60" s="6" t="s">
         <v>626</v>
       </c>
       <c r="C60" s="7"/>
-      <c r="D60" s="34" t="s">
+      <c r="D60" s="35" t="s">
         <v>627</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A61" s="33"/>
+      <c r="A61" s="36"/>
       <c r="B61" s="6" t="s">
         <v>626</v>
       </c>
       <c r="C61" s="7"/>
-      <c r="D61" s="33"/>
+      <c r="D61" s="36"/>
     </row>
     <row r="62" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A62" s="33"/>
+      <c r="A62" s="36"/>
       <c r="B62" s="6" t="s">
         <v>626</v>
       </c>
       <c r="C62" s="7"/>
-      <c r="D62" s="33"/>
+      <c r="D62" s="36"/>
     </row>
     <row r="63" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A63" s="33"/>
+      <c r="A63" s="36"/>
       <c r="B63" s="6" t="s">
         <v>626</v>
       </c>
@@ -7475,7 +7521,7 @@
       <c r="D63" s="8"/>
     </row>
     <row r="64" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A64" s="40" t="s">
+      <c r="A64" s="42" t="s">
         <v>628</v>
       </c>
       <c r="B64" s="9" t="s">
@@ -7485,7 +7531,7 @@
       <c r="D64" s="8"/>
     </row>
     <row r="65" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A65" s="33"/>
+      <c r="A65" s="36"/>
       <c r="B65" s="9" t="s">
         <v>629</v>
       </c>
@@ -7493,7 +7539,7 @@
       <c r="D65" s="2"/>
     </row>
     <row r="66" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A66" s="33"/>
+      <c r="A66" s="36"/>
       <c r="B66" s="9" t="s">
         <v>629</v>
       </c>
@@ -7501,7 +7547,7 @@
       <c r="D66" s="2"/>
     </row>
     <row r="67" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A67" s="33"/>
+      <c r="A67" s="36"/>
       <c r="B67" s="9" t="s">
         <v>629</v>
       </c>
@@ -7509,7 +7555,7 @@
       <c r="D67" s="2"/>
     </row>
     <row r="68" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A68" s="33"/>
+      <c r="A68" s="36"/>
       <c r="B68" s="9" t="s">
         <v>630</v>
       </c>
@@ -7517,7 +7563,7 @@
       <c r="D68" s="2"/>
     </row>
     <row r="69" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A69" s="33"/>
+      <c r="A69" s="36"/>
       <c r="B69" s="9" t="s">
         <v>630</v>
       </c>
@@ -7525,7 +7571,7 @@
       <c r="D69" s="2"/>
     </row>
     <row r="70" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A70" s="33"/>
+      <c r="A70" s="36"/>
       <c r="B70" s="9" t="s">
         <v>630</v>
       </c>
@@ -7533,7 +7579,7 @@
       <c r="D70" s="2"/>
     </row>
     <row r="71" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A71" s="33"/>
+      <c r="A71" s="36"/>
       <c r="B71" s="9" t="s">
         <v>630</v>
       </c>
@@ -7541,7 +7587,7 @@
       <c r="D71" s="2"/>
     </row>
     <row r="72" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A72" s="33"/>
+      <c r="A72" s="36"/>
       <c r="B72" s="9" t="s">
         <v>631</v>
       </c>
@@ -7549,7 +7595,7 @@
       <c r="D72" s="2"/>
     </row>
     <row r="73" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A73" s="33"/>
+      <c r="A73" s="36"/>
       <c r="B73" s="9" t="s">
         <v>631</v>
       </c>
@@ -7557,7 +7603,7 @@
       <c r="D73" s="2"/>
     </row>
     <row r="74" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A74" s="33"/>
+      <c r="A74" s="36"/>
       <c r="B74" s="9" t="s">
         <v>631</v>
       </c>
@@ -7565,7 +7611,7 @@
       <c r="D74" s="2"/>
     </row>
     <row r="75" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A75" s="41" t="s">
+      <c r="A75" s="44" t="s">
         <v>632</v>
       </c>
       <c r="B75" s="6" t="s">
@@ -7574,32 +7620,32 @@
       <c r="C75" s="7" t="s">
         <v>634</v>
       </c>
-      <c r="D75" s="34" t="s">
+      <c r="D75" s="35" t="s">
         <v>635</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A76" s="33"/>
+      <c r="A76" s="36"/>
       <c r="B76" s="6" t="s">
         <v>633</v>
       </c>
       <c r="C76" s="7" t="s">
         <v>636</v>
       </c>
-      <c r="D76" s="33"/>
+      <c r="D76" s="36"/>
     </row>
     <row r="77" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A77" s="33"/>
+      <c r="A77" s="36"/>
       <c r="B77" s="6" t="s">
         <v>633</v>
       </c>
       <c r="C77" s="7" t="s">
         <v>637</v>
       </c>
-      <c r="D77" s="33"/>
+      <c r="D77" s="36"/>
     </row>
     <row r="78" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A78" s="33"/>
+      <c r="A78" s="36"/>
       <c r="B78" s="6" t="s">
         <v>633</v>
       </c>
@@ -7609,7 +7655,7 @@
       <c r="D78" s="2"/>
     </row>
     <row r="79" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A79" s="33"/>
+      <c r="A79" s="36"/>
       <c r="B79" s="6" t="s">
         <v>633</v>
       </c>
@@ -7619,7 +7665,7 @@
       <c r="D79" s="2"/>
     </row>
     <row r="80" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A80" s="33"/>
+      <c r="A80" s="36"/>
       <c r="B80" s="6" t="s">
         <v>633</v>
       </c>
@@ -7629,7 +7675,7 @@
       <c r="D80" s="2"/>
     </row>
     <row r="81" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A81" s="33"/>
+      <c r="A81" s="36"/>
       <c r="B81" s="6" t="s">
         <v>633</v>
       </c>
@@ -7639,7 +7685,7 @@
       <c r="D81" s="2"/>
     </row>
     <row r="82" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A82" s="33"/>
+      <c r="A82" s="36"/>
       <c r="B82" s="6" t="s">
         <v>633</v>
       </c>
@@ -7649,7 +7695,7 @@
       <c r="D82" s="2"/>
     </row>
     <row r="83" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A83" s="33"/>
+      <c r="A83" s="36"/>
       <c r="B83" s="6" t="s">
         <v>633</v>
       </c>
@@ -7659,7 +7705,7 @@
       <c r="D83" s="2"/>
     </row>
     <row r="84" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A84" s="33"/>
+      <c r="A84" s="36"/>
       <c r="B84" s="6" t="s">
         <v>633</v>
       </c>
@@ -7669,7 +7715,7 @@
       <c r="D84" s="2"/>
     </row>
     <row r="85" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A85" s="33"/>
+      <c r="A85" s="36"/>
       <c r="B85" s="6" t="s">
         <v>633</v>
       </c>
@@ -7679,7 +7725,7 @@
       <c r="D85" s="2"/>
     </row>
     <row r="86" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A86" s="33"/>
+      <c r="A86" s="36"/>
       <c r="B86" s="6" t="s">
         <v>633</v>
       </c>
@@ -7689,7 +7735,7 @@
       <c r="D86" s="2"/>
     </row>
     <row r="87" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A87" s="33"/>
+      <c r="A87" s="36"/>
       <c r="B87" s="6" t="s">
         <v>647</v>
       </c>
@@ -7699,7 +7745,7 @@
       <c r="D87" s="2"/>
     </row>
     <row r="88" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A88" s="33"/>
+      <c r="A88" s="36"/>
       <c r="B88" s="6" t="s">
         <v>647</v>
       </c>
@@ -7709,7 +7755,7 @@
       <c r="D88" s="2"/>
     </row>
     <row r="89" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A89" s="33"/>
+      <c r="A89" s="36"/>
       <c r="B89" s="6" t="s">
         <v>647</v>
       </c>
@@ -7719,7 +7765,7 @@
       <c r="D89" s="2"/>
     </row>
     <row r="90" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A90" s="33"/>
+      <c r="A90" s="36"/>
       <c r="B90" s="6" t="s">
         <v>647</v>
       </c>
@@ -7729,7 +7775,7 @@
       <c r="D90" s="2"/>
     </row>
     <row r="91" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A91" s="33"/>
+      <c r="A91" s="36"/>
       <c r="B91" s="6" t="s">
         <v>647</v>
       </c>
@@ -7739,7 +7785,7 @@
       <c r="D91" s="10"/>
     </row>
     <row r="92" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A92" s="33"/>
+      <c r="A92" s="36"/>
       <c r="B92" s="14" t="s">
         <v>647</v>
       </c>
@@ -7749,7 +7795,7 @@
       <c r="D92" s="10"/>
     </row>
     <row r="93" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A93" s="33"/>
+      <c r="A93" s="36"/>
       <c r="B93" s="6" t="s">
         <v>647</v>
       </c>
@@ -7759,7 +7805,7 @@
       <c r="D93" s="2"/>
     </row>
     <row r="94" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A94" s="33"/>
+      <c r="A94" s="36"/>
       <c r="B94" s="6" t="s">
         <v>647</v>
       </c>
@@ -7769,7 +7815,7 @@
       <c r="D94" s="2"/>
     </row>
     <row r="95" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A95" s="33"/>
+      <c r="A95" s="36"/>
       <c r="B95" s="6" t="s">
         <v>647</v>
       </c>
@@ -7779,7 +7825,7 @@
       <c r="D95" s="2"/>
     </row>
     <row r="96" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A96" s="33"/>
+      <c r="A96" s="36"/>
       <c r="B96" s="6" t="s">
         <v>657</v>
       </c>
@@ -7789,7 +7835,7 @@
       <c r="D96" s="2"/>
     </row>
     <row r="97" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A97" s="33"/>
+      <c r="A97" s="36"/>
       <c r="B97" s="6" t="s">
         <v>657</v>
       </c>
@@ -7799,7 +7845,7 @@
       <c r="D97" s="2"/>
     </row>
     <row r="98" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A98" s="33"/>
+      <c r="A98" s="36"/>
       <c r="B98" s="14" t="s">
         <v>657</v>
       </c>
@@ -7809,7 +7855,7 @@
       <c r="D98" s="2"/>
     </row>
     <row r="99" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A99" s="33"/>
+      <c r="A99" s="36"/>
       <c r="B99" s="16" t="s">
         <v>661</v>
       </c>
@@ -7817,7 +7863,7 @@
       <c r="D99" s="2"/>
     </row>
     <row r="100" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A100" s="33"/>
+      <c r="A100" s="36"/>
       <c r="B100" s="9" t="s">
         <v>661</v>
       </c>
@@ -7825,7 +7871,7 @@
       <c r="D100" s="2"/>
     </row>
     <row r="101" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A101" s="33"/>
+      <c r="A101" s="36"/>
       <c r="B101" s="9" t="s">
         <v>661</v>
       </c>
@@ -7833,7 +7879,7 @@
       <c r="D101" s="2"/>
     </row>
     <row r="102" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A102" s="33"/>
+      <c r="A102" s="36"/>
       <c r="B102" s="9" t="s">
         <v>661</v>
       </c>
@@ -7841,7 +7887,7 @@
       <c r="D102" s="2"/>
     </row>
     <row r="103" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A103" s="32" t="s">
+      <c r="A103" s="40" t="s">
         <v>662</v>
       </c>
       <c r="B103" s="6" t="s">
@@ -7853,7 +7899,7 @@
       <c r="D103" s="2"/>
     </row>
     <row r="104" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A104" s="33"/>
+      <c r="A104" s="36"/>
       <c r="B104" s="6" t="s">
         <v>663</v>
       </c>
@@ -7863,7 +7909,7 @@
       <c r="D104" s="2"/>
     </row>
     <row r="105" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A105" s="33"/>
+      <c r="A105" s="36"/>
       <c r="B105" s="6" t="s">
         <v>663</v>
       </c>
@@ -10559,22 +10605,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="D29:D31"/>
-    <mergeCell ref="D34:D36"/>
-    <mergeCell ref="A21:A39"/>
-    <mergeCell ref="A40:A63"/>
-    <mergeCell ref="A64:A74"/>
-    <mergeCell ref="A1:A20"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="D9:D11"/>
-    <mergeCell ref="D13:D15"/>
-    <mergeCell ref="D25:D27"/>
     <mergeCell ref="A103:A105"/>
     <mergeCell ref="D43:D47"/>
     <mergeCell ref="D51:D56"/>
     <mergeCell ref="D60:D62"/>
     <mergeCell ref="D75:D77"/>
     <mergeCell ref="A75:A102"/>
+    <mergeCell ref="A1:A20"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="D13:D15"/>
+    <mergeCell ref="D25:D27"/>
+    <mergeCell ref="D29:D31"/>
+    <mergeCell ref="D34:D36"/>
+    <mergeCell ref="A21:A39"/>
+    <mergeCell ref="A40:A63"/>
+    <mergeCell ref="A64:A74"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -13499,7 +13545,7 @@
       <c r="A2" s="2" t="s">
         <v>1086</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="45" t="s">
         <v>1087</v>
       </c>
     </row>
@@ -13507,31 +13553,31 @@
       <c r="A3" s="2" t="s">
         <v>1088</v>
       </c>
-      <c r="B3" s="33"/>
+      <c r="B3" s="36"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>1089</v>
       </c>
-      <c r="B4" s="33"/>
+      <c r="B4" s="36"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>1090</v>
       </c>
-      <c r="B5" s="33"/>
+      <c r="B5" s="36"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>1091</v>
       </c>
-      <c r="B6" s="33"/>
+      <c r="B6" s="36"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>1092</v>
       </c>
-      <c r="B7" s="42" t="s">
+      <c r="B7" s="45" t="s">
         <v>1093</v>
       </c>
     </row>
@@ -13539,19 +13585,19 @@
       <c r="A8" s="2" t="s">
         <v>1094</v>
       </c>
-      <c r="B8" s="33"/>
+      <c r="B8" s="36"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>1095</v>
       </c>
-      <c r="B9" s="33"/>
+      <c r="B9" s="36"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>1096</v>
       </c>
-      <c r="B10" s="42" t="s">
+      <c r="B10" s="45" t="s">
         <v>1097</v>
       </c>
     </row>
@@ -13559,25 +13605,25 @@
       <c r="A11" s="2" t="s">
         <v>1098</v>
       </c>
-      <c r="B11" s="33"/>
+      <c r="B11" s="36"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>1099</v>
       </c>
-      <c r="B12" s="33"/>
+      <c r="B12" s="36"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>1100</v>
       </c>
-      <c r="B13" s="33"/>
+      <c r="B13" s="36"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>1101</v>
       </c>
-      <c r="B14" s="42" t="s">
+      <c r="B14" s="45" t="s">
         <v>1102</v>
       </c>
     </row>
@@ -13585,61 +13631,61 @@
       <c r="A15" s="2" t="s">
         <v>1103</v>
       </c>
-      <c r="B15" s="33"/>
+      <c r="B15" s="36"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>1104</v>
       </c>
-      <c r="B16" s="33"/>
+      <c r="B16" s="36"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>1105</v>
       </c>
-      <c r="B17" s="33"/>
+      <c r="B17" s="36"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>1106</v>
       </c>
-      <c r="B18" s="33"/>
+      <c r="B18" s="36"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>1107</v>
       </c>
-      <c r="B19" s="33"/>
+      <c r="B19" s="36"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>1108</v>
       </c>
-      <c r="B20" s="33"/>
+      <c r="B20" s="36"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>1109</v>
       </c>
-      <c r="B21" s="33"/>
+      <c r="B21" s="36"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>1110</v>
       </c>
-      <c r="B22" s="33"/>
+      <c r="B22" s="36"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>1111</v>
       </c>
-      <c r="B23" s="33"/>
+      <c r="B23" s="36"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>1112</v>
       </c>
-      <c r="B24" s="43" t="s">
+      <c r="B24" s="46" t="s">
         <v>1113</v>
       </c>
     </row>
@@ -13647,7 +13693,7 @@
       <c r="A25" s="2" t="s">
         <v>1114</v>
       </c>
-      <c r="B25" s="33"/>
+      <c r="B25" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
updated FJP Excel file , did first 3 questions of GETTING_STARTED
</commit_message>
<xml_diff>
--- a/Level_1/First Job Program With Web Development.xlsx
+++ b/Level_1/First Job Program With Web Development.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\Nados\LearnDSA\Level_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{835ACE8E-6FAB-411F-83F0-C00F8E17CB96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCC87715-712C-4BDD-8020-8EF6191790DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1214" uniqueCount="1123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1216" uniqueCount="1123">
   <si>
     <t>Print Z</t>
   </si>
@@ -3428,7 +3428,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="17" x14ac:knownFonts="1">
     <font>
@@ -3755,12 +3755,23 @@
     <xf numFmtId="0" fontId="14" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="15" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3769,23 +3780,12 @@
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4007,7 +4007,7 @@
   <dimension ref="A1:D566"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4039,14 +4039,14 @@
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="49" t="s">
+      <c r="B3" s="37" t="s">
         <v>1121</v>
       </c>
-      <c r="C3" s="48">
+      <c r="C3" s="36">
         <f>DATE(2022,2,6)</f>
         <v>44598</v>
       </c>
-      <c r="D3" s="47" t="s">
+      <c r="D3" s="35" t="s">
         <v>1122</v>
       </c>
     </row>
@@ -4054,23 +4054,37 @@
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="37" t="s">
         <v>1121</v>
+      </c>
+      <c r="C4" s="36">
+        <f t="shared" ref="C4:C5" si="0">DATE(2022,2,6)</f>
+        <v>44598</v>
+      </c>
+      <c r="D4" s="35" t="s">
+        <v>1122</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="37" t="s">
         <v>1121</v>
+      </c>
+      <c r="C5" s="36">
+        <f t="shared" si="0"/>
+        <v>44598</v>
+      </c>
+      <c r="D5" s="35" t="s">
+        <v>1122</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="50" t="s">
+      <c r="B6" s="38" t="s">
         <v>1121</v>
       </c>
     </row>
@@ -4078,7 +4092,7 @@
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="51" t="s">
+      <c r="B7" s="39" t="s">
         <v>1121</v>
       </c>
     </row>
@@ -6897,7 +6911,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="47" t="s">
         <v>544</v>
       </c>
       <c r="B1" s="4" t="s">
@@ -6909,7 +6923,7 @@
       <c r="D1" s="2"/>
     </row>
     <row r="2" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A2" s="36"/>
+      <c r="A2" s="41"/>
       <c r="B2" s="6" t="s">
         <v>547</v>
       </c>
@@ -6919,7 +6933,7 @@
       <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A3" s="36"/>
+      <c r="A3" s="41"/>
       <c r="B3" s="6" t="s">
         <v>547</v>
       </c>
@@ -6929,7 +6943,7 @@
       <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A4" s="36"/>
+      <c r="A4" s="41"/>
       <c r="B4" s="6" t="s">
         <v>547</v>
       </c>
@@ -6939,29 +6953,29 @@
       <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A5" s="36"/>
+      <c r="A5" s="41"/>
       <c r="B5" s="6" t="s">
         <v>551</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>552</v>
       </c>
-      <c r="D5" s="35" t="s">
+      <c r="D5" s="42" t="s">
         <v>553</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A6" s="36"/>
+      <c r="A6" s="41"/>
       <c r="B6" s="6" t="s">
         <v>551</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>554</v>
       </c>
-      <c r="D6" s="36"/>
+      <c r="D6" s="41"/>
     </row>
     <row r="7" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A7" s="36"/>
+      <c r="A7" s="41"/>
       <c r="B7" s="9" t="s">
         <v>555</v>
       </c>
@@ -6971,7 +6985,7 @@
       <c r="D7" s="10"/>
     </row>
     <row r="8" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A8" s="36"/>
+      <c r="A8" s="41"/>
       <c r="B8" s="2" t="s">
         <v>557</v>
       </c>
@@ -6981,39 +6995,39 @@
       <c r="D8" s="10"/>
     </row>
     <row r="9" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A9" s="36"/>
+      <c r="A9" s="41"/>
       <c r="B9" s="6" t="s">
         <v>559</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>560</v>
       </c>
-      <c r="D9" s="35" t="s">
+      <c r="D9" s="42" t="s">
         <v>561</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A10" s="36"/>
+      <c r="A10" s="41"/>
       <c r="B10" s="6" t="s">
         <v>559</v>
       </c>
       <c r="C10" s="12" t="s">
         <v>562</v>
       </c>
-      <c r="D10" s="36"/>
+      <c r="D10" s="41"/>
     </row>
     <row r="11" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A11" s="36"/>
+      <c r="A11" s="41"/>
       <c r="B11" s="6" t="s">
         <v>559</v>
       </c>
       <c r="C11" s="12" t="s">
         <v>563</v>
       </c>
-      <c r="D11" s="36"/>
+      <c r="D11" s="41"/>
     </row>
     <row r="12" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A12" s="36"/>
+      <c r="A12" s="41"/>
       <c r="B12" s="9" t="s">
         <v>564</v>
       </c>
@@ -7023,39 +7037,39 @@
       <c r="D12" s="10"/>
     </row>
     <row r="13" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A13" s="36"/>
+      <c r="A13" s="41"/>
       <c r="B13" s="6" t="s">
         <v>566</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>567</v>
       </c>
-      <c r="D13" s="35" t="s">
+      <c r="D13" s="42" t="s">
         <v>568</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A14" s="36"/>
+      <c r="A14" s="41"/>
       <c r="B14" s="6" t="s">
         <v>566</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>569</v>
       </c>
-      <c r="D14" s="36"/>
+      <c r="D14" s="41"/>
     </row>
     <row r="15" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A15" s="36"/>
+      <c r="A15" s="41"/>
       <c r="B15" s="6" t="s">
         <v>566</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>569</v>
       </c>
-      <c r="D15" s="36"/>
+      <c r="D15" s="41"/>
     </row>
     <row r="16" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A16" s="36"/>
+      <c r="A16" s="41"/>
       <c r="B16" s="9" t="s">
         <v>570</v>
       </c>
@@ -7065,7 +7079,7 @@
       <c r="D16" s="2"/>
     </row>
     <row r="17" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A17" s="36"/>
+      <c r="A17" s="41"/>
       <c r="B17" s="6" t="s">
         <v>566</v>
       </c>
@@ -7075,7 +7089,7 @@
       <c r="D17" s="10"/>
     </row>
     <row r="18" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A18" s="36"/>
+      <c r="A18" s="41"/>
       <c r="B18" s="6" t="s">
         <v>566</v>
       </c>
@@ -7085,7 +7099,7 @@
       <c r="D18" s="10"/>
     </row>
     <row r="19" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A19" s="36"/>
+      <c r="A19" s="41"/>
       <c r="B19" s="9" t="s">
         <v>574</v>
       </c>
@@ -7095,7 +7109,7 @@
       <c r="D19" s="10"/>
     </row>
     <row r="20" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A20" s="36"/>
+      <c r="A20" s="41"/>
       <c r="B20" s="2" t="s">
         <v>557</v>
       </c>
@@ -7117,7 +7131,7 @@
       <c r="D21" s="2"/>
     </row>
     <row r="22" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A22" s="36"/>
+      <c r="A22" s="41"/>
       <c r="B22" s="6" t="s">
         <v>578</v>
       </c>
@@ -7127,7 +7141,7 @@
       <c r="D22" s="2"/>
     </row>
     <row r="23" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A23" s="36"/>
+      <c r="A23" s="41"/>
       <c r="B23" s="6" t="s">
         <v>578</v>
       </c>
@@ -7137,7 +7151,7 @@
       <c r="D23" s="2"/>
     </row>
     <row r="24" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A24" s="36"/>
+      <c r="A24" s="41"/>
       <c r="B24" s="10" t="s">
         <v>582</v>
       </c>
@@ -7147,37 +7161,37 @@
       <c r="D24" s="2"/>
     </row>
     <row r="25" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A25" s="36"/>
+      <c r="A25" s="41"/>
       <c r="B25" s="13" t="s">
         <v>584</v>
       </c>
       <c r="C25" s="7"/>
-      <c r="D25" s="37" t="s">
+      <c r="D25" s="43" t="s">
         <v>585</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A26" s="36"/>
+      <c r="A26" s="41"/>
       <c r="B26" s="6" t="s">
         <v>584</v>
       </c>
       <c r="C26" s="7" t="s">
         <v>586</v>
       </c>
-      <c r="D26" s="38"/>
+      <c r="D26" s="44"/>
     </row>
     <row r="27" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A27" s="36"/>
+      <c r="A27" s="41"/>
       <c r="B27" s="6" t="s">
         <v>584</v>
       </c>
       <c r="C27" s="7" t="s">
         <v>587</v>
       </c>
-      <c r="D27" s="39"/>
+      <c r="D27" s="45"/>
     </row>
     <row r="28" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A28" s="36"/>
+      <c r="A28" s="41"/>
       <c r="B28" s="2" t="s">
         <v>582</v>
       </c>
@@ -7187,39 +7201,39 @@
       <c r="D28" s="2"/>
     </row>
     <row r="29" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A29" s="36"/>
+      <c r="A29" s="41"/>
       <c r="B29" s="6" t="s">
         <v>589</v>
       </c>
       <c r="C29" s="7" t="s">
         <v>590</v>
       </c>
-      <c r="D29" s="35" t="s">
+      <c r="D29" s="42" t="s">
         <v>591</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A30" s="36"/>
+      <c r="A30" s="41"/>
       <c r="B30" s="6" t="s">
         <v>589</v>
       </c>
       <c r="C30" s="7" t="s">
         <v>592</v>
       </c>
-      <c r="D30" s="36"/>
+      <c r="D30" s="41"/>
     </row>
     <row r="31" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A31" s="36"/>
+      <c r="A31" s="41"/>
       <c r="B31" s="6" t="s">
         <v>589</v>
       </c>
       <c r="C31" s="7" t="s">
         <v>593</v>
       </c>
-      <c r="D31" s="36"/>
+      <c r="D31" s="41"/>
     </row>
     <row r="32" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A32" s="36"/>
+      <c r="A32" s="41"/>
       <c r="B32" s="6" t="s">
         <v>594</v>
       </c>
@@ -7229,7 +7243,7 @@
       <c r="D32" s="2"/>
     </row>
     <row r="33" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A33" s="36"/>
+      <c r="A33" s="41"/>
       <c r="B33" s="2" t="s">
         <v>596</v>
       </c>
@@ -7239,39 +7253,39 @@
       <c r="D33" s="2"/>
     </row>
     <row r="34" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A34" s="36"/>
+      <c r="A34" s="41"/>
       <c r="B34" s="6" t="s">
         <v>598</v>
       </c>
       <c r="C34" s="7" t="s">
         <v>599</v>
       </c>
-      <c r="D34" s="37" t="s">
+      <c r="D34" s="43" t="s">
         <v>600</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A35" s="36"/>
+      <c r="A35" s="41"/>
       <c r="B35" s="6" t="s">
         <v>598</v>
       </c>
       <c r="C35" s="7" t="s">
         <v>601</v>
       </c>
-      <c r="D35" s="38"/>
+      <c r="D35" s="44"/>
     </row>
     <row r="36" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A36" s="36"/>
+      <c r="A36" s="41"/>
       <c r="B36" s="6" t="s">
         <v>598</v>
       </c>
       <c r="C36" s="7" t="s">
         <v>602</v>
       </c>
-      <c r="D36" s="39"/>
+      <c r="D36" s="45"/>
     </row>
     <row r="37" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A37" s="36"/>
+      <c r="A37" s="41"/>
       <c r="B37" s="6" t="s">
         <v>598</v>
       </c>
@@ -7281,7 +7295,7 @@
       <c r="D37" s="2"/>
     </row>
     <row r="38" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A38" s="36"/>
+      <c r="A38" s="41"/>
       <c r="B38" s="2" t="s">
         <v>582</v>
       </c>
@@ -7291,7 +7305,7 @@
       <c r="D38" s="2"/>
     </row>
     <row r="39" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A39" s="36"/>
+      <c r="A39" s="41"/>
       <c r="B39" s="9" t="s">
         <v>605</v>
       </c>
@@ -7301,7 +7315,7 @@
       <c r="D39" s="2"/>
     </row>
     <row r="40" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A40" s="41" t="s">
+      <c r="A40" s="48" t="s">
         <v>607</v>
       </c>
       <c r="B40" s="6" t="s">
@@ -7313,7 +7327,7 @@
       <c r="D40" s="2"/>
     </row>
     <row r="41" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A41" s="36"/>
+      <c r="A41" s="41"/>
       <c r="B41" s="6" t="s">
         <v>608</v>
       </c>
@@ -7323,7 +7337,7 @@
       <c r="D41" s="2"/>
     </row>
     <row r="42" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A42" s="36"/>
+      <c r="A42" s="41"/>
       <c r="B42" s="6" t="s">
         <v>608</v>
       </c>
@@ -7333,51 +7347,51 @@
       <c r="D42" s="2"/>
     </row>
     <row r="43" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A43" s="36"/>
+      <c r="A43" s="41"/>
       <c r="B43" s="6" t="s">
         <v>612</v>
       </c>
       <c r="C43" s="7"/>
-      <c r="D43" s="35" t="s">
+      <c r="D43" s="42" t="s">
         <v>613</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A44" s="36"/>
+      <c r="A44" s="41"/>
       <c r="B44" s="6" t="s">
         <v>612</v>
       </c>
       <c r="C44" s="7"/>
-      <c r="D44" s="36"/>
+      <c r="D44" s="41"/>
     </row>
     <row r="45" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A45" s="36"/>
+      <c r="A45" s="41"/>
       <c r="B45" s="6" t="s">
         <v>612</v>
       </c>
       <c r="C45" s="7"/>
-      <c r="D45" s="36"/>
+      <c r="D45" s="41"/>
     </row>
     <row r="46" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A46" s="36"/>
+      <c r="A46" s="41"/>
       <c r="B46" s="6" t="s">
         <v>612</v>
       </c>
       <c r="C46" s="7"/>
-      <c r="D46" s="36"/>
+      <c r="D46" s="41"/>
     </row>
     <row r="47" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A47" s="36"/>
+      <c r="A47" s="41"/>
       <c r="B47" s="6" t="s">
         <v>614</v>
       </c>
       <c r="C47" s="7" t="s">
         <v>615</v>
       </c>
-      <c r="D47" s="36"/>
+      <c r="D47" s="41"/>
     </row>
     <row r="48" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A48" s="36"/>
+      <c r="A48" s="41"/>
       <c r="B48" s="6" t="s">
         <v>614</v>
       </c>
@@ -7387,7 +7401,7 @@
       <c r="D48" s="2"/>
     </row>
     <row r="49" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A49" s="36"/>
+      <c r="A49" s="41"/>
       <c r="B49" s="6" t="s">
         <v>614</v>
       </c>
@@ -7397,7 +7411,7 @@
       <c r="D49" s="2"/>
     </row>
     <row r="50" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A50" s="36"/>
+      <c r="A50" s="41"/>
       <c r="B50" s="2" t="s">
         <v>618</v>
       </c>
@@ -7405,57 +7419,57 @@
       <c r="D50" s="2"/>
     </row>
     <row r="51" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A51" s="36"/>
+      <c r="A51" s="41"/>
       <c r="B51" s="6" t="s">
         <v>619</v>
       </c>
       <c r="C51" s="7"/>
-      <c r="D51" s="37" t="s">
+      <c r="D51" s="43" t="s">
         <v>620</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A52" s="36"/>
+      <c r="A52" s="41"/>
       <c r="B52" s="6" t="s">
         <v>619</v>
       </c>
       <c r="C52" s="7"/>
-      <c r="D52" s="38"/>
+      <c r="D52" s="44"/>
     </row>
     <row r="53" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A53" s="36"/>
+      <c r="A53" s="41"/>
       <c r="B53" s="6" t="s">
         <v>619</v>
       </c>
       <c r="C53" s="7"/>
-      <c r="D53" s="38"/>
+      <c r="D53" s="44"/>
     </row>
     <row r="54" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A54" s="36"/>
+      <c r="A54" s="41"/>
       <c r="B54" s="6" t="s">
         <v>619</v>
       </c>
       <c r="C54" s="7"/>
-      <c r="D54" s="38"/>
+      <c r="D54" s="44"/>
     </row>
     <row r="55" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A55" s="36"/>
+      <c r="A55" s="41"/>
       <c r="B55" s="6" t="s">
         <v>619</v>
       </c>
       <c r="C55" s="7"/>
-      <c r="D55" s="38"/>
+      <c r="D55" s="44"/>
     </row>
     <row r="56" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A56" s="36"/>
+      <c r="A56" s="41"/>
       <c r="B56" s="6" t="s">
         <v>619</v>
       </c>
       <c r="C56" s="7"/>
-      <c r="D56" s="39"/>
+      <c r="D56" s="45"/>
     </row>
     <row r="57" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A57" s="36"/>
+      <c r="A57" s="41"/>
       <c r="B57" s="6" t="s">
         <v>621</v>
       </c>
@@ -7465,7 +7479,7 @@
       <c r="D57" s="2"/>
     </row>
     <row r="58" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A58" s="36"/>
+      <c r="A58" s="41"/>
       <c r="B58" s="6" t="s">
         <v>621</v>
       </c>
@@ -7475,7 +7489,7 @@
       <c r="D58" s="2"/>
     </row>
     <row r="59" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A59" s="36"/>
+      <c r="A59" s="41"/>
       <c r="B59" s="6" t="s">
         <v>621</v>
       </c>
@@ -7487,33 +7501,33 @@
       </c>
     </row>
     <row r="60" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A60" s="36"/>
+      <c r="A60" s="41"/>
       <c r="B60" s="6" t="s">
         <v>626</v>
       </c>
       <c r="C60" s="7"/>
-      <c r="D60" s="35" t="s">
+      <c r="D60" s="42" t="s">
         <v>627</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A61" s="36"/>
+      <c r="A61" s="41"/>
       <c r="B61" s="6" t="s">
         <v>626</v>
       </c>
       <c r="C61" s="7"/>
-      <c r="D61" s="36"/>
+      <c r="D61" s="41"/>
     </row>
     <row r="62" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A62" s="36"/>
+      <c r="A62" s="41"/>
       <c r="B62" s="6" t="s">
         <v>626</v>
       </c>
       <c r="C62" s="7"/>
-      <c r="D62" s="36"/>
+      <c r="D62" s="41"/>
     </row>
     <row r="63" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A63" s="36"/>
+      <c r="A63" s="41"/>
       <c r="B63" s="6" t="s">
         <v>626</v>
       </c>
@@ -7521,7 +7535,7 @@
       <c r="D63" s="8"/>
     </row>
     <row r="64" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A64" s="42" t="s">
+      <c r="A64" s="49" t="s">
         <v>628</v>
       </c>
       <c r="B64" s="9" t="s">
@@ -7531,7 +7545,7 @@
       <c r="D64" s="8"/>
     </row>
     <row r="65" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A65" s="36"/>
+      <c r="A65" s="41"/>
       <c r="B65" s="9" t="s">
         <v>629</v>
       </c>
@@ -7539,7 +7553,7 @@
       <c r="D65" s="2"/>
     </row>
     <row r="66" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A66" s="36"/>
+      <c r="A66" s="41"/>
       <c r="B66" s="9" t="s">
         <v>629</v>
       </c>
@@ -7547,7 +7561,7 @@
       <c r="D66" s="2"/>
     </row>
     <row r="67" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A67" s="36"/>
+      <c r="A67" s="41"/>
       <c r="B67" s="9" t="s">
         <v>629</v>
       </c>
@@ -7555,7 +7569,7 @@
       <c r="D67" s="2"/>
     </row>
     <row r="68" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A68" s="36"/>
+      <c r="A68" s="41"/>
       <c r="B68" s="9" t="s">
         <v>630</v>
       </c>
@@ -7563,7 +7577,7 @@
       <c r="D68" s="2"/>
     </row>
     <row r="69" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A69" s="36"/>
+      <c r="A69" s="41"/>
       <c r="B69" s="9" t="s">
         <v>630</v>
       </c>
@@ -7571,7 +7585,7 @@
       <c r="D69" s="2"/>
     </row>
     <row r="70" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A70" s="36"/>
+      <c r="A70" s="41"/>
       <c r="B70" s="9" t="s">
         <v>630</v>
       </c>
@@ -7579,7 +7593,7 @@
       <c r="D70" s="2"/>
     </row>
     <row r="71" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A71" s="36"/>
+      <c r="A71" s="41"/>
       <c r="B71" s="9" t="s">
         <v>630</v>
       </c>
@@ -7587,7 +7601,7 @@
       <c r="D71" s="2"/>
     </row>
     <row r="72" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A72" s="36"/>
+      <c r="A72" s="41"/>
       <c r="B72" s="9" t="s">
         <v>631</v>
       </c>
@@ -7595,7 +7609,7 @@
       <c r="D72" s="2"/>
     </row>
     <row r="73" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A73" s="36"/>
+      <c r="A73" s="41"/>
       <c r="B73" s="9" t="s">
         <v>631</v>
       </c>
@@ -7603,7 +7617,7 @@
       <c r="D73" s="2"/>
     </row>
     <row r="74" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A74" s="36"/>
+      <c r="A74" s="41"/>
       <c r="B74" s="9" t="s">
         <v>631</v>
       </c>
@@ -7611,7 +7625,7 @@
       <c r="D74" s="2"/>
     </row>
     <row r="75" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A75" s="44" t="s">
+      <c r="A75" s="46" t="s">
         <v>632</v>
       </c>
       <c r="B75" s="6" t="s">
@@ -7620,32 +7634,32 @@
       <c r="C75" s="7" t="s">
         <v>634</v>
       </c>
-      <c r="D75" s="35" t="s">
+      <c r="D75" s="42" t="s">
         <v>635</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A76" s="36"/>
+      <c r="A76" s="41"/>
       <c r="B76" s="6" t="s">
         <v>633</v>
       </c>
       <c r="C76" s="7" t="s">
         <v>636</v>
       </c>
-      <c r="D76" s="36"/>
+      <c r="D76" s="41"/>
     </row>
     <row r="77" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A77" s="36"/>
+      <c r="A77" s="41"/>
       <c r="B77" s="6" t="s">
         <v>633</v>
       </c>
       <c r="C77" s="7" t="s">
         <v>637</v>
       </c>
-      <c r="D77" s="36"/>
+      <c r="D77" s="41"/>
     </row>
     <row r="78" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A78" s="36"/>
+      <c r="A78" s="41"/>
       <c r="B78" s="6" t="s">
         <v>633</v>
       </c>
@@ -7655,7 +7669,7 @@
       <c r="D78" s="2"/>
     </row>
     <row r="79" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A79" s="36"/>
+      <c r="A79" s="41"/>
       <c r="B79" s="6" t="s">
         <v>633</v>
       </c>
@@ -7665,7 +7679,7 @@
       <c r="D79" s="2"/>
     </row>
     <row r="80" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A80" s="36"/>
+      <c r="A80" s="41"/>
       <c r="B80" s="6" t="s">
         <v>633</v>
       </c>
@@ -7675,7 +7689,7 @@
       <c r="D80" s="2"/>
     </row>
     <row r="81" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A81" s="36"/>
+      <c r="A81" s="41"/>
       <c r="B81" s="6" t="s">
         <v>633</v>
       </c>
@@ -7685,7 +7699,7 @@
       <c r="D81" s="2"/>
     </row>
     <row r="82" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A82" s="36"/>
+      <c r="A82" s="41"/>
       <c r="B82" s="6" t="s">
         <v>633</v>
       </c>
@@ -7695,7 +7709,7 @@
       <c r="D82" s="2"/>
     </row>
     <row r="83" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A83" s="36"/>
+      <c r="A83" s="41"/>
       <c r="B83" s="6" t="s">
         <v>633</v>
       </c>
@@ -7705,7 +7719,7 @@
       <c r="D83" s="2"/>
     </row>
     <row r="84" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A84" s="36"/>
+      <c r="A84" s="41"/>
       <c r="B84" s="6" t="s">
         <v>633</v>
       </c>
@@ -7715,7 +7729,7 @@
       <c r="D84" s="2"/>
     </row>
     <row r="85" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A85" s="36"/>
+      <c r="A85" s="41"/>
       <c r="B85" s="6" t="s">
         <v>633</v>
       </c>
@@ -7725,7 +7739,7 @@
       <c r="D85" s="2"/>
     </row>
     <row r="86" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A86" s="36"/>
+      <c r="A86" s="41"/>
       <c r="B86" s="6" t="s">
         <v>633</v>
       </c>
@@ -7735,7 +7749,7 @@
       <c r="D86" s="2"/>
     </row>
     <row r="87" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A87" s="36"/>
+      <c r="A87" s="41"/>
       <c r="B87" s="6" t="s">
         <v>647</v>
       </c>
@@ -7745,7 +7759,7 @@
       <c r="D87" s="2"/>
     </row>
     <row r="88" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A88" s="36"/>
+      <c r="A88" s="41"/>
       <c r="B88" s="6" t="s">
         <v>647</v>
       </c>
@@ -7755,7 +7769,7 @@
       <c r="D88" s="2"/>
     </row>
     <row r="89" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A89" s="36"/>
+      <c r="A89" s="41"/>
       <c r="B89" s="6" t="s">
         <v>647</v>
       </c>
@@ -7765,7 +7779,7 @@
       <c r="D89" s="2"/>
     </row>
     <row r="90" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A90" s="36"/>
+      <c r="A90" s="41"/>
       <c r="B90" s="6" t="s">
         <v>647</v>
       </c>
@@ -7775,7 +7789,7 @@
       <c r="D90" s="2"/>
     </row>
     <row r="91" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A91" s="36"/>
+      <c r="A91" s="41"/>
       <c r="B91" s="6" t="s">
         <v>647</v>
       </c>
@@ -7785,7 +7799,7 @@
       <c r="D91" s="10"/>
     </row>
     <row r="92" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A92" s="36"/>
+      <c r="A92" s="41"/>
       <c r="B92" s="14" t="s">
         <v>647</v>
       </c>
@@ -7795,7 +7809,7 @@
       <c r="D92" s="10"/>
     </row>
     <row r="93" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A93" s="36"/>
+      <c r="A93" s="41"/>
       <c r="B93" s="6" t="s">
         <v>647</v>
       </c>
@@ -7805,7 +7819,7 @@
       <c r="D93" s="2"/>
     </row>
     <row r="94" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A94" s="36"/>
+      <c r="A94" s="41"/>
       <c r="B94" s="6" t="s">
         <v>647</v>
       </c>
@@ -7815,7 +7829,7 @@
       <c r="D94" s="2"/>
     </row>
     <row r="95" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A95" s="36"/>
+      <c r="A95" s="41"/>
       <c r="B95" s="6" t="s">
         <v>647</v>
       </c>
@@ -7825,7 +7839,7 @@
       <c r="D95" s="2"/>
     </row>
     <row r="96" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A96" s="36"/>
+      <c r="A96" s="41"/>
       <c r="B96" s="6" t="s">
         <v>657</v>
       </c>
@@ -7835,7 +7849,7 @@
       <c r="D96" s="2"/>
     </row>
     <row r="97" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A97" s="36"/>
+      <c r="A97" s="41"/>
       <c r="B97" s="6" t="s">
         <v>657</v>
       </c>
@@ -7845,7 +7859,7 @@
       <c r="D97" s="2"/>
     </row>
     <row r="98" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A98" s="36"/>
+      <c r="A98" s="41"/>
       <c r="B98" s="14" t="s">
         <v>657</v>
       </c>
@@ -7855,7 +7869,7 @@
       <c r="D98" s="2"/>
     </row>
     <row r="99" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A99" s="36"/>
+      <c r="A99" s="41"/>
       <c r="B99" s="16" t="s">
         <v>661</v>
       </c>
@@ -7863,7 +7877,7 @@
       <c r="D99" s="2"/>
     </row>
     <row r="100" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A100" s="36"/>
+      <c r="A100" s="41"/>
       <c r="B100" s="9" t="s">
         <v>661</v>
       </c>
@@ -7871,7 +7885,7 @@
       <c r="D100" s="2"/>
     </row>
     <row r="101" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A101" s="36"/>
+      <c r="A101" s="41"/>
       <c r="B101" s="9" t="s">
         <v>661</v>
       </c>
@@ -7879,7 +7893,7 @@
       <c r="D101" s="2"/>
     </row>
     <row r="102" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A102" s="36"/>
+      <c r="A102" s="41"/>
       <c r="B102" s="9" t="s">
         <v>661</v>
       </c>
@@ -7899,7 +7913,7 @@
       <c r="D103" s="2"/>
     </row>
     <row r="104" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A104" s="36"/>
+      <c r="A104" s="41"/>
       <c r="B104" s="6" t="s">
         <v>663</v>
       </c>
@@ -7909,7 +7923,7 @@
       <c r="D104" s="2"/>
     </row>
     <row r="105" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A105" s="36"/>
+      <c r="A105" s="41"/>
       <c r="B105" s="6" t="s">
         <v>663</v>
       </c>
@@ -10605,22 +10619,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="D29:D31"/>
+    <mergeCell ref="D34:D36"/>
+    <mergeCell ref="A21:A39"/>
+    <mergeCell ref="A40:A63"/>
+    <mergeCell ref="A64:A74"/>
+    <mergeCell ref="A1:A20"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="D13:D15"/>
+    <mergeCell ref="D25:D27"/>
     <mergeCell ref="A103:A105"/>
     <mergeCell ref="D43:D47"/>
     <mergeCell ref="D51:D56"/>
     <mergeCell ref="D60:D62"/>
     <mergeCell ref="D75:D77"/>
     <mergeCell ref="A75:A102"/>
-    <mergeCell ref="A1:A20"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="D9:D11"/>
-    <mergeCell ref="D13:D15"/>
-    <mergeCell ref="D25:D27"/>
-    <mergeCell ref="D29:D31"/>
-    <mergeCell ref="D34:D36"/>
-    <mergeCell ref="A21:A39"/>
-    <mergeCell ref="A40:A63"/>
-    <mergeCell ref="A64:A74"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -13545,7 +13559,7 @@
       <c r="A2" s="2" t="s">
         <v>1086</v>
       </c>
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="50" t="s">
         <v>1087</v>
       </c>
     </row>
@@ -13553,31 +13567,31 @@
       <c r="A3" s="2" t="s">
         <v>1088</v>
       </c>
-      <c r="B3" s="36"/>
+      <c r="B3" s="41"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>1089</v>
       </c>
-      <c r="B4" s="36"/>
+      <c r="B4" s="41"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>1090</v>
       </c>
-      <c r="B5" s="36"/>
+      <c r="B5" s="41"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>1091</v>
       </c>
-      <c r="B6" s="36"/>
+      <c r="B6" s="41"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>1092</v>
       </c>
-      <c r="B7" s="45" t="s">
+      <c r="B7" s="50" t="s">
         <v>1093</v>
       </c>
     </row>
@@ -13585,19 +13599,19 @@
       <c r="A8" s="2" t="s">
         <v>1094</v>
       </c>
-      <c r="B8" s="36"/>
+      <c r="B8" s="41"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>1095</v>
       </c>
-      <c r="B9" s="36"/>
+      <c r="B9" s="41"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>1096</v>
       </c>
-      <c r="B10" s="45" t="s">
+      <c r="B10" s="50" t="s">
         <v>1097</v>
       </c>
     </row>
@@ -13605,25 +13619,25 @@
       <c r="A11" s="2" t="s">
         <v>1098</v>
       </c>
-      <c r="B11" s="36"/>
+      <c r="B11" s="41"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>1099</v>
       </c>
-      <c r="B12" s="36"/>
+      <c r="B12" s="41"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>1100</v>
       </c>
-      <c r="B13" s="36"/>
+      <c r="B13" s="41"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>1101</v>
       </c>
-      <c r="B14" s="45" t="s">
+      <c r="B14" s="50" t="s">
         <v>1102</v>
       </c>
     </row>
@@ -13631,61 +13645,61 @@
       <c r="A15" s="2" t="s">
         <v>1103</v>
       </c>
-      <c r="B15" s="36"/>
+      <c r="B15" s="41"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>1104</v>
       </c>
-      <c r="B16" s="36"/>
+      <c r="B16" s="41"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>1105</v>
       </c>
-      <c r="B17" s="36"/>
+      <c r="B17" s="41"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>1106</v>
       </c>
-      <c r="B18" s="36"/>
+      <c r="B18" s="41"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>1107</v>
       </c>
-      <c r="B19" s="36"/>
+      <c r="B19" s="41"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>1108</v>
       </c>
-      <c r="B20" s="36"/>
+      <c r="B20" s="41"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>1109</v>
       </c>
-      <c r="B21" s="36"/>
+      <c r="B21" s="41"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>1110</v>
       </c>
-      <c r="B22" s="36"/>
+      <c r="B22" s="41"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>1111</v>
       </c>
-      <c r="B23" s="36"/>
+      <c r="B23" s="41"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>1112</v>
       </c>
-      <c r="B24" s="46" t="s">
+      <c r="B24" s="51" t="s">
         <v>1113</v>
       </c>
     </row>
@@ -13693,7 +13707,7 @@
       <c r="A25" s="2" t="s">
         <v>1114</v>
       </c>
-      <c r="B25" s="36"/>
+      <c r="B25" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
updated FJP with questions i completed today 7th Feb 2022, 9:45 AM
</commit_message>
<xml_diff>
--- a/Level_1/First Job Program With Web Development.xlsx
+++ b/Level_1/First Job Program With Web Development.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\Nados\LearnDSA\Level_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCC87715-712C-4BDD-8020-8EF6191790DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F5BA858-171D-4176-AA93-E3696844A9CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1216" uniqueCount="1123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1223" uniqueCount="1123">
   <si>
     <t>Print Z</t>
   </si>
@@ -3760,24 +3760,24 @@
     <xf numFmtId="0" fontId="16" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="16" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="16" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -4007,7 +4007,7 @@
   <dimension ref="A1:D566"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4058,7 +4058,7 @@
         <v>1121</v>
       </c>
       <c r="C4" s="36">
-        <f t="shared" ref="C4:C5" si="0">DATE(2022,2,6)</f>
+        <f t="shared" ref="C4:C6" si="0">DATE(2022,2,6)</f>
         <v>44598</v>
       </c>
       <c r="D4" s="35" t="s">
@@ -4087,6 +4087,13 @@
       <c r="B6" s="38" t="s">
         <v>1121</v>
       </c>
+      <c r="C6" s="36">
+        <f>DATE(2022,2,6)+1</f>
+        <v>44599</v>
+      </c>
+      <c r="D6" s="35" t="s">
+        <v>1122</v>
+      </c>
     </row>
     <row r="7" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -4095,45 +4102,87 @@
       <c r="B7" s="39" t="s">
         <v>1121</v>
       </c>
+      <c r="C7" s="36">
+        <f>DATE(2022,2,6)+1</f>
+        <v>44599</v>
+      </c>
+      <c r="D7" s="35" t="s">
+        <v>1122</v>
+      </c>
     </row>
     <row r="8" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="37" t="s">
         <v>1121</v>
+      </c>
+      <c r="C8" s="36">
+        <f t="shared" ref="C8:C11" si="1">DATE(2022,2,6)+1</f>
+        <v>44599</v>
+      </c>
+      <c r="D8" s="35" t="s">
+        <v>1122</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="34" t="s">
+      <c r="B9" s="38" t="s">
         <v>1121</v>
+      </c>
+      <c r="C9" s="36">
+        <f t="shared" si="1"/>
+        <v>44599</v>
+      </c>
+      <c r="D9" s="35" t="s">
+        <v>1122</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="34" t="s">
+      <c r="B10" s="37" t="s">
         <v>1121</v>
+      </c>
+      <c r="C10" s="36">
+        <f t="shared" si="1"/>
+        <v>44599</v>
+      </c>
+      <c r="D10" s="35" t="s">
+        <v>1122</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="34" t="s">
+      <c r="B11" s="37" t="s">
         <v>1121</v>
+      </c>
+      <c r="C11" s="36">
+        <f t="shared" si="1"/>
+        <v>44599</v>
+      </c>
+      <c r="D11" s="35" t="s">
+        <v>1122</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="34" t="s">
+      <c r="B12" s="38" t="s">
         <v>1121</v>
+      </c>
+      <c r="C12" s="36">
+        <f>DATE(2022,2,6)+1</f>
+        <v>44599</v>
+      </c>
+      <c r="D12" s="35" t="s">
+        <v>1122</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
@@ -6911,7 +6960,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="48" t="s">
         <v>544</v>
       </c>
       <c r="B1" s="4" t="s">
@@ -6960,7 +7009,7 @@
       <c r="C5" s="7" t="s">
         <v>552</v>
       </c>
-      <c r="D5" s="42" t="s">
+      <c r="D5" s="40" t="s">
         <v>553</v>
       </c>
     </row>
@@ -7002,7 +7051,7 @@
       <c r="C9" s="7" t="s">
         <v>560</v>
       </c>
-      <c r="D9" s="42" t="s">
+      <c r="D9" s="40" t="s">
         <v>561</v>
       </c>
     </row>
@@ -7044,7 +7093,7 @@
       <c r="C13" s="7" t="s">
         <v>567</v>
       </c>
-      <c r="D13" s="42" t="s">
+      <c r="D13" s="40" t="s">
         <v>568</v>
       </c>
     </row>
@@ -7119,7 +7168,7 @@
       <c r="D20" s="10"/>
     </row>
     <row r="21" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A21" s="40" t="s">
+      <c r="A21" s="45" t="s">
         <v>577</v>
       </c>
       <c r="B21" s="6" t="s">
@@ -7166,7 +7215,7 @@
         <v>584</v>
       </c>
       <c r="C25" s="7"/>
-      <c r="D25" s="43" t="s">
+      <c r="D25" s="42" t="s">
         <v>585</v>
       </c>
     </row>
@@ -7178,7 +7227,7 @@
       <c r="C26" s="7" t="s">
         <v>586</v>
       </c>
-      <c r="D26" s="44"/>
+      <c r="D26" s="43"/>
     </row>
     <row r="27" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A27" s="41"/>
@@ -7188,7 +7237,7 @@
       <c r="C27" s="7" t="s">
         <v>587</v>
       </c>
-      <c r="D27" s="45"/>
+      <c r="D27" s="44"/>
     </row>
     <row r="28" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A28" s="41"/>
@@ -7208,7 +7257,7 @@
       <c r="C29" s="7" t="s">
         <v>590</v>
       </c>
-      <c r="D29" s="42" t="s">
+      <c r="D29" s="40" t="s">
         <v>591</v>
       </c>
     </row>
@@ -7260,7 +7309,7 @@
       <c r="C34" s="7" t="s">
         <v>599</v>
       </c>
-      <c r="D34" s="43" t="s">
+      <c r="D34" s="42" t="s">
         <v>600</v>
       </c>
     </row>
@@ -7272,7 +7321,7 @@
       <c r="C35" s="7" t="s">
         <v>601</v>
       </c>
-      <c r="D35" s="44"/>
+      <c r="D35" s="43"/>
     </row>
     <row r="36" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A36" s="41"/>
@@ -7282,7 +7331,7 @@
       <c r="C36" s="7" t="s">
         <v>602</v>
       </c>
-      <c r="D36" s="45"/>
+      <c r="D36" s="44"/>
     </row>
     <row r="37" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A37" s="41"/>
@@ -7315,7 +7364,7 @@
       <c r="D39" s="2"/>
     </row>
     <row r="40" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A40" s="48" t="s">
+      <c r="A40" s="46" t="s">
         <v>607</v>
       </c>
       <c r="B40" s="6" t="s">
@@ -7352,7 +7401,7 @@
         <v>612</v>
       </c>
       <c r="C43" s="7"/>
-      <c r="D43" s="42" t="s">
+      <c r="D43" s="40" t="s">
         <v>613</v>
       </c>
     </row>
@@ -7424,7 +7473,7 @@
         <v>619</v>
       </c>
       <c r="C51" s="7"/>
-      <c r="D51" s="43" t="s">
+      <c r="D51" s="42" t="s">
         <v>620</v>
       </c>
     </row>
@@ -7434,7 +7483,7 @@
         <v>619</v>
       </c>
       <c r="C52" s="7"/>
-      <c r="D52" s="44"/>
+      <c r="D52" s="43"/>
     </row>
     <row r="53" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A53" s="41"/>
@@ -7442,7 +7491,7 @@
         <v>619</v>
       </c>
       <c r="C53" s="7"/>
-      <c r="D53" s="44"/>
+      <c r="D53" s="43"/>
     </row>
     <row r="54" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A54" s="41"/>
@@ -7450,7 +7499,7 @@
         <v>619</v>
       </c>
       <c r="C54" s="7"/>
-      <c r="D54" s="44"/>
+      <c r="D54" s="43"/>
     </row>
     <row r="55" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A55" s="41"/>
@@ -7458,7 +7507,7 @@
         <v>619</v>
       </c>
       <c r="C55" s="7"/>
-      <c r="D55" s="44"/>
+      <c r="D55" s="43"/>
     </row>
     <row r="56" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A56" s="41"/>
@@ -7466,7 +7515,7 @@
         <v>619</v>
       </c>
       <c r="C56" s="7"/>
-      <c r="D56" s="45"/>
+      <c r="D56" s="44"/>
     </row>
     <row r="57" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A57" s="41"/>
@@ -7506,7 +7555,7 @@
         <v>626</v>
       </c>
       <c r="C60" s="7"/>
-      <c r="D60" s="42" t="s">
+      <c r="D60" s="40" t="s">
         <v>627</v>
       </c>
     </row>
@@ -7535,7 +7584,7 @@
       <c r="D63" s="8"/>
     </row>
     <row r="64" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A64" s="49" t="s">
+      <c r="A64" s="47" t="s">
         <v>628</v>
       </c>
       <c r="B64" s="9" t="s">
@@ -7625,7 +7674,7 @@
       <c r="D74" s="2"/>
     </row>
     <row r="75" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A75" s="46" t="s">
+      <c r="A75" s="49" t="s">
         <v>632</v>
       </c>
       <c r="B75" s="6" t="s">
@@ -7634,7 +7683,7 @@
       <c r="C75" s="7" t="s">
         <v>634</v>
       </c>
-      <c r="D75" s="42" t="s">
+      <c r="D75" s="40" t="s">
         <v>635</v>
       </c>
     </row>
@@ -7901,7 +7950,7 @@
       <c r="D102" s="2"/>
     </row>
     <row r="103" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A103" s="40" t="s">
+      <c r="A103" s="45" t="s">
         <v>662</v>
       </c>
       <c r="B103" s="6" t="s">
@@ -10619,22 +10668,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="D29:D31"/>
-    <mergeCell ref="D34:D36"/>
-    <mergeCell ref="A21:A39"/>
-    <mergeCell ref="A40:A63"/>
-    <mergeCell ref="A64:A74"/>
-    <mergeCell ref="A1:A20"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="D9:D11"/>
-    <mergeCell ref="D13:D15"/>
-    <mergeCell ref="D25:D27"/>
     <mergeCell ref="A103:A105"/>
     <mergeCell ref="D43:D47"/>
     <mergeCell ref="D51:D56"/>
     <mergeCell ref="D60:D62"/>
     <mergeCell ref="D75:D77"/>
     <mergeCell ref="A75:A102"/>
+    <mergeCell ref="A1:A20"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="D13:D15"/>
+    <mergeCell ref="D25:D27"/>
+    <mergeCell ref="D29:D31"/>
+    <mergeCell ref="D34:D36"/>
+    <mergeCell ref="A21:A39"/>
+    <mergeCell ref="A40:A63"/>
+    <mergeCell ref="A64:A74"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated FJP @ 9 Feb, 2022 9:30 AM
</commit_message>
<xml_diff>
--- a/Level_1/First Job Program With Web Development.xlsx
+++ b/Level_1/First Job Program With Web Development.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\Nados\LearnDSA\Level_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F5BA858-171D-4176-AA93-E3696844A9CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B0045CD-7EFB-4BD7-BF44-7002BB7ACBD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1223" uniqueCount="1123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1228" uniqueCount="1123">
   <si>
     <t>Print Z</t>
   </si>
@@ -3697,7 +3697,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -3754,30 +3754,29 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="15" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="16" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="16" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="16" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -4007,7 +4006,7 @@
   <dimension ref="A1:D566"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4039,14 +4038,14 @@
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="37" t="s">
+      <c r="B3" s="36" t="s">
         <v>1121</v>
       </c>
-      <c r="C3" s="36">
+      <c r="C3" s="35">
         <f>DATE(2022,2,6)</f>
         <v>44598</v>
       </c>
-      <c r="D3" s="35" t="s">
+      <c r="D3" s="34" t="s">
         <v>1122</v>
       </c>
     </row>
@@ -4054,14 +4053,14 @@
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="36" t="s">
         <v>1121</v>
       </c>
-      <c r="C4" s="36">
-        <f t="shared" ref="C4:C6" si="0">DATE(2022,2,6)</f>
+      <c r="C4" s="35">
+        <f t="shared" ref="C4:C5" si="0">DATE(2022,2,6)</f>
         <v>44598</v>
       </c>
-      <c r="D4" s="35" t="s">
+      <c r="D4" s="34" t="s">
         <v>1122</v>
       </c>
     </row>
@@ -4069,14 +4068,14 @@
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="36" t="s">
         <v>1121</v>
       </c>
-      <c r="C5" s="36">
+      <c r="C5" s="35">
         <f t="shared" si="0"/>
         <v>44598</v>
       </c>
-      <c r="D5" s="35" t="s">
+      <c r="D5" s="34" t="s">
         <v>1122</v>
       </c>
     </row>
@@ -4084,14 +4083,14 @@
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="38" t="s">
+      <c r="B6" s="37" t="s">
         <v>1121</v>
       </c>
-      <c r="C6" s="36">
+      <c r="C6" s="35">
         <f>DATE(2022,2,6)+1</f>
         <v>44599</v>
       </c>
-      <c r="D6" s="35" t="s">
+      <c r="D6" s="34" t="s">
         <v>1122</v>
       </c>
     </row>
@@ -4099,14 +4098,14 @@
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="39" t="s">
+      <c r="B7" s="38" t="s">
         <v>1121</v>
       </c>
-      <c r="C7" s="36">
+      <c r="C7" s="35">
         <f>DATE(2022,2,6)+1</f>
         <v>44599</v>
       </c>
-      <c r="D7" s="35" t="s">
+      <c r="D7" s="34" t="s">
         <v>1122</v>
       </c>
     </row>
@@ -4114,14 +4113,14 @@
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="36" t="s">
         <v>1121</v>
       </c>
-      <c r="C8" s="36">
+      <c r="C8" s="35">
         <f t="shared" ref="C8:C11" si="1">DATE(2022,2,6)+1</f>
         <v>44599</v>
       </c>
-      <c r="D8" s="35" t="s">
+      <c r="D8" s="34" t="s">
         <v>1122</v>
       </c>
     </row>
@@ -4129,14 +4128,14 @@
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="38" t="s">
+      <c r="B9" s="37" t="s">
         <v>1121</v>
       </c>
-      <c r="C9" s="36">
+      <c r="C9" s="35">
         <f t="shared" si="1"/>
         <v>44599</v>
       </c>
-      <c r="D9" s="35" t="s">
+      <c r="D9" s="34" t="s">
         <v>1122</v>
       </c>
     </row>
@@ -4144,14 +4143,14 @@
       <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="37" t="s">
+      <c r="B10" s="36" t="s">
         <v>1121</v>
       </c>
-      <c r="C10" s="36">
+      <c r="C10" s="35">
         <f t="shared" si="1"/>
         <v>44599</v>
       </c>
-      <c r="D10" s="35" t="s">
+      <c r="D10" s="34" t="s">
         <v>1122</v>
       </c>
     </row>
@@ -4159,14 +4158,14 @@
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="37" t="s">
+      <c r="B11" s="36" t="s">
         <v>1121</v>
       </c>
-      <c r="C11" s="36">
+      <c r="C11" s="35">
         <f t="shared" si="1"/>
         <v>44599</v>
       </c>
-      <c r="D11" s="35" t="s">
+      <c r="D11" s="34" t="s">
         <v>1122</v>
       </c>
     </row>
@@ -4174,14 +4173,14 @@
       <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="38" t="s">
+      <c r="B12" s="37" t="s">
         <v>1121</v>
       </c>
-      <c r="C12" s="36">
+      <c r="C12" s="35">
         <f>DATE(2022,2,6)+1</f>
         <v>44599</v>
       </c>
-      <c r="D12" s="35" t="s">
+      <c r="D12" s="34" t="s">
         <v>1122</v>
       </c>
     </row>
@@ -4189,113 +4188,148 @@
       <c r="A13" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="34" t="s">
+      <c r="B13" s="37" t="s">
         <v>1121</v>
+      </c>
+      <c r="C13" s="35">
+        <f>DATE(2022,2,6)+2</f>
+        <v>44600</v>
+      </c>
+      <c r="D13" s="34" t="s">
+        <v>1122</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="34" t="s">
+      <c r="B14" s="36" t="s">
         <v>1121</v>
+      </c>
+      <c r="C14" s="35">
+        <f>DATE(2022,2,6)+2</f>
+        <v>44600</v>
+      </c>
+      <c r="D14" s="34" t="s">
+        <v>1122</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="34" t="s">
+      <c r="B15" s="37" t="s">
         <v>1121</v>
+      </c>
+      <c r="C15" s="35">
+        <f>DATE(2022,2,6)+3</f>
+        <v>44601</v>
+      </c>
+      <c r="D15" s="34" t="s">
+        <v>1122</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="34" t="s">
+      <c r="B16" s="36" t="s">
         <v>1121</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="C16" s="35">
+        <f t="shared" ref="C16:C17" si="2">DATE(2022,2,6)+3</f>
+        <v>44601</v>
+      </c>
+      <c r="D16" s="34" t="s">
+        <v>1122</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="34" t="s">
+      <c r="B17" s="36" t="s">
         <v>1121</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="C17" s="35">
+        <f t="shared" si="2"/>
+        <v>44601</v>
+      </c>
+      <c r="D17" s="34" t="s">
+        <v>1122</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A18" s="33" t="s">
         <v>1120</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>28</v>
       </c>
@@ -6960,7 +6994,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="46" t="s">
         <v>544</v>
       </c>
       <c r="B1" s="4" t="s">
@@ -6972,7 +7006,7 @@
       <c r="D1" s="2"/>
     </row>
     <row r="2" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A2" s="41"/>
+      <c r="A2" s="40"/>
       <c r="B2" s="6" t="s">
         <v>547</v>
       </c>
@@ -6982,7 +7016,7 @@
       <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A3" s="41"/>
+      <c r="A3" s="40"/>
       <c r="B3" s="6" t="s">
         <v>547</v>
       </c>
@@ -6992,7 +7026,7 @@
       <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A4" s="41"/>
+      <c r="A4" s="40"/>
       <c r="B4" s="6" t="s">
         <v>547</v>
       </c>
@@ -7002,29 +7036,29 @@
       <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A5" s="41"/>
+      <c r="A5" s="40"/>
       <c r="B5" s="6" t="s">
         <v>551</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>552</v>
       </c>
-      <c r="D5" s="40" t="s">
+      <c r="D5" s="41" t="s">
         <v>553</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A6" s="41"/>
+      <c r="A6" s="40"/>
       <c r="B6" s="6" t="s">
         <v>551</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>554</v>
       </c>
-      <c r="D6" s="41"/>
+      <c r="D6" s="40"/>
     </row>
     <row r="7" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A7" s="41"/>
+      <c r="A7" s="40"/>
       <c r="B7" s="9" t="s">
         <v>555</v>
       </c>
@@ -7034,7 +7068,7 @@
       <c r="D7" s="10"/>
     </row>
     <row r="8" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A8" s="41"/>
+      <c r="A8" s="40"/>
       <c r="B8" s="2" t="s">
         <v>557</v>
       </c>
@@ -7044,39 +7078,39 @@
       <c r="D8" s="10"/>
     </row>
     <row r="9" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A9" s="41"/>
+      <c r="A9" s="40"/>
       <c r="B9" s="6" t="s">
         <v>559</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>560</v>
       </c>
-      <c r="D9" s="40" t="s">
+      <c r="D9" s="41" t="s">
         <v>561</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A10" s="41"/>
+      <c r="A10" s="40"/>
       <c r="B10" s="6" t="s">
         <v>559</v>
       </c>
       <c r="C10" s="12" t="s">
         <v>562</v>
       </c>
-      <c r="D10" s="41"/>
+      <c r="D10" s="40"/>
     </row>
     <row r="11" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A11" s="41"/>
+      <c r="A11" s="40"/>
       <c r="B11" s="6" t="s">
         <v>559</v>
       </c>
       <c r="C11" s="12" t="s">
         <v>563</v>
       </c>
-      <c r="D11" s="41"/>
+      <c r="D11" s="40"/>
     </row>
     <row r="12" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A12" s="41"/>
+      <c r="A12" s="40"/>
       <c r="B12" s="9" t="s">
         <v>564</v>
       </c>
@@ -7086,39 +7120,39 @@
       <c r="D12" s="10"/>
     </row>
     <row r="13" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A13" s="41"/>
+      <c r="A13" s="40"/>
       <c r="B13" s="6" t="s">
         <v>566</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>567</v>
       </c>
-      <c r="D13" s="40" t="s">
+      <c r="D13" s="41" t="s">
         <v>568</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A14" s="41"/>
+      <c r="A14" s="40"/>
       <c r="B14" s="6" t="s">
         <v>566</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>569</v>
       </c>
-      <c r="D14" s="41"/>
+      <c r="D14" s="40"/>
     </row>
     <row r="15" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A15" s="41"/>
+      <c r="A15" s="40"/>
       <c r="B15" s="6" t="s">
         <v>566</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>569</v>
       </c>
-      <c r="D15" s="41"/>
+      <c r="D15" s="40"/>
     </row>
     <row r="16" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A16" s="41"/>
+      <c r="A16" s="40"/>
       <c r="B16" s="9" t="s">
         <v>570</v>
       </c>
@@ -7128,7 +7162,7 @@
       <c r="D16" s="2"/>
     </row>
     <row r="17" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A17" s="41"/>
+      <c r="A17" s="40"/>
       <c r="B17" s="6" t="s">
         <v>566</v>
       </c>
@@ -7138,7 +7172,7 @@
       <c r="D17" s="10"/>
     </row>
     <row r="18" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A18" s="41"/>
+      <c r="A18" s="40"/>
       <c r="B18" s="6" t="s">
         <v>566</v>
       </c>
@@ -7148,7 +7182,7 @@
       <c r="D18" s="10"/>
     </row>
     <row r="19" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A19" s="41"/>
+      <c r="A19" s="40"/>
       <c r="B19" s="9" t="s">
         <v>574</v>
       </c>
@@ -7158,7 +7192,7 @@
       <c r="D19" s="10"/>
     </row>
     <row r="20" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A20" s="41"/>
+      <c r="A20" s="40"/>
       <c r="B20" s="2" t="s">
         <v>557</v>
       </c>
@@ -7168,7 +7202,7 @@
       <c r="D20" s="10"/>
     </row>
     <row r="21" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A21" s="45" t="s">
+      <c r="A21" s="39" t="s">
         <v>577</v>
       </c>
       <c r="B21" s="6" t="s">
@@ -7180,7 +7214,7 @@
       <c r="D21" s="2"/>
     </row>
     <row r="22" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A22" s="41"/>
+      <c r="A22" s="40"/>
       <c r="B22" s="6" t="s">
         <v>578</v>
       </c>
@@ -7190,7 +7224,7 @@
       <c r="D22" s="2"/>
     </row>
     <row r="23" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A23" s="41"/>
+      <c r="A23" s="40"/>
       <c r="B23" s="6" t="s">
         <v>578</v>
       </c>
@@ -7200,7 +7234,7 @@
       <c r="D23" s="2"/>
     </row>
     <row r="24" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A24" s="41"/>
+      <c r="A24" s="40"/>
       <c r="B24" s="10" t="s">
         <v>582</v>
       </c>
@@ -7210,7 +7244,7 @@
       <c r="D24" s="2"/>
     </row>
     <row r="25" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A25" s="41"/>
+      <c r="A25" s="40"/>
       <c r="B25" s="13" t="s">
         <v>584</v>
       </c>
@@ -7220,7 +7254,7 @@
       </c>
     </row>
     <row r="26" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A26" s="41"/>
+      <c r="A26" s="40"/>
       <c r="B26" s="6" t="s">
         <v>584</v>
       </c>
@@ -7230,7 +7264,7 @@
       <c r="D26" s="43"/>
     </row>
     <row r="27" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A27" s="41"/>
+      <c r="A27" s="40"/>
       <c r="B27" s="6" t="s">
         <v>584</v>
       </c>
@@ -7240,7 +7274,7 @@
       <c r="D27" s="44"/>
     </row>
     <row r="28" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A28" s="41"/>
+      <c r="A28" s="40"/>
       <c r="B28" s="2" t="s">
         <v>582</v>
       </c>
@@ -7250,39 +7284,39 @@
       <c r="D28" s="2"/>
     </row>
     <row r="29" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A29" s="41"/>
+      <c r="A29" s="40"/>
       <c r="B29" s="6" t="s">
         <v>589</v>
       </c>
       <c r="C29" s="7" t="s">
         <v>590</v>
       </c>
-      <c r="D29" s="40" t="s">
+      <c r="D29" s="41" t="s">
         <v>591</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A30" s="41"/>
+      <c r="A30" s="40"/>
       <c r="B30" s="6" t="s">
         <v>589</v>
       </c>
       <c r="C30" s="7" t="s">
         <v>592</v>
       </c>
-      <c r="D30" s="41"/>
+      <c r="D30" s="40"/>
     </row>
     <row r="31" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A31" s="41"/>
+      <c r="A31" s="40"/>
       <c r="B31" s="6" t="s">
         <v>589</v>
       </c>
       <c r="C31" s="7" t="s">
         <v>593</v>
       </c>
-      <c r="D31" s="41"/>
+      <c r="D31" s="40"/>
     </row>
     <row r="32" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A32" s="41"/>
+      <c r="A32" s="40"/>
       <c r="B32" s="6" t="s">
         <v>594</v>
       </c>
@@ -7292,7 +7326,7 @@
       <c r="D32" s="2"/>
     </row>
     <row r="33" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A33" s="41"/>
+      <c r="A33" s="40"/>
       <c r="B33" s="2" t="s">
         <v>596</v>
       </c>
@@ -7302,7 +7336,7 @@
       <c r="D33" s="2"/>
     </row>
     <row r="34" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A34" s="41"/>
+      <c r="A34" s="40"/>
       <c r="B34" s="6" t="s">
         <v>598</v>
       </c>
@@ -7314,7 +7348,7 @@
       </c>
     </row>
     <row r="35" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A35" s="41"/>
+      <c r="A35" s="40"/>
       <c r="B35" s="6" t="s">
         <v>598</v>
       </c>
@@ -7324,7 +7358,7 @@
       <c r="D35" s="43"/>
     </row>
     <row r="36" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A36" s="41"/>
+      <c r="A36" s="40"/>
       <c r="B36" s="6" t="s">
         <v>598</v>
       </c>
@@ -7334,7 +7368,7 @@
       <c r="D36" s="44"/>
     </row>
     <row r="37" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A37" s="41"/>
+      <c r="A37" s="40"/>
       <c r="B37" s="6" t="s">
         <v>598</v>
       </c>
@@ -7344,7 +7378,7 @@
       <c r="D37" s="2"/>
     </row>
     <row r="38" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A38" s="41"/>
+      <c r="A38" s="40"/>
       <c r="B38" s="2" t="s">
         <v>582</v>
       </c>
@@ -7354,7 +7388,7 @@
       <c r="D38" s="2"/>
     </row>
     <row r="39" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A39" s="41"/>
+      <c r="A39" s="40"/>
       <c r="B39" s="9" t="s">
         <v>605</v>
       </c>
@@ -7364,7 +7398,7 @@
       <c r="D39" s="2"/>
     </row>
     <row r="40" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A40" s="46" t="s">
+      <c r="A40" s="47" t="s">
         <v>607</v>
       </c>
       <c r="B40" s="6" t="s">
@@ -7376,7 +7410,7 @@
       <c r="D40" s="2"/>
     </row>
     <row r="41" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A41" s="41"/>
+      <c r="A41" s="40"/>
       <c r="B41" s="6" t="s">
         <v>608</v>
       </c>
@@ -7386,7 +7420,7 @@
       <c r="D41" s="2"/>
     </row>
     <row r="42" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A42" s="41"/>
+      <c r="A42" s="40"/>
       <c r="B42" s="6" t="s">
         <v>608</v>
       </c>
@@ -7396,51 +7430,51 @@
       <c r="D42" s="2"/>
     </row>
     <row r="43" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A43" s="41"/>
+      <c r="A43" s="40"/>
       <c r="B43" s="6" t="s">
         <v>612</v>
       </c>
       <c r="C43" s="7"/>
-      <c r="D43" s="40" t="s">
+      <c r="D43" s="41" t="s">
         <v>613</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A44" s="41"/>
+      <c r="A44" s="40"/>
       <c r="B44" s="6" t="s">
         <v>612</v>
       </c>
       <c r="C44" s="7"/>
-      <c r="D44" s="41"/>
+      <c r="D44" s="40"/>
     </row>
     <row r="45" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A45" s="41"/>
+      <c r="A45" s="40"/>
       <c r="B45" s="6" t="s">
         <v>612</v>
       </c>
       <c r="C45" s="7"/>
-      <c r="D45" s="41"/>
+      <c r="D45" s="40"/>
     </row>
     <row r="46" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A46" s="41"/>
+      <c r="A46" s="40"/>
       <c r="B46" s="6" t="s">
         <v>612</v>
       </c>
       <c r="C46" s="7"/>
-      <c r="D46" s="41"/>
+      <c r="D46" s="40"/>
     </row>
     <row r="47" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A47" s="41"/>
+      <c r="A47" s="40"/>
       <c r="B47" s="6" t="s">
         <v>614</v>
       </c>
       <c r="C47" s="7" t="s">
         <v>615</v>
       </c>
-      <c r="D47" s="41"/>
+      <c r="D47" s="40"/>
     </row>
     <row r="48" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A48" s="41"/>
+      <c r="A48" s="40"/>
       <c r="B48" s="6" t="s">
         <v>614</v>
       </c>
@@ -7450,7 +7484,7 @@
       <c r="D48" s="2"/>
     </row>
     <row r="49" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A49" s="41"/>
+      <c r="A49" s="40"/>
       <c r="B49" s="6" t="s">
         <v>614</v>
       </c>
@@ -7460,7 +7494,7 @@
       <c r="D49" s="2"/>
     </row>
     <row r="50" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A50" s="41"/>
+      <c r="A50" s="40"/>
       <c r="B50" s="2" t="s">
         <v>618</v>
       </c>
@@ -7468,7 +7502,7 @@
       <c r="D50" s="2"/>
     </row>
     <row r="51" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A51" s="41"/>
+      <c r="A51" s="40"/>
       <c r="B51" s="6" t="s">
         <v>619</v>
       </c>
@@ -7478,7 +7512,7 @@
       </c>
     </row>
     <row r="52" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A52" s="41"/>
+      <c r="A52" s="40"/>
       <c r="B52" s="6" t="s">
         <v>619</v>
       </c>
@@ -7486,7 +7520,7 @@
       <c r="D52" s="43"/>
     </row>
     <row r="53" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A53" s="41"/>
+      <c r="A53" s="40"/>
       <c r="B53" s="6" t="s">
         <v>619</v>
       </c>
@@ -7494,7 +7528,7 @@
       <c r="D53" s="43"/>
     </row>
     <row r="54" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A54" s="41"/>
+      <c r="A54" s="40"/>
       <c r="B54" s="6" t="s">
         <v>619</v>
       </c>
@@ -7502,7 +7536,7 @@
       <c r="D54" s="43"/>
     </row>
     <row r="55" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A55" s="41"/>
+      <c r="A55" s="40"/>
       <c r="B55" s="6" t="s">
         <v>619</v>
       </c>
@@ -7510,7 +7544,7 @@
       <c r="D55" s="43"/>
     </row>
     <row r="56" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A56" s="41"/>
+      <c r="A56" s="40"/>
       <c r="B56" s="6" t="s">
         <v>619</v>
       </c>
@@ -7518,7 +7552,7 @@
       <c r="D56" s="44"/>
     </row>
     <row r="57" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A57" s="41"/>
+      <c r="A57" s="40"/>
       <c r="B57" s="6" t="s">
         <v>621</v>
       </c>
@@ -7528,7 +7562,7 @@
       <c r="D57" s="2"/>
     </row>
     <row r="58" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A58" s="41"/>
+      <c r="A58" s="40"/>
       <c r="B58" s="6" t="s">
         <v>621</v>
       </c>
@@ -7538,7 +7572,7 @@
       <c r="D58" s="2"/>
     </row>
     <row r="59" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A59" s="41"/>
+      <c r="A59" s="40"/>
       <c r="B59" s="6" t="s">
         <v>621</v>
       </c>
@@ -7550,33 +7584,33 @@
       </c>
     </row>
     <row r="60" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A60" s="41"/>
+      <c r="A60" s="40"/>
       <c r="B60" s="6" t="s">
         <v>626</v>
       </c>
       <c r="C60" s="7"/>
-      <c r="D60" s="40" t="s">
+      <c r="D60" s="41" t="s">
         <v>627</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A61" s="41"/>
+      <c r="A61" s="40"/>
       <c r="B61" s="6" t="s">
         <v>626</v>
       </c>
       <c r="C61" s="7"/>
-      <c r="D61" s="41"/>
+      <c r="D61" s="40"/>
     </row>
     <row r="62" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A62" s="41"/>
+      <c r="A62" s="40"/>
       <c r="B62" s="6" t="s">
         <v>626</v>
       </c>
       <c r="C62" s="7"/>
-      <c r="D62" s="41"/>
+      <c r="D62" s="40"/>
     </row>
     <row r="63" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A63" s="41"/>
+      <c r="A63" s="40"/>
       <c r="B63" s="6" t="s">
         <v>626</v>
       </c>
@@ -7584,7 +7618,7 @@
       <c r="D63" s="8"/>
     </row>
     <row r="64" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A64" s="47" t="s">
+      <c r="A64" s="48" t="s">
         <v>628</v>
       </c>
       <c r="B64" s="9" t="s">
@@ -7594,7 +7628,7 @@
       <c r="D64" s="8"/>
     </row>
     <row r="65" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A65" s="41"/>
+      <c r="A65" s="40"/>
       <c r="B65" s="9" t="s">
         <v>629</v>
       </c>
@@ -7602,7 +7636,7 @@
       <c r="D65" s="2"/>
     </row>
     <row r="66" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A66" s="41"/>
+      <c r="A66" s="40"/>
       <c r="B66" s="9" t="s">
         <v>629</v>
       </c>
@@ -7610,7 +7644,7 @@
       <c r="D66" s="2"/>
     </row>
     <row r="67" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A67" s="41"/>
+      <c r="A67" s="40"/>
       <c r="B67" s="9" t="s">
         <v>629</v>
       </c>
@@ -7618,7 +7652,7 @@
       <c r="D67" s="2"/>
     </row>
     <row r="68" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A68" s="41"/>
+      <c r="A68" s="40"/>
       <c r="B68" s="9" t="s">
         <v>630</v>
       </c>
@@ -7626,7 +7660,7 @@
       <c r="D68" s="2"/>
     </row>
     <row r="69" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A69" s="41"/>
+      <c r="A69" s="40"/>
       <c r="B69" s="9" t="s">
         <v>630</v>
       </c>
@@ -7634,7 +7668,7 @@
       <c r="D69" s="2"/>
     </row>
     <row r="70" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A70" s="41"/>
+      <c r="A70" s="40"/>
       <c r="B70" s="9" t="s">
         <v>630</v>
       </c>
@@ -7642,7 +7676,7 @@
       <c r="D70" s="2"/>
     </row>
     <row r="71" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A71" s="41"/>
+      <c r="A71" s="40"/>
       <c r="B71" s="9" t="s">
         <v>630</v>
       </c>
@@ -7650,7 +7684,7 @@
       <c r="D71" s="2"/>
     </row>
     <row r="72" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A72" s="41"/>
+      <c r="A72" s="40"/>
       <c r="B72" s="9" t="s">
         <v>631</v>
       </c>
@@ -7658,7 +7692,7 @@
       <c r="D72" s="2"/>
     </row>
     <row r="73" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A73" s="41"/>
+      <c r="A73" s="40"/>
       <c r="B73" s="9" t="s">
         <v>631</v>
       </c>
@@ -7666,7 +7700,7 @@
       <c r="D73" s="2"/>
     </row>
     <row r="74" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A74" s="41"/>
+      <c r="A74" s="40"/>
       <c r="B74" s="9" t="s">
         <v>631</v>
       </c>
@@ -7674,7 +7708,7 @@
       <c r="D74" s="2"/>
     </row>
     <row r="75" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A75" s="49" t="s">
+      <c r="A75" s="45" t="s">
         <v>632</v>
       </c>
       <c r="B75" s="6" t="s">
@@ -7683,32 +7717,32 @@
       <c r="C75" s="7" t="s">
         <v>634</v>
       </c>
-      <c r="D75" s="40" t="s">
+      <c r="D75" s="41" t="s">
         <v>635</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A76" s="41"/>
+      <c r="A76" s="40"/>
       <c r="B76" s="6" t="s">
         <v>633</v>
       </c>
       <c r="C76" s="7" t="s">
         <v>636</v>
       </c>
-      <c r="D76" s="41"/>
+      <c r="D76" s="40"/>
     </row>
     <row r="77" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A77" s="41"/>
+      <c r="A77" s="40"/>
       <c r="B77" s="6" t="s">
         <v>633</v>
       </c>
       <c r="C77" s="7" t="s">
         <v>637</v>
       </c>
-      <c r="D77" s="41"/>
+      <c r="D77" s="40"/>
     </row>
     <row r="78" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A78" s="41"/>
+      <c r="A78" s="40"/>
       <c r="B78" s="6" t="s">
         <v>633</v>
       </c>
@@ -7718,7 +7752,7 @@
       <c r="D78" s="2"/>
     </row>
     <row r="79" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A79" s="41"/>
+      <c r="A79" s="40"/>
       <c r="B79" s="6" t="s">
         <v>633</v>
       </c>
@@ -7728,7 +7762,7 @@
       <c r="D79" s="2"/>
     </row>
     <row r="80" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A80" s="41"/>
+      <c r="A80" s="40"/>
       <c r="B80" s="6" t="s">
         <v>633</v>
       </c>
@@ -7738,7 +7772,7 @@
       <c r="D80" s="2"/>
     </row>
     <row r="81" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A81" s="41"/>
+      <c r="A81" s="40"/>
       <c r="B81" s="6" t="s">
         <v>633</v>
       </c>
@@ -7748,7 +7782,7 @@
       <c r="D81" s="2"/>
     </row>
     <row r="82" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A82" s="41"/>
+      <c r="A82" s="40"/>
       <c r="B82" s="6" t="s">
         <v>633</v>
       </c>
@@ -7758,7 +7792,7 @@
       <c r="D82" s="2"/>
     </row>
     <row r="83" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A83" s="41"/>
+      <c r="A83" s="40"/>
       <c r="B83" s="6" t="s">
         <v>633</v>
       </c>
@@ -7768,7 +7802,7 @@
       <c r="D83" s="2"/>
     </row>
     <row r="84" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A84" s="41"/>
+      <c r="A84" s="40"/>
       <c r="B84" s="6" t="s">
         <v>633</v>
       </c>
@@ -7778,7 +7812,7 @@
       <c r="D84" s="2"/>
     </row>
     <row r="85" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A85" s="41"/>
+      <c r="A85" s="40"/>
       <c r="B85" s="6" t="s">
         <v>633</v>
       </c>
@@ -7788,7 +7822,7 @@
       <c r="D85" s="2"/>
     </row>
     <row r="86" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A86" s="41"/>
+      <c r="A86" s="40"/>
       <c r="B86" s="6" t="s">
         <v>633</v>
       </c>
@@ -7798,7 +7832,7 @@
       <c r="D86" s="2"/>
     </row>
     <row r="87" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A87" s="41"/>
+      <c r="A87" s="40"/>
       <c r="B87" s="6" t="s">
         <v>647</v>
       </c>
@@ -7808,7 +7842,7 @@
       <c r="D87" s="2"/>
     </row>
     <row r="88" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A88" s="41"/>
+      <c r="A88" s="40"/>
       <c r="B88" s="6" t="s">
         <v>647</v>
       </c>
@@ -7818,7 +7852,7 @@
       <c r="D88" s="2"/>
     </row>
     <row r="89" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A89" s="41"/>
+      <c r="A89" s="40"/>
       <c r="B89" s="6" t="s">
         <v>647</v>
       </c>
@@ -7828,7 +7862,7 @@
       <c r="D89" s="2"/>
     </row>
     <row r="90" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A90" s="41"/>
+      <c r="A90" s="40"/>
       <c r="B90" s="6" t="s">
         <v>647</v>
       </c>
@@ -7838,7 +7872,7 @@
       <c r="D90" s="2"/>
     </row>
     <row r="91" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A91" s="41"/>
+      <c r="A91" s="40"/>
       <c r="B91" s="6" t="s">
         <v>647</v>
       </c>
@@ -7848,7 +7882,7 @@
       <c r="D91" s="10"/>
     </row>
     <row r="92" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A92" s="41"/>
+      <c r="A92" s="40"/>
       <c r="B92" s="14" t="s">
         <v>647</v>
       </c>
@@ -7858,7 +7892,7 @@
       <c r="D92" s="10"/>
     </row>
     <row r="93" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A93" s="41"/>
+      <c r="A93" s="40"/>
       <c r="B93" s="6" t="s">
         <v>647</v>
       </c>
@@ -7868,7 +7902,7 @@
       <c r="D93" s="2"/>
     </row>
     <row r="94" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A94" s="41"/>
+      <c r="A94" s="40"/>
       <c r="B94" s="6" t="s">
         <v>647</v>
       </c>
@@ -7878,7 +7912,7 @@
       <c r="D94" s="2"/>
     </row>
     <row r="95" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A95" s="41"/>
+      <c r="A95" s="40"/>
       <c r="B95" s="6" t="s">
         <v>647</v>
       </c>
@@ -7888,7 +7922,7 @@
       <c r="D95" s="2"/>
     </row>
     <row r="96" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A96" s="41"/>
+      <c r="A96" s="40"/>
       <c r="B96" s="6" t="s">
         <v>657</v>
       </c>
@@ -7898,7 +7932,7 @@
       <c r="D96" s="2"/>
     </row>
     <row r="97" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A97" s="41"/>
+      <c r="A97" s="40"/>
       <c r="B97" s="6" t="s">
         <v>657</v>
       </c>
@@ -7908,7 +7942,7 @@
       <c r="D97" s="2"/>
     </row>
     <row r="98" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A98" s="41"/>
+      <c r="A98" s="40"/>
       <c r="B98" s="14" t="s">
         <v>657</v>
       </c>
@@ -7918,7 +7952,7 @@
       <c r="D98" s="2"/>
     </row>
     <row r="99" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A99" s="41"/>
+      <c r="A99" s="40"/>
       <c r="B99" s="16" t="s">
         <v>661</v>
       </c>
@@ -7926,7 +7960,7 @@
       <c r="D99" s="2"/>
     </row>
     <row r="100" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A100" s="41"/>
+      <c r="A100" s="40"/>
       <c r="B100" s="9" t="s">
         <v>661</v>
       </c>
@@ -7934,7 +7968,7 @@
       <c r="D100" s="2"/>
     </row>
     <row r="101" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A101" s="41"/>
+      <c r="A101" s="40"/>
       <c r="B101" s="9" t="s">
         <v>661</v>
       </c>
@@ -7942,7 +7976,7 @@
       <c r="D101" s="2"/>
     </row>
     <row r="102" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A102" s="41"/>
+      <c r="A102" s="40"/>
       <c r="B102" s="9" t="s">
         <v>661</v>
       </c>
@@ -7950,7 +7984,7 @@
       <c r="D102" s="2"/>
     </row>
     <row r="103" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A103" s="45" t="s">
+      <c r="A103" s="39" t="s">
         <v>662</v>
       </c>
       <c r="B103" s="6" t="s">
@@ -7962,7 +7996,7 @@
       <c r="D103" s="2"/>
     </row>
     <row r="104" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A104" s="41"/>
+      <c r="A104" s="40"/>
       <c r="B104" s="6" t="s">
         <v>663</v>
       </c>
@@ -7972,7 +8006,7 @@
       <c r="D104" s="2"/>
     </row>
     <row r="105" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A105" s="41"/>
+      <c r="A105" s="40"/>
       <c r="B105" s="6" t="s">
         <v>663</v>
       </c>
@@ -10668,22 +10702,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="D29:D31"/>
+    <mergeCell ref="D34:D36"/>
+    <mergeCell ref="A21:A39"/>
+    <mergeCell ref="A40:A63"/>
+    <mergeCell ref="A64:A74"/>
+    <mergeCell ref="A1:A20"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="D13:D15"/>
+    <mergeCell ref="D25:D27"/>
     <mergeCell ref="A103:A105"/>
     <mergeCell ref="D43:D47"/>
     <mergeCell ref="D51:D56"/>
     <mergeCell ref="D60:D62"/>
     <mergeCell ref="D75:D77"/>
     <mergeCell ref="A75:A102"/>
-    <mergeCell ref="A1:A20"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="D9:D11"/>
-    <mergeCell ref="D13:D15"/>
-    <mergeCell ref="D25:D27"/>
-    <mergeCell ref="D29:D31"/>
-    <mergeCell ref="D34:D36"/>
-    <mergeCell ref="A21:A39"/>
-    <mergeCell ref="A40:A63"/>
-    <mergeCell ref="A64:A74"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -13608,7 +13642,7 @@
       <c r="A2" s="2" t="s">
         <v>1086</v>
       </c>
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="49" t="s">
         <v>1087</v>
       </c>
     </row>
@@ -13616,31 +13650,31 @@
       <c r="A3" s="2" t="s">
         <v>1088</v>
       </c>
-      <c r="B3" s="41"/>
+      <c r="B3" s="40"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>1089</v>
       </c>
-      <c r="B4" s="41"/>
+      <c r="B4" s="40"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>1090</v>
       </c>
-      <c r="B5" s="41"/>
+      <c r="B5" s="40"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>1091</v>
       </c>
-      <c r="B6" s="41"/>
+      <c r="B6" s="40"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>1092</v>
       </c>
-      <c r="B7" s="50" t="s">
+      <c r="B7" s="49" t="s">
         <v>1093</v>
       </c>
     </row>
@@ -13648,19 +13682,19 @@
       <c r="A8" s="2" t="s">
         <v>1094</v>
       </c>
-      <c r="B8" s="41"/>
+      <c r="B8" s="40"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>1095</v>
       </c>
-      <c r="B9" s="41"/>
+      <c r="B9" s="40"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>1096</v>
       </c>
-      <c r="B10" s="50" t="s">
+      <c r="B10" s="49" t="s">
         <v>1097</v>
       </c>
     </row>
@@ -13668,25 +13702,25 @@
       <c r="A11" s="2" t="s">
         <v>1098</v>
       </c>
-      <c r="B11" s="41"/>
+      <c r="B11" s="40"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>1099</v>
       </c>
-      <c r="B12" s="41"/>
+      <c r="B12" s="40"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>1100</v>
       </c>
-      <c r="B13" s="41"/>
+      <c r="B13" s="40"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>1101</v>
       </c>
-      <c r="B14" s="50" t="s">
+      <c r="B14" s="49" t="s">
         <v>1102</v>
       </c>
     </row>
@@ -13694,61 +13728,61 @@
       <c r="A15" s="2" t="s">
         <v>1103</v>
       </c>
-      <c r="B15" s="41"/>
+      <c r="B15" s="40"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>1104</v>
       </c>
-      <c r="B16" s="41"/>
+      <c r="B16" s="40"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>1105</v>
       </c>
-      <c r="B17" s="41"/>
+      <c r="B17" s="40"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>1106</v>
       </c>
-      <c r="B18" s="41"/>
+      <c r="B18" s="40"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>1107</v>
       </c>
-      <c r="B19" s="41"/>
+      <c r="B19" s="40"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>1108</v>
       </c>
-      <c r="B20" s="41"/>
+      <c r="B20" s="40"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>1109</v>
       </c>
-      <c r="B21" s="41"/>
+      <c r="B21" s="40"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>1110</v>
       </c>
-      <c r="B22" s="41"/>
+      <c r="B22" s="40"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>1111</v>
       </c>
-      <c r="B23" s="41"/>
+      <c r="B23" s="40"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>1112</v>
       </c>
-      <c r="B24" s="51" t="s">
+      <c r="B24" s="50" t="s">
         <v>1113</v>
       </c>
     </row>
@@ -13756,7 +13790,7 @@
       <c r="A25" s="2" t="s">
         <v>1114</v>
       </c>
-      <c r="B25" s="41"/>
+      <c r="B25" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
Completed Recusion with arryas of level_1
</commit_message>
<xml_diff>
--- a/Level_1/First Job Program With Web Development.xlsx
+++ b/Level_1/First Job Program With Web Development.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\Nados\LearnDSA\Level_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4544612-9BD3-426F-9222-9F40AB882872}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF07D213-7FDD-45D6-8139-6F6DF52EA042}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
     <sheet name="Puzzles" sheetId="5" r:id="rId5"/>
     <sheet name="Guesstimates" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191029" calcMode="autoNoTable"/>
+  <calcPr calcId="191029" calcMode="manual"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1250" uniqueCount="1126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1262" uniqueCount="1126">
   <si>
     <t>Print Z</t>
   </si>
@@ -3732,7 +3732,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -3825,6 +3825,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4045,8 +4046,8 @@
   </sheetPr>
   <dimension ref="A1:D569"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="F88" sqref="F88"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="A101" sqref="A101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4661,7 +4662,7 @@
         <v>1121</v>
       </c>
       <c r="C84" s="35">
-        <f ca="1">TODAY()</f>
+        <f ca="1">TODAY()-1</f>
         <v>44613</v>
       </c>
       <c r="D84" s="34" t="s">
@@ -4676,7 +4677,7 @@
         <v>1121</v>
       </c>
       <c r="C85" s="35">
-        <f t="shared" ref="C85:C89" ca="1" si="4">TODAY()</f>
+        <f t="shared" ref="C85:C89" ca="1" si="4">TODAY()-1</f>
         <v>44613</v>
       </c>
       <c r="D85" s="34" t="s">
@@ -4729,10 +4730,10 @@
       </c>
     </row>
     <row r="89" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A89" s="2" t="s">
+      <c r="A89" s="56" t="s">
         <v>78</v>
       </c>
-      <c r="B89" s="36" t="s">
+      <c r="B89" s="37" t="s">
         <v>1121</v>
       </c>
       <c r="C89" s="35">
@@ -4745,35 +4746,96 @@
     </row>
     <row r="90" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A90" s="2"/>
+      <c r="C90" s="35"/>
     </row>
     <row r="91" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>79</v>
       </c>
+      <c r="B91" s="36" t="s">
+        <v>1121</v>
+      </c>
+      <c r="C91" s="35">
+        <f ca="1">TODAY()</f>
+        <v>44614</v>
+      </c>
+      <c r="D91" s="34" t="s">
+        <v>1122</v>
+      </c>
     </row>
     <row r="92" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>80</v>
       </c>
+      <c r="B92" s="36" t="s">
+        <v>1121</v>
+      </c>
+      <c r="C92" s="35">
+        <f t="shared" ref="C92:C96" ca="1" si="5">TODAY()</f>
+        <v>44614</v>
+      </c>
+      <c r="D92" s="34" t="s">
+        <v>1122</v>
+      </c>
     </row>
     <row r="93" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A93" s="2" t="s">
+      <c r="A93" s="56" t="s">
         <v>81</v>
+      </c>
+      <c r="B93" s="37" t="s">
+        <v>1121</v>
+      </c>
+      <c r="C93" s="35">
+        <f t="shared" ca="1" si="5"/>
+        <v>44614</v>
+      </c>
+      <c r="D93" s="34" t="s">
+        <v>1122</v>
       </c>
     </row>
     <row r="94" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>82</v>
       </c>
+      <c r="B94" s="36" t="s">
+        <v>1121</v>
+      </c>
+      <c r="C94" s="35">
+        <f t="shared" ca="1" si="5"/>
+        <v>44614</v>
+      </c>
+      <c r="D94" s="34" t="s">
+        <v>1122</v>
+      </c>
     </row>
     <row r="95" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>83</v>
       </c>
+      <c r="B95" s="36" t="s">
+        <v>1121</v>
+      </c>
+      <c r="C95" s="35">
+        <f t="shared" ca="1" si="5"/>
+        <v>44614</v>
+      </c>
+      <c r="D95" s="34" t="s">
+        <v>1122</v>
+      </c>
     </row>
     <row r="96" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A96" s="2" t="s">
+      <c r="A96" s="43" t="s">
         <v>84</v>
+      </c>
+      <c r="B96" s="37" t="s">
+        <v>1121</v>
+      </c>
+      <c r="C96" s="35">
+        <f t="shared" ca="1" si="5"/>
+        <v>44614</v>
+      </c>
+      <c r="D96" s="34" t="s">
+        <v>1122</v>
       </c>
     </row>
     <row r="97" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Started Stacks and Queues
</commit_message>
<xml_diff>
--- a/Level_1/First Job Program With Web Development.xlsx
+++ b/Level_1/First Job Program With Web Development.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\Nados\LearnDSA\Level_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF07D213-7FDD-45D6-8139-6F6DF52EA042}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ABB5B29-CF69-46C7-90F9-20573F4B496B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1262" uniqueCount="1126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1272" uniqueCount="1131">
   <si>
     <t>Print Z</t>
   </si>
@@ -3413,12 +3413,6 @@
     <t>Status</t>
   </si>
   <si>
-    <t>Getting Started</t>
-  </si>
-  <si>
-    <t>Patterns</t>
-  </si>
-  <si>
     <t>Easy</t>
   </si>
   <si>
@@ -3432,6 +3426,27 @@
   </si>
   <si>
     <t>2.1 Introduction to Recursion</t>
+  </si>
+  <si>
+    <t>2.2 Recursion in Arrays</t>
+  </si>
+  <si>
+    <t>2.3 Recursion with ArrayList</t>
+  </si>
+  <si>
+    <t>2.4 Recursion on the way up</t>
+  </si>
+  <si>
+    <t>2.5 Recursion Backtracking</t>
+  </si>
+  <si>
+    <t>3. Time and Space Complexity</t>
+  </si>
+  <si>
+    <t>1.1 Getting Started</t>
+  </si>
+  <si>
+    <t>1.2 Patterns</t>
   </si>
 </sst>
 </file>
@@ -3732,7 +3747,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -3788,7 +3803,6 @@
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="16" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -3799,6 +3813,9 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -3825,7 +3842,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4044,10 +4060,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D569"/>
+  <dimension ref="A1:D570"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="A101" sqref="A101"/>
+    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="D133" sqref="D133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4070,9 +4086,9 @@
         <v>1118</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="39" customFormat="1" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" s="38" customFormat="1" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="31" t="s">
-        <v>1123</v>
+        <v>1121</v>
       </c>
       <c r="B2" s="31"/>
       <c r="C2" s="31"/>
@@ -4080,237 +4096,237 @@
     </row>
     <row r="3" spans="1:4" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="32" t="s">
-        <v>1119</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="36" t="s">
-        <v>1121</v>
-      </c>
-      <c r="C4" s="35">
+      <c r="B4" s="35" t="s">
+        <v>1119</v>
+      </c>
+      <c r="C4" s="34">
         <f>DATE(2022,2,6)</f>
         <v>44598</v>
       </c>
-      <c r="D4" s="34" t="s">
-        <v>1122</v>
+      <c r="D4" s="33" t="s">
+        <v>1120</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="36" t="s">
-        <v>1121</v>
-      </c>
-      <c r="C5" s="35">
+      <c r="B5" s="35" t="s">
+        <v>1119</v>
+      </c>
+      <c r="C5" s="34">
         <f t="shared" ref="C5:C6" si="0">DATE(2022,2,6)</f>
         <v>44598</v>
       </c>
-      <c r="D5" s="34" t="s">
-        <v>1122</v>
+      <c r="D5" s="33" t="s">
+        <v>1120</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="36" t="s">
-        <v>1121</v>
-      </c>
-      <c r="C6" s="35">
+      <c r="B6" s="35" t="s">
+        <v>1119</v>
+      </c>
+      <c r="C6" s="34">
         <f t="shared" si="0"/>
         <v>44598</v>
       </c>
-      <c r="D6" s="34" t="s">
-        <v>1122</v>
+      <c r="D6" s="33" t="s">
+        <v>1120</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="37" t="s">
-        <v>1121</v>
-      </c>
-      <c r="C7" s="35">
+      <c r="B7" s="36" t="s">
+        <v>1119</v>
+      </c>
+      <c r="C7" s="34">
         <f>DATE(2022,2,6)+1</f>
         <v>44599</v>
       </c>
-      <c r="D7" s="34" t="s">
-        <v>1122</v>
+      <c r="D7" s="33" t="s">
+        <v>1120</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="38" t="s">
-        <v>1121</v>
-      </c>
-      <c r="C8" s="35">
+      <c r="B8" s="37" t="s">
+        <v>1119</v>
+      </c>
+      <c r="C8" s="34">
         <f>DATE(2022,2,6)+1</f>
         <v>44599</v>
       </c>
-      <c r="D8" s="34" t="s">
-        <v>1122</v>
+      <c r="D8" s="33" t="s">
+        <v>1120</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="36" t="s">
-        <v>1121</v>
-      </c>
-      <c r="C9" s="35">
+      <c r="B9" s="35" t="s">
+        <v>1119</v>
+      </c>
+      <c r="C9" s="34">
         <f t="shared" ref="C9:C12" si="1">DATE(2022,2,6)+1</f>
         <v>44599</v>
       </c>
-      <c r="D9" s="34" t="s">
-        <v>1122</v>
+      <c r="D9" s="33" t="s">
+        <v>1120</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="37" t="s">
-        <v>1121</v>
-      </c>
-      <c r="C10" s="35">
+      <c r="B10" s="36" t="s">
+        <v>1119</v>
+      </c>
+      <c r="C10" s="34">
         <f t="shared" si="1"/>
         <v>44599</v>
       </c>
-      <c r="D10" s="34" t="s">
-        <v>1122</v>
+      <c r="D10" s="33" t="s">
+        <v>1120</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="36" t="s">
-        <v>1121</v>
-      </c>
-      <c r="C11" s="35">
+      <c r="B11" s="35" t="s">
+        <v>1119</v>
+      </c>
+      <c r="C11" s="34">
         <f t="shared" si="1"/>
         <v>44599</v>
       </c>
-      <c r="D11" s="34" t="s">
-        <v>1122</v>
+      <c r="D11" s="33" t="s">
+        <v>1120</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="36" t="s">
-        <v>1121</v>
-      </c>
-      <c r="C12" s="35">
+      <c r="B12" s="35" t="s">
+        <v>1119</v>
+      </c>
+      <c r="C12" s="34">
         <f t="shared" si="1"/>
         <v>44599</v>
       </c>
-      <c r="D12" s="34" t="s">
-        <v>1122</v>
+      <c r="D12" s="33" t="s">
+        <v>1120</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="37" t="s">
-        <v>1121</v>
-      </c>
-      <c r="C13" s="35">
+      <c r="B13" s="36" t="s">
+        <v>1119</v>
+      </c>
+      <c r="C13" s="34">
         <f>DATE(2022,2,6)+1</f>
         <v>44599</v>
       </c>
-      <c r="D13" s="34" t="s">
-        <v>1122</v>
+      <c r="D13" s="33" t="s">
+        <v>1120</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="37" t="s">
-        <v>1121</v>
-      </c>
-      <c r="C14" s="35">
+      <c r="B14" s="36" t="s">
+        <v>1119</v>
+      </c>
+      <c r="C14" s="34">
         <f>DATE(2022,2,6)+2</f>
         <v>44600</v>
       </c>
-      <c r="D14" s="34" t="s">
-        <v>1122</v>
+      <c r="D14" s="33" t="s">
+        <v>1120</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="36" t="s">
-        <v>1121</v>
-      </c>
-      <c r="C15" s="35">
+      <c r="B15" s="35" t="s">
+        <v>1119</v>
+      </c>
+      <c r="C15" s="34">
         <f>DATE(2022,2,6)+2</f>
         <v>44600</v>
       </c>
-      <c r="D15" s="34" t="s">
-        <v>1122</v>
+      <c r="D15" s="33" t="s">
+        <v>1120</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="37" t="s">
-        <v>1121</v>
-      </c>
-      <c r="C16" s="35">
+      <c r="B16" s="36" t="s">
+        <v>1119</v>
+      </c>
+      <c r="C16" s="34">
         <f>DATE(2022,2,6)+3</f>
         <v>44601</v>
       </c>
-      <c r="D16" s="34" t="s">
-        <v>1122</v>
+      <c r="D16" s="33" t="s">
+        <v>1120</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="36" t="s">
-        <v>1121</v>
-      </c>
-      <c r="C17" s="35">
+      <c r="B17" s="35" t="s">
+        <v>1119</v>
+      </c>
+      <c r="C17" s="34">
         <f t="shared" ref="C17:C18" si="2">DATE(2022,2,6)+3</f>
         <v>44601</v>
       </c>
-      <c r="D17" s="34" t="s">
-        <v>1122</v>
+      <c r="D17" s="33" t="s">
+        <v>1120</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A18" s="43" t="s">
+      <c r="A18" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="36" t="s">
-        <v>1121</v>
-      </c>
-      <c r="C18" s="35">
+      <c r="B18" s="35" t="s">
+        <v>1119</v>
+      </c>
+      <c r="C18" s="34">
         <f t="shared" si="2"/>
         <v>44601</v>
       </c>
-      <c r="D18" s="34" t="s">
-        <v>1122</v>
+      <c r="D18" s="33" t="s">
+        <v>1120</v>
       </c>
     </row>
     <row r="19" spans="1:4" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A19" s="33" t="s">
-        <v>1120</v>
+      <c r="A19" s="45" t="s">
+        <v>1130</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
@@ -4610,9 +4626,9 @@
     <row r="80" spans="1:1" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A80" s="27"/>
     </row>
-    <row r="81" spans="1:4" s="40" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="41" t="s">
-        <v>1124</v>
+    <row r="81" spans="1:4" s="39" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="40" t="s">
+        <v>1122</v>
       </c>
       <c r="B81" s="31" t="s">
         <v>1116</v>
@@ -4624,222 +4640,226 @@
         <v>1118</v>
       </c>
     </row>
-    <row r="82" spans="1:4" s="40" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="42" t="s">
-        <v>1125</v>
-      </c>
-      <c r="B82" s="36" t="s">
-        <v>1121</v>
-      </c>
-      <c r="C82" s="35">
+    <row r="82" spans="1:4" s="39" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="41" t="s">
+        <v>1123</v>
+      </c>
+      <c r="B82" s="35" t="s">
+        <v>1119</v>
+      </c>
+      <c r="C82" s="34">
         <f t="shared" ref="C82:C83" si="3">DATE(2022,2,6)+3</f>
         <v>44601</v>
       </c>
-      <c r="D82" s="34" t="s">
-        <v>1122</v>
+      <c r="D82" s="33" t="s">
+        <v>1120</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B83" s="36" t="s">
-        <v>1121</v>
-      </c>
-      <c r="C83" s="35">
+      <c r="B83" s="35" t="s">
+        <v>1119</v>
+      </c>
+      <c r="C83" s="34">
         <f t="shared" si="3"/>
         <v>44601</v>
       </c>
-      <c r="D83" s="34" t="s">
-        <v>1122</v>
+      <c r="D83" s="33" t="s">
+        <v>1120</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B84" s="36" t="s">
-        <v>1121</v>
-      </c>
-      <c r="C84" s="35">
+      <c r="B84" s="35" t="s">
+        <v>1119</v>
+      </c>
+      <c r="C84" s="34">
         <f ca="1">TODAY()-1</f>
-        <v>44613</v>
-      </c>
-      <c r="D84" s="34" t="s">
-        <v>1122</v>
+        <v>44615</v>
+      </c>
+      <c r="D84" s="33" t="s">
+        <v>1120</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B85" s="36" t="s">
-        <v>1121</v>
-      </c>
-      <c r="C85" s="35">
+      <c r="B85" s="35" t="s">
+        <v>1119</v>
+      </c>
+      <c r="C85" s="34">
         <f t="shared" ref="C85:C89" ca="1" si="4">TODAY()-1</f>
-        <v>44613</v>
-      </c>
-      <c r="D85" s="34" t="s">
-        <v>1122</v>
+        <v>44615</v>
+      </c>
+      <c r="D85" s="33" t="s">
+        <v>1120</v>
       </c>
     </row>
     <row r="86" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B86" s="36" t="s">
-        <v>1121</v>
-      </c>
-      <c r="C86" s="35">
+      <c r="B86" s="35" t="s">
+        <v>1119</v>
+      </c>
+      <c r="C86" s="34">
         <f t="shared" ca="1" si="4"/>
-        <v>44613</v>
-      </c>
-      <c r="D86" s="34" t="s">
-        <v>1122</v>
+        <v>44615</v>
+      </c>
+      <c r="D86" s="33" t="s">
+        <v>1120</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B87" s="36" t="s">
-        <v>1121</v>
-      </c>
-      <c r="C87" s="35">
+      <c r="B87" s="35" t="s">
+        <v>1119</v>
+      </c>
+      <c r="C87" s="34">
         <f t="shared" ca="1" si="4"/>
-        <v>44613</v>
-      </c>
-      <c r="D87" s="34" t="s">
-        <v>1122</v>
+        <v>44615</v>
+      </c>
+      <c r="D87" s="33" t="s">
+        <v>1120</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B88" s="36" t="s">
-        <v>1121</v>
-      </c>
-      <c r="C88" s="35">
+      <c r="B88" s="35" t="s">
+        <v>1119</v>
+      </c>
+      <c r="C88" s="34">
         <f t="shared" ca="1" si="4"/>
-        <v>44613</v>
-      </c>
-      <c r="D88" s="34" t="s">
-        <v>1122</v>
+        <v>44615</v>
+      </c>
+      <c r="D88" s="33" t="s">
+        <v>1120</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A89" s="56" t="s">
+      <c r="A89" s="43" t="s">
         <v>78</v>
       </c>
-      <c r="B89" s="37" t="s">
-        <v>1121</v>
-      </c>
-      <c r="C89" s="35">
+      <c r="B89" s="36" t="s">
+        <v>1119</v>
+      </c>
+      <c r="C89" s="34">
         <f t="shared" ca="1" si="4"/>
-        <v>44613</v>
-      </c>
-      <c r="D89" s="34" t="s">
-        <v>1122</v>
+        <v>44615</v>
+      </c>
+      <c r="D89" s="33" t="s">
+        <v>1120</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A90" s="2"/>
-      <c r="C90" s="35"/>
+      <c r="A90" s="44" t="s">
+        <v>1124</v>
+      </c>
+      <c r="C90" s="34"/>
     </row>
     <row r="91" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B91" s="36" t="s">
-        <v>1121</v>
-      </c>
-      <c r="C91" s="35">
+      <c r="B91" s="35" t="s">
+        <v>1119</v>
+      </c>
+      <c r="C91" s="34">
         <f ca="1">TODAY()</f>
-        <v>44614</v>
-      </c>
-      <c r="D91" s="34" t="s">
-        <v>1122</v>
+        <v>44616</v>
+      </c>
+      <c r="D91" s="33" t="s">
+        <v>1120</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B92" s="36" t="s">
-        <v>1121</v>
-      </c>
-      <c r="C92" s="35">
+      <c r="B92" s="35" t="s">
+        <v>1119</v>
+      </c>
+      <c r="C92" s="34">
         <f t="shared" ref="C92:C96" ca="1" si="5">TODAY()</f>
-        <v>44614</v>
-      </c>
-      <c r="D92" s="34" t="s">
-        <v>1122</v>
+        <v>44616</v>
+      </c>
+      <c r="D92" s="33" t="s">
+        <v>1120</v>
       </c>
     </row>
     <row r="93" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A93" s="56" t="s">
+      <c r="A93" s="43" t="s">
         <v>81</v>
       </c>
-      <c r="B93" s="37" t="s">
-        <v>1121</v>
-      </c>
-      <c r="C93" s="35">
+      <c r="B93" s="36" t="s">
+        <v>1119</v>
+      </c>
+      <c r="C93" s="34">
         <f t="shared" ca="1" si="5"/>
-        <v>44614</v>
-      </c>
-      <c r="D93" s="34" t="s">
-        <v>1122</v>
+        <v>44616</v>
+      </c>
+      <c r="D93" s="33" t="s">
+        <v>1120</v>
       </c>
     </row>
     <row r="94" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B94" s="36" t="s">
-        <v>1121</v>
-      </c>
-      <c r="C94" s="35">
+      <c r="B94" s="35" t="s">
+        <v>1119</v>
+      </c>
+      <c r="C94" s="34">
         <f t="shared" ca="1" si="5"/>
-        <v>44614</v>
-      </c>
-      <c r="D94" s="34" t="s">
-        <v>1122</v>
+        <v>44616</v>
+      </c>
+      <c r="D94" s="33" t="s">
+        <v>1120</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B95" s="36" t="s">
-        <v>1121</v>
-      </c>
-      <c r="C95" s="35">
+      <c r="B95" s="35" t="s">
+        <v>1119</v>
+      </c>
+      <c r="C95" s="34">
         <f t="shared" ca="1" si="5"/>
-        <v>44614</v>
-      </c>
-      <c r="D95" s="34" t="s">
-        <v>1122</v>
+        <v>44616</v>
+      </c>
+      <c r="D95" s="33" t="s">
+        <v>1120</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A96" s="43" t="s">
+      <c r="A96" s="42" t="s">
         <v>84</v>
       </c>
-      <c r="B96" s="37" t="s">
-        <v>1121</v>
-      </c>
-      <c r="C96" s="35">
+      <c r="B96" s="36" t="s">
+        <v>1119</v>
+      </c>
+      <c r="C96" s="34">
         <f t="shared" ca="1" si="5"/>
-        <v>44614</v>
-      </c>
-      <c r="D96" s="34" t="s">
-        <v>1122</v>
+        <v>44616</v>
+      </c>
+      <c r="D96" s="33" t="s">
+        <v>1120</v>
       </c>
     </row>
     <row r="97" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A97" s="2"/>
+      <c r="A97" s="44" t="s">
+        <v>1125</v>
+      </c>
     </row>
     <row r="98" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
@@ -4867,7 +4887,9 @@
       </c>
     </row>
     <row r="103" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A103" s="2"/>
+      <c r="A103" s="44" t="s">
+        <v>1126</v>
+      </c>
     </row>
     <row r="104" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
@@ -4905,418 +4927,439 @@
       </c>
     </row>
     <row r="111" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A111" s="2"/>
+      <c r="A111" s="44" t="s">
+        <v>1127</v>
+      </c>
     </row>
     <row r="112" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="113" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="114" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="115" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="116" spans="1:1" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A116" s="27"/>
     </row>
-    <row r="117" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A117" s="2" t="s">
+    <row r="117" spans="1:4" s="39" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A117" s="40" t="s">
+        <v>1128</v>
+      </c>
+      <c r="B117" s="31" t="s">
+        <v>1116</v>
+      </c>
+      <c r="C117" s="31" t="s">
+        <v>1117</v>
+      </c>
+      <c r="D117" s="31" t="s">
+        <v>1118</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A118" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="118" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A118" s="2" t="s">
+    <row r="119" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A119" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="119" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A119" s="2" t="s">
+    <row r="120" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A120" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="120" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A120" s="2" t="s">
+    <row r="121" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A121" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="121" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A121" s="2" t="s">
+    <row r="122" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A122" s="2" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="122" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A122" s="2" t="s">
+    <row r="123" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A123" s="2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="123" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A123" s="2" t="s">
+    <row r="124" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A124" s="2" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="124" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A124" s="2" t="s">
+    <row r="125" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A125" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="125" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A125" s="2" t="s">
+    <row r="126" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A126" s="2" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="126" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A126" s="2" t="s">
+    <row r="127" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A127" s="2" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="127" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A127" s="2" t="s">
+    <row r="128" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A128" s="2" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="128" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A128" s="2" t="s">
+    <row r="129" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A129" s="2" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="129" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A129" s="2" t="s">
+    <row r="130" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A130" s="2" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="130" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A130" s="2" t="s">
+    <row r="131" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A131" s="2" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="131" spans="1:1" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A131" s="27"/>
-    </row>
-    <row r="132" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A132" s="2" t="s">
+    <row r="132" spans="1:4" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A132" s="27"/>
+    </row>
+    <row r="133" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A133" s="2" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="133" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A133" s="2" t="s">
+      <c r="B133" s="35" t="s">
+        <v>1119</v>
+      </c>
+      <c r="C133" s="34">
+        <f ca="1">TODAY()</f>
+        <v>44616</v>
+      </c>
+      <c r="D133" s="33" t="s">
+        <v>1120</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A134" s="2" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="134" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A134" s="2" t="s">
+    <row r="135" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A135" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="135" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A135" s="2" t="s">
+    <row r="136" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A136" s="2" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="136" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A136" s="2" t="s">
+    <row r="137" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A137" s="2" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="137" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A137" s="2" t="s">
+    <row r="138" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A138" s="2" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="138" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A138" s="2" t="s">
+    <row r="139" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A139" s="2" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="139" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A139" s="2" t="s">
+    <row r="140" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A140" s="2" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="140" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A140" s="2" t="s">
+    <row r="141" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A141" s="2" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="141" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A141" s="2" t="s">
+    <row r="142" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A142" s="2" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="142" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A142" s="2" t="s">
+    <row r="143" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A143" s="2" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="143" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A143" s="2" t="s">
+    <row r="144" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A144" s="2" t="s">
         <v>126</v>
-      </c>
-    </row>
-    <row r="144" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A144" s="2" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="145" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="146" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="147" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="148" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="149" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="150" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="151" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="152" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A153" s="2" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="153" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A153" s="2"/>
-    </row>
     <row r="154" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A154" s="2" t="s">
-        <v>136</v>
-      </c>
+      <c r="A154" s="2"/>
     </row>
     <row r="155" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="156" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="157" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="158" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="159" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="160" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="161" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="162" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="163" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="164" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="165" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="166" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="167" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="168" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="169" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="170" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="171" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="172" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="173" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A173" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="174" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A174" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="175" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="176" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A176" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="177" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A177" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="178" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A178" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="179" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="180" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="181" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="182" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="183" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A184" s="2" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="184" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A184" s="2"/>
-    </row>
     <row r="185" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A185" s="2" t="s">
-        <v>166</v>
-      </c>
+      <c r="A185" s="2"/>
     </row>
     <row r="186" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A186" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="187" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A187" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="188" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A188" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="189" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A189" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="190" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A190" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="191" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A191" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="192" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A192" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="193" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A193" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="194" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A194" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="195" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A195" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="196" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
@@ -5326,1854 +5369,1859 @@
     </row>
     <row r="197" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A197" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="198" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A198" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="199" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A199" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="200" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A200" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="201" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A201" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="202" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A202" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="203" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A203" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="204" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A204" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="205" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A205" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="206" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="207" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="208" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A208" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="209" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A209" s="2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A210" s="2" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="210" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A210" s="2"/>
-    </row>
     <row r="211" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A211" s="2" t="s">
-        <v>190</v>
-      </c>
+      <c r="A211" s="2"/>
     </row>
     <row r="212" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A212" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="213" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A213" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="214" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A214" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="215" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A215" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="216" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A216" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="217" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A217" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="218" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A218" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="219" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A219" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="220" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A220" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="221" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A221" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="222" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A222" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="223" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A223" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="224" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A224" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="225" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A225" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="226" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A226" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="227" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A227" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="228" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A228" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="229" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A229" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="230" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A230" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="231" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A231" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="232" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A232" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="233" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A233" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="234" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A234" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="235" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A235" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="236" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A236" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="237" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A237" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="238" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A238" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="239" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A239" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="240" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A240" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="241" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A241" s="2" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="242" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A242" s="2" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="242" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A242" s="2"/>
-    </row>
     <row r="243" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A243" s="2" t="s">
-        <v>221</v>
-      </c>
+      <c r="A243" s="2"/>
     </row>
     <row r="244" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A244" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="245" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A245" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="246" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A246" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="247" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A247" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="248" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A248" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="249" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A249" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="250" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A250" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="251" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A251" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="252" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A252" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="253" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A253" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="254" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A254" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="255" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A255" s="2" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="256" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A256" s="2" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="256" spans="1:1" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A256" s="27"/>
-    </row>
-    <row r="257" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A257" s="2" t="s">
-        <v>234</v>
-      </c>
+    <row r="257" spans="1:1" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A257" s="27"/>
     </row>
     <row r="258" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A258" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="259" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A259" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="260" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A260" s="2" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="261" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A261" s="2" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="261" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A261" s="2"/>
-    </row>
     <row r="262" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A262" s="2" t="s">
-        <v>238</v>
-      </c>
+      <c r="A262" s="2"/>
     </row>
     <row r="263" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A263" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="264" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A264" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="265" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A265" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="266" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A266" s="2" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="267" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A267" s="2" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="267" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A267" s="2"/>
-    </row>
     <row r="268" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A268" s="2" t="s">
-        <v>243</v>
-      </c>
+      <c r="A268" s="2"/>
     </row>
     <row r="269" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A269" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="270" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A270" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="271" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A271" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="272" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A272" s="2" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="273" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A273" s="2" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="273" spans="1:1" s="30" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A273" s="29"/>
-    </row>
-    <row r="274" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A274" s="2" t="s">
-        <v>248</v>
-      </c>
+    <row r="274" spans="1:1" s="30" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A274" s="29"/>
     </row>
     <row r="275" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A275" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="276" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A276" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="277" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A277" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="278" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A278" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="279" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A279" s="2" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="280" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A280" s="2" t="s">
         <v>253</v>
-      </c>
-    </row>
-    <row r="280" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A280" s="3" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="281" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A281" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="282" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A282" s="3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="283" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A283" s="3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="284" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A284" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="285" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A285" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="286" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A286" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="287" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A287" s="3" t="s">
         <v>260</v>
-      </c>
-    </row>
-    <row r="287" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A287" s="2" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="288" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A288" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="289" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A289" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="290" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A290" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="291" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A291" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="292" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A292" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="293" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A293" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="294" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A294" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="295" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A295" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="296" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A296" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="297" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A297" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="298" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A298" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="299" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A299" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="300" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A300" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="301" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A301" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="302" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A302" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="303" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A303" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="304" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A304" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="305" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A305" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="306" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A306" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="307" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A307" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="308" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A308" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="309" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A309" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="310" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A310" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="311" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A311" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="312" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A312" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="313" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A313" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="314" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A314" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="315" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A315" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="316" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A316" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="317" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A317" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="318" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A318" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="319" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A319" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="320" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A320" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="321" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A321" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="322" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A322" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="323" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A323" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="324" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A324" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="325" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A325" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="326" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A326" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="327" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A327" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="328" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A328" s="2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="329" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A329" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="330" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A330" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="331" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A331" s="2" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="332" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A332" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="333" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A333" s="2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="334" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A334" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="335" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A335" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="336" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A336" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="337" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A337" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="338" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A338" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="339" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A339" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="340" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A340" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="341" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A341" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="342" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A342" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="343" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A343" s="2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="344" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A344" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="345" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A345" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="346" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A346" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="347" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A347" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="348" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A348" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="349" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A349" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="350" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A350" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="351" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A351" s="2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="352" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A352" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="353" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A353" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="354" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A354" s="2" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="355" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A355" s="2" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="355" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A355" s="3" t="s">
+    <row r="356" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A356" s="3" t="s">
         <v>329</v>
-      </c>
-    </row>
-    <row r="356" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A356" s="2" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="357" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A357" s="2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="358" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A358" s="2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="359" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A359" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="360" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A360" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="361" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A361" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="362" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A362" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="363" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A363" s="2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="364" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A364" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="365" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A365" s="2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="366" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A366" s="2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="367" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A367" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="368" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A368" s="2" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="369" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A369" s="2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="370" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A370" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="371" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A371" s="2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="372" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A372" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="373" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A373" s="2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="374" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A374" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="375" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A375" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="376" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A376" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="377" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A377" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="378" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A378" s="2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="379" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A379" s="2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="380" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A380" s="2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="381" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A381" s="2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="382" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A382" s="2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="383" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A383" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="384" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A384" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="385" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A385" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="386" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A386" s="2" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="387" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A387" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="388" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A388" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="389" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A389" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="390" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A390" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="391" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A391" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="392" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A392" s="2" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="393" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A393" s="2" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="394" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A394" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="395" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A395" s="2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="396" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A396" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="397" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A397" s="2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="398" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A398" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="399" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A399" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="400" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A400" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="401" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A401" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="402" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A402" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="403" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A403" s="2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="404" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A404" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="405" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A405" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="406" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A406" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="407" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A407" s="2" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="408" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A408" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="409" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A409" s="2" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="410" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A410" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="411" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A411" s="2" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="412" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A412" s="2" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="413" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A413" s="2" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="414" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A414" s="2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="415" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A415" s="2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="416" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A416" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="417" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A417" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="418" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A418" s="2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="419" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A419" s="2" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="420" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A420" s="2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="421" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A421" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="422" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A422" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="423" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A423" s="2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="424" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A424" s="2" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="425" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A425" s="2" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="426" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A426" s="2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="427" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A427" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="428" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A428" s="2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="429" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A429" s="2" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="430" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A430" s="2" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="431" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A431" s="2" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="432" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A432" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="433" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A433" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="434" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A434" s="2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="435" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A435" s="2" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="436" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A436" s="2" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="437" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A437" s="2" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="438" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A438" s="2" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="439" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A439" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="440" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A440" s="2" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="441" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A441" s="2" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="442" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A442" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="443" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A443" s="2" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="444" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A444" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="445" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A445" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="446" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A446" s="2" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="447" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A447" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="448" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A448" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="449" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A449" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="450" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A450" s="2" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="451" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A451" s="2" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="452" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A452" s="2" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="453" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A453" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="454" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A454" s="2" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="455" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A455" s="2" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="456" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A456" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="457" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A457" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="458" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A458" s="2" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="459" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A459" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="460" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A460" s="2" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="461" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A461" s="2" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="462" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A462" s="2" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="463" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A463" s="2" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="464" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A464" s="2" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="465" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A465" s="2" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="466" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A466" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="467" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A467" s="2" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="468" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A468" s="2" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="469" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A469" s="2" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="470" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A470" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="471" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A471" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="472" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A472" s="2" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="473" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A473" s="2" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="474" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A474" s="2" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="475" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A475" s="2" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="476" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A476" s="2" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="477" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A477" s="2" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="478" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A478" s="2" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="479" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A479" s="2" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="480" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A480" s="2" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="481" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A481" s="2" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="482" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A482" s="2" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="483" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A483" s="2" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="484" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A484" s="2" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="485" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A485" s="2" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="486" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A486" s="2" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="487" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A487" s="2" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="488" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A488" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="489" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A489" s="2" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="490" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A490" s="2" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="491" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A491" s="2" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="492" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A492" s="2" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="493" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A493" s="2" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="494" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A494" s="2" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="495" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A495" s="2" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="496" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A496" s="2" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="497" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A497" s="2" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="498" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A498" s="2" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="499" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A499" s="2" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="500" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A500" s="2" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="501" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A501" s="2" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="502" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A502" s="2" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="503" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A503" s="2" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="504" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A504" s="2" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="505" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A505" s="2" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="506" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A506" s="2" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="507" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A507" s="2" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="508" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A508" s="2" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="509" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A509" s="2" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="510" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A510" s="2" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="511" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A511" s="2" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="512" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A512" s="2" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="513" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A513" s="2" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="514" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A514" s="2" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="515" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A515" s="2" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="516" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A516" s="2" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="517" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A517" s="2" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="518" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A518" s="2" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="519" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A519" s="2" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="520" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A520" s="2" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="521" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A521" s="2" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="522" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A522" s="2" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="523" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A523" s="2" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="524" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A524" s="2" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="525" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A525" s="2" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="526" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A526" s="2" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="527" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A527" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="528" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A528" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="529" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A529" s="2" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="530" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A530" s="2" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="531" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A531" s="2" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="532" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A532" s="2" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="533" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A533" s="2" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="534" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A534" s="2" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="535" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A535" s="2" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="536" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A536" s="2" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="537" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A537" s="2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="538" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A538" s="2" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="539" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A539" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="540" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A540" s="2" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="541" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A541" s="2" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="542" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A542" s="2" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="543" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A543" s="2" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="544" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A544" s="2" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="545" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A545" s="2" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="546" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A546" s="2" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="547" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A547" s="2" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="548" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A548" s="2" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="549" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A549" s="2" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="550" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A550" s="2" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="551" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A551" s="2" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="552" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A552" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="553" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A553" s="2" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="554" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A554" s="2" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="555" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A555" s="2" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="556" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A556" s="2" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="557" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A557" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="558" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A558" s="2" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="559" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A559" s="2" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="560" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A560" s="2" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="561" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A561" s="2" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="562" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A562" s="2" t="s">
         <v>535</v>
-      </c>
-    </row>
-    <row r="562" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A562" s="3" t="s">
-        <v>536</v>
       </c>
     </row>
     <row r="563" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A563" s="3" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="564" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A564" s="3" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="565" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A565" s="3" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="566" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A566" s="3" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="567" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A567" s="3" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="568" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A568" s="3" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="569" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A569" s="3" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="570" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A570" s="3" t="s">
         <v>543</v>
       </c>
     </row>
@@ -7203,7 +7251,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="54" t="s">
         <v>544</v>
       </c>
       <c r="B1" s="4" t="s">
@@ -7215,7 +7263,7 @@
       <c r="D1" s="2"/>
     </row>
     <row r="2" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A2" s="45"/>
+      <c r="A2" s="47"/>
       <c r="B2" s="6" t="s">
         <v>547</v>
       </c>
@@ -7225,7 +7273,7 @@
       <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A3" s="45"/>
+      <c r="A3" s="47"/>
       <c r="B3" s="6" t="s">
         <v>547</v>
       </c>
@@ -7235,7 +7283,7 @@
       <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A4" s="45"/>
+      <c r="A4" s="47"/>
       <c r="B4" s="6" t="s">
         <v>547</v>
       </c>
@@ -7245,29 +7293,29 @@
       <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A5" s="45"/>
+      <c r="A5" s="47"/>
       <c r="B5" s="6" t="s">
         <v>551</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>552</v>
       </c>
-      <c r="D5" s="44" t="s">
+      <c r="D5" s="46" t="s">
         <v>553</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A6" s="45"/>
+      <c r="A6" s="47"/>
       <c r="B6" s="6" t="s">
         <v>551</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>554</v>
       </c>
-      <c r="D6" s="45"/>
+      <c r="D6" s="47"/>
     </row>
     <row r="7" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A7" s="45"/>
+      <c r="A7" s="47"/>
       <c r="B7" s="9" t="s">
         <v>555</v>
       </c>
@@ -7277,7 +7325,7 @@
       <c r="D7" s="10"/>
     </row>
     <row r="8" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A8" s="45"/>
+      <c r="A8" s="47"/>
       <c r="B8" s="2" t="s">
         <v>557</v>
       </c>
@@ -7287,39 +7335,39 @@
       <c r="D8" s="10"/>
     </row>
     <row r="9" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A9" s="45"/>
+      <c r="A9" s="47"/>
       <c r="B9" s="6" t="s">
         <v>559</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>560</v>
       </c>
-      <c r="D9" s="44" t="s">
+      <c r="D9" s="46" t="s">
         <v>561</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A10" s="45"/>
+      <c r="A10" s="47"/>
       <c r="B10" s="6" t="s">
         <v>559</v>
       </c>
       <c r="C10" s="12" t="s">
         <v>562</v>
       </c>
-      <c r="D10" s="45"/>
+      <c r="D10" s="47"/>
     </row>
     <row r="11" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A11" s="45"/>
+      <c r="A11" s="47"/>
       <c r="B11" s="6" t="s">
         <v>559</v>
       </c>
       <c r="C11" s="12" t="s">
         <v>563</v>
       </c>
-      <c r="D11" s="45"/>
+      <c r="D11" s="47"/>
     </row>
     <row r="12" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A12" s="45"/>
+      <c r="A12" s="47"/>
       <c r="B12" s="9" t="s">
         <v>564</v>
       </c>
@@ -7329,39 +7377,39 @@
       <c r="D12" s="10"/>
     </row>
     <row r="13" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A13" s="45"/>
+      <c r="A13" s="47"/>
       <c r="B13" s="6" t="s">
         <v>566</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>567</v>
       </c>
-      <c r="D13" s="44" t="s">
+      <c r="D13" s="46" t="s">
         <v>568</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A14" s="45"/>
+      <c r="A14" s="47"/>
       <c r="B14" s="6" t="s">
         <v>566</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>569</v>
       </c>
-      <c r="D14" s="45"/>
+      <c r="D14" s="47"/>
     </row>
     <row r="15" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A15" s="45"/>
+      <c r="A15" s="47"/>
       <c r="B15" s="6" t="s">
         <v>566</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>569</v>
       </c>
-      <c r="D15" s="45"/>
+      <c r="D15" s="47"/>
     </row>
     <row r="16" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A16" s="45"/>
+      <c r="A16" s="47"/>
       <c r="B16" s="9" t="s">
         <v>570</v>
       </c>
@@ -7371,7 +7419,7 @@
       <c r="D16" s="2"/>
     </row>
     <row r="17" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A17" s="45"/>
+      <c r="A17" s="47"/>
       <c r="B17" s="6" t="s">
         <v>566</v>
       </c>
@@ -7381,7 +7429,7 @@
       <c r="D17" s="10"/>
     </row>
     <row r="18" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A18" s="45"/>
+      <c r="A18" s="47"/>
       <c r="B18" s="6" t="s">
         <v>566</v>
       </c>
@@ -7391,7 +7439,7 @@
       <c r="D18" s="10"/>
     </row>
     <row r="19" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A19" s="45"/>
+      <c r="A19" s="47"/>
       <c r="B19" s="9" t="s">
         <v>574</v>
       </c>
@@ -7401,7 +7449,7 @@
       <c r="D19" s="10"/>
     </row>
     <row r="20" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A20" s="45"/>
+      <c r="A20" s="47"/>
       <c r="B20" s="2" t="s">
         <v>557</v>
       </c>
@@ -7411,7 +7459,7 @@
       <c r="D20" s="10"/>
     </row>
     <row r="21" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A21" s="49" t="s">
+      <c r="A21" s="51" t="s">
         <v>577</v>
       </c>
       <c r="B21" s="6" t="s">
@@ -7423,7 +7471,7 @@
       <c r="D21" s="2"/>
     </row>
     <row r="22" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A22" s="45"/>
+      <c r="A22" s="47"/>
       <c r="B22" s="6" t="s">
         <v>578</v>
       </c>
@@ -7433,7 +7481,7 @@
       <c r="D22" s="2"/>
     </row>
     <row r="23" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A23" s="45"/>
+      <c r="A23" s="47"/>
       <c r="B23" s="6" t="s">
         <v>578</v>
       </c>
@@ -7443,7 +7491,7 @@
       <c r="D23" s="2"/>
     </row>
     <row r="24" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A24" s="45"/>
+      <c r="A24" s="47"/>
       <c r="B24" s="10" t="s">
         <v>582</v>
       </c>
@@ -7453,37 +7501,37 @@
       <c r="D24" s="2"/>
     </row>
     <row r="25" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A25" s="45"/>
+      <c r="A25" s="47"/>
       <c r="B25" s="13" t="s">
         <v>584</v>
       </c>
       <c r="C25" s="7"/>
-      <c r="D25" s="46" t="s">
+      <c r="D25" s="48" t="s">
         <v>585</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A26" s="45"/>
+      <c r="A26" s="47"/>
       <c r="B26" s="6" t="s">
         <v>584</v>
       </c>
       <c r="C26" s="7" t="s">
         <v>586</v>
       </c>
-      <c r="D26" s="47"/>
+      <c r="D26" s="49"/>
     </row>
     <row r="27" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A27" s="45"/>
+      <c r="A27" s="47"/>
       <c r="B27" s="6" t="s">
         <v>584</v>
       </c>
       <c r="C27" s="7" t="s">
         <v>587</v>
       </c>
-      <c r="D27" s="48"/>
+      <c r="D27" s="50"/>
     </row>
     <row r="28" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A28" s="45"/>
+      <c r="A28" s="47"/>
       <c r="B28" s="2" t="s">
         <v>582</v>
       </c>
@@ -7493,39 +7541,39 @@
       <c r="D28" s="2"/>
     </row>
     <row r="29" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A29" s="45"/>
+      <c r="A29" s="47"/>
       <c r="B29" s="6" t="s">
         <v>589</v>
       </c>
       <c r="C29" s="7" t="s">
         <v>590</v>
       </c>
-      <c r="D29" s="44" t="s">
+      <c r="D29" s="46" t="s">
         <v>591</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A30" s="45"/>
+      <c r="A30" s="47"/>
       <c r="B30" s="6" t="s">
         <v>589</v>
       </c>
       <c r="C30" s="7" t="s">
         <v>592</v>
       </c>
-      <c r="D30" s="45"/>
+      <c r="D30" s="47"/>
     </row>
     <row r="31" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A31" s="45"/>
+      <c r="A31" s="47"/>
       <c r="B31" s="6" t="s">
         <v>589</v>
       </c>
       <c r="C31" s="7" t="s">
         <v>593</v>
       </c>
-      <c r="D31" s="45"/>
+      <c r="D31" s="47"/>
     </row>
     <row r="32" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A32" s="45"/>
+      <c r="A32" s="47"/>
       <c r="B32" s="6" t="s">
         <v>594</v>
       </c>
@@ -7535,7 +7583,7 @@
       <c r="D32" s="2"/>
     </row>
     <row r="33" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A33" s="45"/>
+      <c r="A33" s="47"/>
       <c r="B33" s="2" t="s">
         <v>596</v>
       </c>
@@ -7545,39 +7593,39 @@
       <c r="D33" s="2"/>
     </row>
     <row r="34" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A34" s="45"/>
+      <c r="A34" s="47"/>
       <c r="B34" s="6" t="s">
         <v>598</v>
       </c>
       <c r="C34" s="7" t="s">
         <v>599</v>
       </c>
-      <c r="D34" s="46" t="s">
+      <c r="D34" s="48" t="s">
         <v>600</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A35" s="45"/>
+      <c r="A35" s="47"/>
       <c r="B35" s="6" t="s">
         <v>598</v>
       </c>
       <c r="C35" s="7" t="s">
         <v>601</v>
       </c>
-      <c r="D35" s="47"/>
+      <c r="D35" s="49"/>
     </row>
     <row r="36" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A36" s="45"/>
+      <c r="A36" s="47"/>
       <c r="B36" s="6" t="s">
         <v>598</v>
       </c>
       <c r="C36" s="7" t="s">
         <v>602</v>
       </c>
-      <c r="D36" s="48"/>
+      <c r="D36" s="50"/>
     </row>
     <row r="37" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A37" s="45"/>
+      <c r="A37" s="47"/>
       <c r="B37" s="6" t="s">
         <v>598</v>
       </c>
@@ -7587,7 +7635,7 @@
       <c r="D37" s="2"/>
     </row>
     <row r="38" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A38" s="45"/>
+      <c r="A38" s="47"/>
       <c r="B38" s="2" t="s">
         <v>582</v>
       </c>
@@ -7597,7 +7645,7 @@
       <c r="D38" s="2"/>
     </row>
     <row r="39" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A39" s="45"/>
+      <c r="A39" s="47"/>
       <c r="B39" s="9" t="s">
         <v>605</v>
       </c>
@@ -7607,7 +7655,7 @@
       <c r="D39" s="2"/>
     </row>
     <row r="40" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A40" s="50" t="s">
+      <c r="A40" s="52" t="s">
         <v>607</v>
       </c>
       <c r="B40" s="6" t="s">
@@ -7619,7 +7667,7 @@
       <c r="D40" s="2"/>
     </row>
     <row r="41" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A41" s="45"/>
+      <c r="A41" s="47"/>
       <c r="B41" s="6" t="s">
         <v>608</v>
       </c>
@@ -7629,7 +7677,7 @@
       <c r="D41" s="2"/>
     </row>
     <row r="42" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A42" s="45"/>
+      <c r="A42" s="47"/>
       <c r="B42" s="6" t="s">
         <v>608</v>
       </c>
@@ -7639,51 +7687,51 @@
       <c r="D42" s="2"/>
     </row>
     <row r="43" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A43" s="45"/>
+      <c r="A43" s="47"/>
       <c r="B43" s="6" t="s">
         <v>612</v>
       </c>
       <c r="C43" s="7"/>
-      <c r="D43" s="44" t="s">
+      <c r="D43" s="46" t="s">
         <v>613</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A44" s="45"/>
+      <c r="A44" s="47"/>
       <c r="B44" s="6" t="s">
         <v>612</v>
       </c>
       <c r="C44" s="7"/>
-      <c r="D44" s="45"/>
+      <c r="D44" s="47"/>
     </row>
     <row r="45" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A45" s="45"/>
+      <c r="A45" s="47"/>
       <c r="B45" s="6" t="s">
         <v>612</v>
       </c>
       <c r="C45" s="7"/>
-      <c r="D45" s="45"/>
+      <c r="D45" s="47"/>
     </row>
     <row r="46" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A46" s="45"/>
+      <c r="A46" s="47"/>
       <c r="B46" s="6" t="s">
         <v>612</v>
       </c>
       <c r="C46" s="7"/>
-      <c r="D46" s="45"/>
+      <c r="D46" s="47"/>
     </row>
     <row r="47" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A47" s="45"/>
+      <c r="A47" s="47"/>
       <c r="B47" s="6" t="s">
         <v>614</v>
       </c>
       <c r="C47" s="7" t="s">
         <v>615</v>
       </c>
-      <c r="D47" s="45"/>
+      <c r="D47" s="47"/>
     </row>
     <row r="48" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A48" s="45"/>
+      <c r="A48" s="47"/>
       <c r="B48" s="6" t="s">
         <v>614</v>
       </c>
@@ -7693,7 +7741,7 @@
       <c r="D48" s="2"/>
     </row>
     <row r="49" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A49" s="45"/>
+      <c r="A49" s="47"/>
       <c r="B49" s="6" t="s">
         <v>614</v>
       </c>
@@ -7703,7 +7751,7 @@
       <c r="D49" s="2"/>
     </row>
     <row r="50" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A50" s="45"/>
+      <c r="A50" s="47"/>
       <c r="B50" s="2" t="s">
         <v>618</v>
       </c>
@@ -7711,57 +7759,57 @@
       <c r="D50" s="2"/>
     </row>
     <row r="51" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A51" s="45"/>
+      <c r="A51" s="47"/>
       <c r="B51" s="6" t="s">
         <v>619</v>
       </c>
       <c r="C51" s="7"/>
-      <c r="D51" s="46" t="s">
+      <c r="D51" s="48" t="s">
         <v>620</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A52" s="45"/>
+      <c r="A52" s="47"/>
       <c r="B52" s="6" t="s">
         <v>619</v>
       </c>
       <c r="C52" s="7"/>
-      <c r="D52" s="47"/>
+      <c r="D52" s="49"/>
     </row>
     <row r="53" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A53" s="45"/>
+      <c r="A53" s="47"/>
       <c r="B53" s="6" t="s">
         <v>619</v>
       </c>
       <c r="C53" s="7"/>
-      <c r="D53" s="47"/>
+      <c r="D53" s="49"/>
     </row>
     <row r="54" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A54" s="45"/>
+      <c r="A54" s="47"/>
       <c r="B54" s="6" t="s">
         <v>619</v>
       </c>
       <c r="C54" s="7"/>
-      <c r="D54" s="47"/>
+      <c r="D54" s="49"/>
     </row>
     <row r="55" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A55" s="45"/>
+      <c r="A55" s="47"/>
       <c r="B55" s="6" t="s">
         <v>619</v>
       </c>
       <c r="C55" s="7"/>
-      <c r="D55" s="47"/>
+      <c r="D55" s="49"/>
     </row>
     <row r="56" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A56" s="45"/>
+      <c r="A56" s="47"/>
       <c r="B56" s="6" t="s">
         <v>619</v>
       </c>
       <c r="C56" s="7"/>
-      <c r="D56" s="48"/>
+      <c r="D56" s="50"/>
     </row>
     <row r="57" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A57" s="45"/>
+      <c r="A57" s="47"/>
       <c r="B57" s="6" t="s">
         <v>621</v>
       </c>
@@ -7771,7 +7819,7 @@
       <c r="D57" s="2"/>
     </row>
     <row r="58" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A58" s="45"/>
+      <c r="A58" s="47"/>
       <c r="B58" s="6" t="s">
         <v>621</v>
       </c>
@@ -7781,7 +7829,7 @@
       <c r="D58" s="2"/>
     </row>
     <row r="59" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A59" s="45"/>
+      <c r="A59" s="47"/>
       <c r="B59" s="6" t="s">
         <v>621</v>
       </c>
@@ -7793,33 +7841,33 @@
       </c>
     </row>
     <row r="60" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A60" s="45"/>
+      <c r="A60" s="47"/>
       <c r="B60" s="6" t="s">
         <v>626</v>
       </c>
       <c r="C60" s="7"/>
-      <c r="D60" s="44" t="s">
+      <c r="D60" s="46" t="s">
         <v>627</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A61" s="45"/>
+      <c r="A61" s="47"/>
       <c r="B61" s="6" t="s">
         <v>626</v>
       </c>
       <c r="C61" s="7"/>
-      <c r="D61" s="45"/>
+      <c r="D61" s="47"/>
     </row>
     <row r="62" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A62" s="45"/>
+      <c r="A62" s="47"/>
       <c r="B62" s="6" t="s">
         <v>626</v>
       </c>
       <c r="C62" s="7"/>
-      <c r="D62" s="45"/>
+      <c r="D62" s="47"/>
     </row>
     <row r="63" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A63" s="45"/>
+      <c r="A63" s="47"/>
       <c r="B63" s="6" t="s">
         <v>626</v>
       </c>
@@ -7827,7 +7875,7 @@
       <c r="D63" s="8"/>
     </row>
     <row r="64" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A64" s="51" t="s">
+      <c r="A64" s="53" t="s">
         <v>628</v>
       </c>
       <c r="B64" s="9" t="s">
@@ -7837,7 +7885,7 @@
       <c r="D64" s="8"/>
     </row>
     <row r="65" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A65" s="45"/>
+      <c r="A65" s="47"/>
       <c r="B65" s="9" t="s">
         <v>629</v>
       </c>
@@ -7845,7 +7893,7 @@
       <c r="D65" s="2"/>
     </row>
     <row r="66" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A66" s="45"/>
+      <c r="A66" s="47"/>
       <c r="B66" s="9" t="s">
         <v>629</v>
       </c>
@@ -7853,7 +7901,7 @@
       <c r="D66" s="2"/>
     </row>
     <row r="67" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A67" s="45"/>
+      <c r="A67" s="47"/>
       <c r="B67" s="9" t="s">
         <v>629</v>
       </c>
@@ -7861,7 +7909,7 @@
       <c r="D67" s="2"/>
     </row>
     <row r="68" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A68" s="45"/>
+      <c r="A68" s="47"/>
       <c r="B68" s="9" t="s">
         <v>630</v>
       </c>
@@ -7869,7 +7917,7 @@
       <c r="D68" s="2"/>
     </row>
     <row r="69" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A69" s="45"/>
+      <c r="A69" s="47"/>
       <c r="B69" s="9" t="s">
         <v>630</v>
       </c>
@@ -7877,7 +7925,7 @@
       <c r="D69" s="2"/>
     </row>
     <row r="70" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A70" s="45"/>
+      <c r="A70" s="47"/>
       <c r="B70" s="9" t="s">
         <v>630</v>
       </c>
@@ -7885,7 +7933,7 @@
       <c r="D70" s="2"/>
     </row>
     <row r="71" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A71" s="45"/>
+      <c r="A71" s="47"/>
       <c r="B71" s="9" t="s">
         <v>630</v>
       </c>
@@ -7893,7 +7941,7 @@
       <c r="D71" s="2"/>
     </row>
     <row r="72" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A72" s="45"/>
+      <c r="A72" s="47"/>
       <c r="B72" s="9" t="s">
         <v>631</v>
       </c>
@@ -7901,7 +7949,7 @@
       <c r="D72" s="2"/>
     </row>
     <row r="73" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A73" s="45"/>
+      <c r="A73" s="47"/>
       <c r="B73" s="9" t="s">
         <v>631</v>
       </c>
@@ -7909,7 +7957,7 @@
       <c r="D73" s="2"/>
     </row>
     <row r="74" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A74" s="45"/>
+      <c r="A74" s="47"/>
       <c r="B74" s="9" t="s">
         <v>631</v>
       </c>
@@ -7917,7 +7965,7 @@
       <c r="D74" s="2"/>
     </row>
     <row r="75" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A75" s="53" t="s">
+      <c r="A75" s="55" t="s">
         <v>632</v>
       </c>
       <c r="B75" s="6" t="s">
@@ -7926,32 +7974,32 @@
       <c r="C75" s="7" t="s">
         <v>634</v>
       </c>
-      <c r="D75" s="44" t="s">
+      <c r="D75" s="46" t="s">
         <v>635</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A76" s="45"/>
+      <c r="A76" s="47"/>
       <c r="B76" s="6" t="s">
         <v>633</v>
       </c>
       <c r="C76" s="7" t="s">
         <v>636</v>
       </c>
-      <c r="D76" s="45"/>
+      <c r="D76" s="47"/>
     </row>
     <row r="77" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A77" s="45"/>
+      <c r="A77" s="47"/>
       <c r="B77" s="6" t="s">
         <v>633</v>
       </c>
       <c r="C77" s="7" t="s">
         <v>637</v>
       </c>
-      <c r="D77" s="45"/>
+      <c r="D77" s="47"/>
     </row>
     <row r="78" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A78" s="45"/>
+      <c r="A78" s="47"/>
       <c r="B78" s="6" t="s">
         <v>633</v>
       </c>
@@ -7961,7 +8009,7 @@
       <c r="D78" s="2"/>
     </row>
     <row r="79" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A79" s="45"/>
+      <c r="A79" s="47"/>
       <c r="B79" s="6" t="s">
         <v>633</v>
       </c>
@@ -7971,7 +8019,7 @@
       <c r="D79" s="2"/>
     </row>
     <row r="80" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A80" s="45"/>
+      <c r="A80" s="47"/>
       <c r="B80" s="6" t="s">
         <v>633</v>
       </c>
@@ -7981,7 +8029,7 @@
       <c r="D80" s="2"/>
     </row>
     <row r="81" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A81" s="45"/>
+      <c r="A81" s="47"/>
       <c r="B81" s="6" t="s">
         <v>633</v>
       </c>
@@ -7991,7 +8039,7 @@
       <c r="D81" s="2"/>
     </row>
     <row r="82" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A82" s="45"/>
+      <c r="A82" s="47"/>
       <c r="B82" s="6" t="s">
         <v>633</v>
       </c>
@@ -8001,7 +8049,7 @@
       <c r="D82" s="2"/>
     </row>
     <row r="83" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A83" s="45"/>
+      <c r="A83" s="47"/>
       <c r="B83" s="6" t="s">
         <v>633</v>
       </c>
@@ -8011,7 +8059,7 @@
       <c r="D83" s="2"/>
     </row>
     <row r="84" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A84" s="45"/>
+      <c r="A84" s="47"/>
       <c r="B84" s="6" t="s">
         <v>633</v>
       </c>
@@ -8021,7 +8069,7 @@
       <c r="D84" s="2"/>
     </row>
     <row r="85" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A85" s="45"/>
+      <c r="A85" s="47"/>
       <c r="B85" s="6" t="s">
         <v>633</v>
       </c>
@@ -8031,7 +8079,7 @@
       <c r="D85" s="2"/>
     </row>
     <row r="86" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A86" s="45"/>
+      <c r="A86" s="47"/>
       <c r="B86" s="6" t="s">
         <v>633</v>
       </c>
@@ -8041,7 +8089,7 @@
       <c r="D86" s="2"/>
     </row>
     <row r="87" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A87" s="45"/>
+      <c r="A87" s="47"/>
       <c r="B87" s="6" t="s">
         <v>647</v>
       </c>
@@ -8051,7 +8099,7 @@
       <c r="D87" s="2"/>
     </row>
     <row r="88" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A88" s="45"/>
+      <c r="A88" s="47"/>
       <c r="B88" s="6" t="s">
         <v>647</v>
       </c>
@@ -8061,7 +8109,7 @@
       <c r="D88" s="2"/>
     </row>
     <row r="89" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A89" s="45"/>
+      <c r="A89" s="47"/>
       <c r="B89" s="6" t="s">
         <v>647</v>
       </c>
@@ -8071,7 +8119,7 @@
       <c r="D89" s="2"/>
     </row>
     <row r="90" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A90" s="45"/>
+      <c r="A90" s="47"/>
       <c r="B90" s="6" t="s">
         <v>647</v>
       </c>
@@ -8081,7 +8129,7 @@
       <c r="D90" s="2"/>
     </row>
     <row r="91" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A91" s="45"/>
+      <c r="A91" s="47"/>
       <c r="B91" s="6" t="s">
         <v>647</v>
       </c>
@@ -8091,7 +8139,7 @@
       <c r="D91" s="10"/>
     </row>
     <row r="92" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A92" s="45"/>
+      <c r="A92" s="47"/>
       <c r="B92" s="14" t="s">
         <v>647</v>
       </c>
@@ -8101,7 +8149,7 @@
       <c r="D92" s="10"/>
     </row>
     <row r="93" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A93" s="45"/>
+      <c r="A93" s="47"/>
       <c r="B93" s="6" t="s">
         <v>647</v>
       </c>
@@ -8111,7 +8159,7 @@
       <c r="D93" s="2"/>
     </row>
     <row r="94" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A94" s="45"/>
+      <c r="A94" s="47"/>
       <c r="B94" s="6" t="s">
         <v>647</v>
       </c>
@@ -8121,7 +8169,7 @@
       <c r="D94" s="2"/>
     </row>
     <row r="95" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A95" s="45"/>
+      <c r="A95" s="47"/>
       <c r="B95" s="6" t="s">
         <v>647</v>
       </c>
@@ -8131,7 +8179,7 @@
       <c r="D95" s="2"/>
     </row>
     <row r="96" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A96" s="45"/>
+      <c r="A96" s="47"/>
       <c r="B96" s="6" t="s">
         <v>657</v>
       </c>
@@ -8141,7 +8189,7 @@
       <c r="D96" s="2"/>
     </row>
     <row r="97" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A97" s="45"/>
+      <c r="A97" s="47"/>
       <c r="B97" s="6" t="s">
         <v>657</v>
       </c>
@@ -8151,7 +8199,7 @@
       <c r="D97" s="2"/>
     </row>
     <row r="98" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A98" s="45"/>
+      <c r="A98" s="47"/>
       <c r="B98" s="14" t="s">
         <v>657</v>
       </c>
@@ -8161,7 +8209,7 @@
       <c r="D98" s="2"/>
     </row>
     <row r="99" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A99" s="45"/>
+      <c r="A99" s="47"/>
       <c r="B99" s="16" t="s">
         <v>661</v>
       </c>
@@ -8169,7 +8217,7 @@
       <c r="D99" s="2"/>
     </row>
     <row r="100" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A100" s="45"/>
+      <c r="A100" s="47"/>
       <c r="B100" s="9" t="s">
         <v>661</v>
       </c>
@@ -8177,7 +8225,7 @@
       <c r="D100" s="2"/>
     </row>
     <row r="101" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A101" s="45"/>
+      <c r="A101" s="47"/>
       <c r="B101" s="9" t="s">
         <v>661</v>
       </c>
@@ -8185,7 +8233,7 @@
       <c r="D101" s="2"/>
     </row>
     <row r="102" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A102" s="45"/>
+      <c r="A102" s="47"/>
       <c r="B102" s="9" t="s">
         <v>661</v>
       </c>
@@ -8193,7 +8241,7 @@
       <c r="D102" s="2"/>
     </row>
     <row r="103" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A103" s="49" t="s">
+      <c r="A103" s="51" t="s">
         <v>662</v>
       </c>
       <c r="B103" s="6" t="s">
@@ -8205,7 +8253,7 @@
       <c r="D103" s="2"/>
     </row>
     <row r="104" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A104" s="45"/>
+      <c r="A104" s="47"/>
       <c r="B104" s="6" t="s">
         <v>663</v>
       </c>
@@ -8215,7 +8263,7 @@
       <c r="D104" s="2"/>
     </row>
     <row r="105" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A105" s="45"/>
+      <c r="A105" s="47"/>
       <c r="B105" s="6" t="s">
         <v>663</v>
       </c>
@@ -13851,7 +13899,7 @@
       <c r="A2" s="2" t="s">
         <v>1086</v>
       </c>
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="56" t="s">
         <v>1087</v>
       </c>
     </row>
@@ -13859,31 +13907,31 @@
       <c r="A3" s="2" t="s">
         <v>1088</v>
       </c>
-      <c r="B3" s="45"/>
+      <c r="B3" s="47"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>1089</v>
       </c>
-      <c r="B4" s="45"/>
+      <c r="B4" s="47"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>1090</v>
       </c>
-      <c r="B5" s="45"/>
+      <c r="B5" s="47"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>1091</v>
       </c>
-      <c r="B6" s="45"/>
+      <c r="B6" s="47"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>1092</v>
       </c>
-      <c r="B7" s="54" t="s">
+      <c r="B7" s="56" t="s">
         <v>1093</v>
       </c>
     </row>
@@ -13891,19 +13939,19 @@
       <c r="A8" s="2" t="s">
         <v>1094</v>
       </c>
-      <c r="B8" s="45"/>
+      <c r="B8" s="47"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>1095</v>
       </c>
-      <c r="B9" s="45"/>
+      <c r="B9" s="47"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>1096</v>
       </c>
-      <c r="B10" s="54" t="s">
+      <c r="B10" s="56" t="s">
         <v>1097</v>
       </c>
     </row>
@@ -13911,25 +13959,25 @@
       <c r="A11" s="2" t="s">
         <v>1098</v>
       </c>
-      <c r="B11" s="45"/>
+      <c r="B11" s="47"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>1099</v>
       </c>
-      <c r="B12" s="45"/>
+      <c r="B12" s="47"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>1100</v>
       </c>
-      <c r="B13" s="45"/>
+      <c r="B13" s="47"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>1101</v>
       </c>
-      <c r="B14" s="54" t="s">
+      <c r="B14" s="56" t="s">
         <v>1102</v>
       </c>
     </row>
@@ -13937,61 +13985,61 @@
       <c r="A15" s="2" t="s">
         <v>1103</v>
       </c>
-      <c r="B15" s="45"/>
+      <c r="B15" s="47"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>1104</v>
       </c>
-      <c r="B16" s="45"/>
+      <c r="B16" s="47"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>1105</v>
       </c>
-      <c r="B17" s="45"/>
+      <c r="B17" s="47"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>1106</v>
       </c>
-      <c r="B18" s="45"/>
+      <c r="B18" s="47"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>1107</v>
       </c>
-      <c r="B19" s="45"/>
+      <c r="B19" s="47"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>1108</v>
       </c>
-      <c r="B20" s="45"/>
+      <c r="B20" s="47"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>1109</v>
       </c>
-      <c r="B21" s="45"/>
+      <c r="B21" s="47"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>1110</v>
       </c>
-      <c r="B22" s="45"/>
+      <c r="B22" s="47"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>1111</v>
       </c>
-      <c r="B23" s="45"/>
+      <c r="B23" s="47"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>1112</v>
       </c>
-      <c r="B24" s="55" t="s">
+      <c r="B24" s="57" t="s">
         <v>1113</v>
       </c>
     </row>
@@ -13999,7 +14047,7 @@
       <c r="A25" s="2" t="s">
         <v>1114</v>
       </c>
-      <c r="B25" s="45"/>
+      <c r="B25" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
Completed Recursion with ArrayList
</commit_message>
<xml_diff>
--- a/Level_1/First Job Program With Web Development.xlsx
+++ b/Level_1/First Job Program With Web Development.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\Nados\LearnDSA\Level_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ABB5B29-CF69-46C7-90F9-20573F4B496B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73076965-344E-49C9-ADA3-1E39F37D255C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1272" uniqueCount="1131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1282" uniqueCount="1131">
   <si>
     <t>Print Z</t>
   </si>
@@ -3816,24 +3816,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -4062,8 +4062,8 @@
   </sheetPr>
   <dimension ref="A1:D570"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="D133" sqref="D133"/>
+    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="C134" sqref="C134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4678,7 +4678,7 @@
         <v>1119</v>
       </c>
       <c r="C84" s="34">
-        <f ca="1">TODAY()-1</f>
+        <f>DATE(2022,2,6)+17</f>
         <v>44615</v>
       </c>
       <c r="D84" s="33" t="s">
@@ -4693,7 +4693,7 @@
         <v>1119</v>
       </c>
       <c r="C85" s="34">
-        <f t="shared" ref="C85:C89" ca="1" si="4">TODAY()-1</f>
+        <f t="shared" ref="C85:C89" si="4">DATE(2022,2,6)+17</f>
         <v>44615</v>
       </c>
       <c r="D85" s="33" t="s">
@@ -4708,7 +4708,7 @@
         <v>1119</v>
       </c>
       <c r="C86" s="34">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="4"/>
         <v>44615</v>
       </c>
       <c r="D86" s="33" t="s">
@@ -4723,7 +4723,7 @@
         <v>1119</v>
       </c>
       <c r="C87" s="34">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="4"/>
         <v>44615</v>
       </c>
       <c r="D87" s="33" t="s">
@@ -4738,7 +4738,7 @@
         <v>1119</v>
       </c>
       <c r="C88" s="34">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="4"/>
         <v>44615</v>
       </c>
       <c r="D88" s="33" t="s">
@@ -4753,7 +4753,7 @@
         <v>1119</v>
       </c>
       <c r="C89" s="34">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="4"/>
         <v>44615</v>
       </c>
       <c r="D89" s="33" t="s">
@@ -4774,7 +4774,7 @@
         <v>1119</v>
       </c>
       <c r="C91" s="34">
-        <f ca="1">TODAY()</f>
+        <f>DATE(2022,2,6)+18</f>
         <v>44616</v>
       </c>
       <c r="D91" s="33" t="s">
@@ -4789,7 +4789,7 @@
         <v>1119</v>
       </c>
       <c r="C92" s="34">
-        <f t="shared" ref="C92:C96" ca="1" si="5">TODAY()</f>
+        <f t="shared" ref="C92:C96" si="5">DATE(2022,2,6)+18</f>
         <v>44616</v>
       </c>
       <c r="D92" s="33" t="s">
@@ -4804,7 +4804,7 @@
         <v>1119</v>
       </c>
       <c r="C93" s="34">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>44616</v>
       </c>
       <c r="D93" s="33" t="s">
@@ -4819,7 +4819,7 @@
         <v>1119</v>
       </c>
       <c r="C94" s="34">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>44616</v>
       </c>
       <c r="D94" s="33" t="s">
@@ -4834,7 +4834,7 @@
         <v>1119</v>
       </c>
       <c r="C95" s="34">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>44616</v>
       </c>
       <c r="D95" s="33" t="s">
@@ -4849,89 +4849,139 @@
         <v>1119</v>
       </c>
       <c r="C96" s="34">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>44616</v>
       </c>
       <c r="D96" s="33" t="s">
         <v>1120</v>
       </c>
     </row>
-    <row r="97" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A97" s="44" t="s">
         <v>1125</v>
       </c>
     </row>
-    <row r="98" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="99" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B98" s="36" t="s">
+        <v>1119</v>
+      </c>
+      <c r="C98" s="34">
+        <f>DATE(2022,2,6)+25</f>
+        <v>44623</v>
+      </c>
+      <c r="D98" s="33" t="s">
+        <v>1120</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="100" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B99" s="36" t="s">
+        <v>1119</v>
+      </c>
+      <c r="C99" s="34">
+        <f t="shared" ref="C99:C102" si="6">DATE(2022,2,6)+25</f>
+        <v>44623</v>
+      </c>
+      <c r="D99" s="33" t="s">
+        <v>1120</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="101" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B100" s="36" t="s">
+        <v>1119</v>
+      </c>
+      <c r="C100" s="34">
+        <f t="shared" si="6"/>
+        <v>44623</v>
+      </c>
+      <c r="D100" s="33" t="s">
+        <v>1120</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="102" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A102" s="2" t="s">
+      <c r="B101" s="36" t="s">
+        <v>1119</v>
+      </c>
+      <c r="C101" s="34">
+        <f t="shared" si="6"/>
+        <v>44623</v>
+      </c>
+      <c r="D101" s="33" t="s">
+        <v>1120</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A102" s="42" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="103" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B102" s="36" t="s">
+        <v>1119</v>
+      </c>
+      <c r="C102" s="34">
+        <f>DATE(2022,2,6)+29</f>
+        <v>44627</v>
+      </c>
+      <c r="D102" s="33" t="s">
+        <v>1120</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A103" s="44" t="s">
         <v>1126</v>
       </c>
     </row>
-    <row r="104" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="105" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="106" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="107" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="108" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="109" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="110" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="111" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A111" s="44" t="s">
         <v>1127</v>
       </c>
     </row>
-    <row r="112" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
         <v>97</v>
       </c>
@@ -5049,8 +5099,8 @@
         <v>1119</v>
       </c>
       <c r="C133" s="34">
-        <f ca="1">TODAY()</f>
-        <v>44616</v>
+        <f>DATE(2022,2,6)+25</f>
+        <v>44623</v>
       </c>
       <c r="D133" s="33" t="s">
         <v>1120</v>
@@ -7251,7 +7301,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="53" t="s">
         <v>544</v>
       </c>
       <c r="B1" s="4" t="s">
@@ -7300,7 +7350,7 @@
       <c r="C5" s="7" t="s">
         <v>552</v>
       </c>
-      <c r="D5" s="46" t="s">
+      <c r="D5" s="48" t="s">
         <v>553</v>
       </c>
     </row>
@@ -7342,7 +7392,7 @@
       <c r="C9" s="7" t="s">
         <v>560</v>
       </c>
-      <c r="D9" s="46" t="s">
+      <c r="D9" s="48" t="s">
         <v>561</v>
       </c>
     </row>
@@ -7384,7 +7434,7 @@
       <c r="C13" s="7" t="s">
         <v>567</v>
       </c>
-      <c r="D13" s="46" t="s">
+      <c r="D13" s="48" t="s">
         <v>568</v>
       </c>
     </row>
@@ -7459,7 +7509,7 @@
       <c r="D20" s="10"/>
     </row>
     <row r="21" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A21" s="51" t="s">
+      <c r="A21" s="46" t="s">
         <v>577</v>
       </c>
       <c r="B21" s="6" t="s">
@@ -7506,7 +7556,7 @@
         <v>584</v>
       </c>
       <c r="C25" s="7"/>
-      <c r="D25" s="48" t="s">
+      <c r="D25" s="49" t="s">
         <v>585</v>
       </c>
     </row>
@@ -7518,7 +7568,7 @@
       <c r="C26" s="7" t="s">
         <v>586</v>
       </c>
-      <c r="D26" s="49"/>
+      <c r="D26" s="50"/>
     </row>
     <row r="27" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A27" s="47"/>
@@ -7528,7 +7578,7 @@
       <c r="C27" s="7" t="s">
         <v>587</v>
       </c>
-      <c r="D27" s="50"/>
+      <c r="D27" s="51"/>
     </row>
     <row r="28" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A28" s="47"/>
@@ -7548,7 +7598,7 @@
       <c r="C29" s="7" t="s">
         <v>590</v>
       </c>
-      <c r="D29" s="46" t="s">
+      <c r="D29" s="48" t="s">
         <v>591</v>
       </c>
     </row>
@@ -7600,7 +7650,7 @@
       <c r="C34" s="7" t="s">
         <v>599</v>
       </c>
-      <c r="D34" s="48" t="s">
+      <c r="D34" s="49" t="s">
         <v>600</v>
       </c>
     </row>
@@ -7612,7 +7662,7 @@
       <c r="C35" s="7" t="s">
         <v>601</v>
       </c>
-      <c r="D35" s="49"/>
+      <c r="D35" s="50"/>
     </row>
     <row r="36" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A36" s="47"/>
@@ -7622,7 +7672,7 @@
       <c r="C36" s="7" t="s">
         <v>602</v>
       </c>
-      <c r="D36" s="50"/>
+      <c r="D36" s="51"/>
     </row>
     <row r="37" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A37" s="47"/>
@@ -7655,7 +7705,7 @@
       <c r="D39" s="2"/>
     </row>
     <row r="40" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A40" s="52" t="s">
+      <c r="A40" s="54" t="s">
         <v>607</v>
       </c>
       <c r="B40" s="6" t="s">
@@ -7692,7 +7742,7 @@
         <v>612</v>
       </c>
       <c r="C43" s="7"/>
-      <c r="D43" s="46" t="s">
+      <c r="D43" s="48" t="s">
         <v>613</v>
       </c>
     </row>
@@ -7764,7 +7814,7 @@
         <v>619</v>
       </c>
       <c r="C51" s="7"/>
-      <c r="D51" s="48" t="s">
+      <c r="D51" s="49" t="s">
         <v>620</v>
       </c>
     </row>
@@ -7774,7 +7824,7 @@
         <v>619</v>
       </c>
       <c r="C52" s="7"/>
-      <c r="D52" s="49"/>
+      <c r="D52" s="50"/>
     </row>
     <row r="53" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A53" s="47"/>
@@ -7782,7 +7832,7 @@
         <v>619</v>
       </c>
       <c r="C53" s="7"/>
-      <c r="D53" s="49"/>
+      <c r="D53" s="50"/>
     </row>
     <row r="54" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A54" s="47"/>
@@ -7790,7 +7840,7 @@
         <v>619</v>
       </c>
       <c r="C54" s="7"/>
-      <c r="D54" s="49"/>
+      <c r="D54" s="50"/>
     </row>
     <row r="55" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A55" s="47"/>
@@ -7798,7 +7848,7 @@
         <v>619</v>
       </c>
       <c r="C55" s="7"/>
-      <c r="D55" s="49"/>
+      <c r="D55" s="50"/>
     </row>
     <row r="56" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A56" s="47"/>
@@ -7806,7 +7856,7 @@
         <v>619</v>
       </c>
       <c r="C56" s="7"/>
-      <c r="D56" s="50"/>
+      <c r="D56" s="51"/>
     </row>
     <row r="57" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A57" s="47"/>
@@ -7846,7 +7896,7 @@
         <v>626</v>
       </c>
       <c r="C60" s="7"/>
-      <c r="D60" s="46" t="s">
+      <c r="D60" s="48" t="s">
         <v>627</v>
       </c>
     </row>
@@ -7875,7 +7925,7 @@
       <c r="D63" s="8"/>
     </row>
     <row r="64" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A64" s="53" t="s">
+      <c r="A64" s="55" t="s">
         <v>628</v>
       </c>
       <c r="B64" s="9" t="s">
@@ -7965,7 +8015,7 @@
       <c r="D74" s="2"/>
     </row>
     <row r="75" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A75" s="55" t="s">
+      <c r="A75" s="52" t="s">
         <v>632</v>
       </c>
       <c r="B75" s="6" t="s">
@@ -7974,7 +8024,7 @@
       <c r="C75" s="7" t="s">
         <v>634</v>
       </c>
-      <c r="D75" s="46" t="s">
+      <c r="D75" s="48" t="s">
         <v>635</v>
       </c>
     </row>
@@ -8241,7 +8291,7 @@
       <c r="D102" s="2"/>
     </row>
     <row r="103" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A103" s="51" t="s">
+      <c r="A103" s="46" t="s">
         <v>662</v>
       </c>
       <c r="B103" s="6" t="s">
@@ -10959,22 +11009,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="D29:D31"/>
+    <mergeCell ref="D34:D36"/>
+    <mergeCell ref="A21:A39"/>
+    <mergeCell ref="A40:A63"/>
+    <mergeCell ref="A64:A74"/>
+    <mergeCell ref="A1:A20"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="D13:D15"/>
+    <mergeCell ref="D25:D27"/>
     <mergeCell ref="A103:A105"/>
     <mergeCell ref="D43:D47"/>
     <mergeCell ref="D51:D56"/>
     <mergeCell ref="D60:D62"/>
     <mergeCell ref="D75:D77"/>
     <mergeCell ref="A75:A102"/>
-    <mergeCell ref="A1:A20"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="D9:D11"/>
-    <mergeCell ref="D13:D15"/>
-    <mergeCell ref="D25:D27"/>
-    <mergeCell ref="D29:D31"/>
-    <mergeCell ref="D34:D36"/>
-    <mergeCell ref="A21:A39"/>
-    <mergeCell ref="A40:A63"/>
-    <mergeCell ref="A64:A74"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
completed Recursion on the way up
</commit_message>
<xml_diff>
--- a/Level_1/First Job Program With Web Development.xlsx
+++ b/Level_1/First Job Program With Web Development.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\Nados\LearnDSA\Level_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73076965-344E-49C9-ADA3-1E39F37D255C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24CFEA99-9ACB-4C4C-81D3-A1AA7536ABE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1282" uniqueCount="1131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1317" uniqueCount="1143">
   <si>
     <t>Print Z</t>
   </si>
@@ -3447,6 +3447,42 @@
   </si>
   <si>
     <t>1.2 Patterns</t>
+  </si>
+  <si>
+    <t>4. Basic Data Structures</t>
+  </si>
+  <si>
+    <t>4.1 Stacks and Queues</t>
+  </si>
+  <si>
+    <t>4.2 Linked List</t>
+  </si>
+  <si>
+    <t>4.3 Generic Tree</t>
+  </si>
+  <si>
+    <t>4.4 Binary Tree</t>
+  </si>
+  <si>
+    <t>4.5 Binary Search Tree</t>
+  </si>
+  <si>
+    <t>5. Advance Data Structures</t>
+  </si>
+  <si>
+    <t>6. Dynamic Programming</t>
+  </si>
+  <si>
+    <t>5.1 AVL Tree</t>
+  </si>
+  <si>
+    <t>5.2 Hashmap</t>
+  </si>
+  <si>
+    <t>5.3 Heap</t>
+  </si>
+  <si>
+    <t>5.4 Graphs</t>
   </si>
 </sst>
 </file>
@@ -3573,7 +3609,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="19">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3682,6 +3718,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -3747,7 +3789,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -3797,7 +3839,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -3816,6 +3857,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3842,6 +3884,8 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4060,10 +4104,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D570"/>
+  <dimension ref="A1:D581"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="C134" sqref="C134"/>
+    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="A300" sqref="A300"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4073,29 +4117,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="26" customFormat="1" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="30" t="s">
         <v>1115</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="30" t="s">
         <v>1116</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="30" t="s">
         <v>1117</v>
       </c>
-      <c r="D1" s="31" t="s">
+      <c r="D1" s="30" t="s">
         <v>1118</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="38" customFormat="1" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="31" t="s">
+    <row r="2" spans="1:4" s="37" customFormat="1" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="30" t="s">
         <v>1121</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-    </row>
-    <row r="3" spans="1:4" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="32" t="s">
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+    </row>
+    <row r="3" spans="1:4" s="27" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="31" t="s">
         <v>1129</v>
       </c>
     </row>
@@ -4103,14 +4147,14 @@
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="34" t="s">
         <v>1119</v>
       </c>
-      <c r="C4" s="34">
+      <c r="C4" s="33">
         <f>DATE(2022,2,6)</f>
         <v>44598</v>
       </c>
-      <c r="D4" s="33" t="s">
+      <c r="D4" s="32" t="s">
         <v>1120</v>
       </c>
     </row>
@@ -4118,14 +4162,14 @@
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="34" t="s">
         <v>1119</v>
       </c>
-      <c r="C5" s="34">
+      <c r="C5" s="33">
         <f t="shared" ref="C5:C6" si="0">DATE(2022,2,6)</f>
         <v>44598</v>
       </c>
-      <c r="D5" s="33" t="s">
+      <c r="D5" s="32" t="s">
         <v>1120</v>
       </c>
     </row>
@@ -4133,14 +4177,14 @@
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="34" t="s">
         <v>1119</v>
       </c>
-      <c r="C6" s="34">
+      <c r="C6" s="33">
         <f t="shared" si="0"/>
         <v>44598</v>
       </c>
-      <c r="D6" s="33" t="s">
+      <c r="D6" s="32" t="s">
         <v>1120</v>
       </c>
     </row>
@@ -4148,14 +4192,14 @@
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="36" t="s">
+      <c r="B7" s="35" t="s">
         <v>1119</v>
       </c>
-      <c r="C7" s="34">
+      <c r="C7" s="33">
         <f>DATE(2022,2,6)+1</f>
         <v>44599</v>
       </c>
-      <c r="D7" s="33" t="s">
+      <c r="D7" s="32" t="s">
         <v>1120</v>
       </c>
     </row>
@@ -4163,14 +4207,14 @@
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="36" t="s">
         <v>1119</v>
       </c>
-      <c r="C8" s="34">
+      <c r="C8" s="33">
         <f>DATE(2022,2,6)+1</f>
         <v>44599</v>
       </c>
-      <c r="D8" s="33" t="s">
+      <c r="D8" s="32" t="s">
         <v>1120</v>
       </c>
     </row>
@@ -4178,14 +4222,14 @@
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="35" t="s">
+      <c r="B9" s="34" t="s">
         <v>1119</v>
       </c>
-      <c r="C9" s="34">
+      <c r="C9" s="33">
         <f t="shared" ref="C9:C12" si="1">DATE(2022,2,6)+1</f>
         <v>44599</v>
       </c>
-      <c r="D9" s="33" t="s">
+      <c r="D9" s="32" t="s">
         <v>1120</v>
       </c>
     </row>
@@ -4193,14 +4237,14 @@
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="36" t="s">
+      <c r="B10" s="35" t="s">
         <v>1119</v>
       </c>
-      <c r="C10" s="34">
+      <c r="C10" s="33">
         <f t="shared" si="1"/>
         <v>44599</v>
       </c>
-      <c r="D10" s="33" t="s">
+      <c r="D10" s="32" t="s">
         <v>1120</v>
       </c>
     </row>
@@ -4208,14 +4252,14 @@
       <c r="A11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="35" t="s">
+      <c r="B11" s="34" t="s">
         <v>1119</v>
       </c>
-      <c r="C11" s="34">
+      <c r="C11" s="33">
         <f t="shared" si="1"/>
         <v>44599</v>
       </c>
-      <c r="D11" s="33" t="s">
+      <c r="D11" s="32" t="s">
         <v>1120</v>
       </c>
     </row>
@@ -4223,14 +4267,14 @@
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="35" t="s">
+      <c r="B12" s="34" t="s">
         <v>1119</v>
       </c>
-      <c r="C12" s="34">
+      <c r="C12" s="33">
         <f t="shared" si="1"/>
         <v>44599</v>
       </c>
-      <c r="D12" s="33" t="s">
+      <c r="D12" s="32" t="s">
         <v>1120</v>
       </c>
     </row>
@@ -4238,14 +4282,14 @@
       <c r="A13" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="36" t="s">
+      <c r="B13" s="35" t="s">
         <v>1119</v>
       </c>
-      <c r="C13" s="34">
+      <c r="C13" s="33">
         <f>DATE(2022,2,6)+1</f>
         <v>44599</v>
       </c>
-      <c r="D13" s="33" t="s">
+      <c r="D13" s="32" t="s">
         <v>1120</v>
       </c>
     </row>
@@ -4253,14 +4297,14 @@
       <c r="A14" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="36" t="s">
+      <c r="B14" s="35" t="s">
         <v>1119</v>
       </c>
-      <c r="C14" s="34">
+      <c r="C14" s="33">
         <f>DATE(2022,2,6)+2</f>
         <v>44600</v>
       </c>
-      <c r="D14" s="33" t="s">
+      <c r="D14" s="32" t="s">
         <v>1120</v>
       </c>
     </row>
@@ -4268,14 +4312,14 @@
       <c r="A15" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="35" t="s">
+      <c r="B15" s="34" t="s">
         <v>1119</v>
       </c>
-      <c r="C15" s="34">
+      <c r="C15" s="33">
         <f>DATE(2022,2,6)+2</f>
         <v>44600</v>
       </c>
-      <c r="D15" s="33" t="s">
+      <c r="D15" s="32" t="s">
         <v>1120</v>
       </c>
     </row>
@@ -4283,14 +4327,14 @@
       <c r="A16" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="36" t="s">
+      <c r="B16" s="35" t="s">
         <v>1119</v>
       </c>
-      <c r="C16" s="34">
+      <c r="C16" s="33">
         <f>DATE(2022,2,6)+3</f>
         <v>44601</v>
       </c>
-      <c r="D16" s="33" t="s">
+      <c r="D16" s="32" t="s">
         <v>1120</v>
       </c>
     </row>
@@ -4298,34 +4342,34 @@
       <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="35" t="s">
+      <c r="B17" s="34" t="s">
         <v>1119</v>
       </c>
-      <c r="C17" s="34">
+      <c r="C17" s="33">
         <f t="shared" ref="C17:C18" si="2">DATE(2022,2,6)+3</f>
         <v>44601</v>
       </c>
-      <c r="D17" s="33" t="s">
+      <c r="D17" s="32" t="s">
         <v>1120</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A18" s="42" t="s">
+      <c r="A18" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="35" t="s">
+      <c r="B18" s="34" t="s">
         <v>1119</v>
       </c>
-      <c r="C18" s="34">
+      <c r="C18" s="33">
         <f t="shared" si="2"/>
         <v>44601</v>
       </c>
-      <c r="D18" s="33" t="s">
+      <c r="D18" s="32" t="s">
         <v>1120</v>
       </c>
     </row>
-    <row r="19" spans="1:4" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A19" s="45" t="s">
+    <row r="19" spans="1:4" s="27" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A19" s="44" t="s">
         <v>1130</v>
       </c>
     </row>
@@ -4623,35 +4667,35 @@
         <v>71</v>
       </c>
     </row>
-    <row r="80" spans="1:1" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A80" s="27"/>
-    </row>
-    <row r="81" spans="1:4" s="39" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="40" t="s">
+    <row r="80" spans="1:1" s="59" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A80" s="58"/>
+    </row>
+    <row r="81" spans="1:4" s="38" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="39" t="s">
         <v>1122</v>
       </c>
-      <c r="B81" s="31" t="s">
+      <c r="B81" s="30" t="s">
         <v>1116</v>
       </c>
-      <c r="C81" s="31" t="s">
+      <c r="C81" s="30" t="s">
         <v>1117</v>
       </c>
-      <c r="D81" s="31" t="s">
+      <c r="D81" s="30" t="s">
         <v>1118</v>
       </c>
     </row>
-    <row r="82" spans="1:4" s="39" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="41" t="s">
+    <row r="82" spans="1:4" s="38" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="40" t="s">
         <v>1123</v>
       </c>
-      <c r="B82" s="35" t="s">
+      <c r="B82" s="34" t="s">
         <v>1119</v>
       </c>
-      <c r="C82" s="34">
+      <c r="C82" s="33">
         <f t="shared" ref="C82:C83" si="3">DATE(2022,2,6)+3</f>
         <v>44601</v>
       </c>
-      <c r="D82" s="33" t="s">
+      <c r="D82" s="32" t="s">
         <v>1120</v>
       </c>
     </row>
@@ -4659,14 +4703,14 @@
       <c r="A83" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B83" s="35" t="s">
+      <c r="B83" s="34" t="s">
         <v>1119</v>
       </c>
-      <c r="C83" s="34">
+      <c r="C83" s="33">
         <f t="shared" si="3"/>
         <v>44601</v>
       </c>
-      <c r="D83" s="33" t="s">
+      <c r="D83" s="32" t="s">
         <v>1120</v>
       </c>
     </row>
@@ -4674,14 +4718,14 @@
       <c r="A84" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B84" s="35" t="s">
+      <c r="B84" s="34" t="s">
         <v>1119</v>
       </c>
-      <c r="C84" s="34">
+      <c r="C84" s="33">
         <f>DATE(2022,2,6)+17</f>
         <v>44615</v>
       </c>
-      <c r="D84" s="33" t="s">
+      <c r="D84" s="32" t="s">
         <v>1120</v>
       </c>
     </row>
@@ -4689,14 +4733,14 @@
       <c r="A85" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B85" s="35" t="s">
+      <c r="B85" s="34" t="s">
         <v>1119</v>
       </c>
-      <c r="C85" s="34">
+      <c r="C85" s="33">
         <f t="shared" ref="C85:C89" si="4">DATE(2022,2,6)+17</f>
         <v>44615</v>
       </c>
-      <c r="D85" s="33" t="s">
+      <c r="D85" s="32" t="s">
         <v>1120</v>
       </c>
     </row>
@@ -4704,14 +4748,14 @@
       <c r="A86" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B86" s="35" t="s">
+      <c r="B86" s="34" t="s">
         <v>1119</v>
       </c>
-      <c r="C86" s="34">
+      <c r="C86" s="33">
         <f t="shared" si="4"/>
         <v>44615</v>
       </c>
-      <c r="D86" s="33" t="s">
+      <c r="D86" s="32" t="s">
         <v>1120</v>
       </c>
     </row>
@@ -4719,14 +4763,14 @@
       <c r="A87" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B87" s="35" t="s">
+      <c r="B87" s="34" t="s">
         <v>1119</v>
       </c>
-      <c r="C87" s="34">
+      <c r="C87" s="33">
         <f t="shared" si="4"/>
         <v>44615</v>
       </c>
-      <c r="D87" s="33" t="s">
+      <c r="D87" s="32" t="s">
         <v>1120</v>
       </c>
     </row>
@@ -4734,50 +4778,50 @@
       <c r="A88" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B88" s="35" t="s">
+      <c r="B88" s="34" t="s">
         <v>1119</v>
       </c>
-      <c r="C88" s="34">
+      <c r="C88" s="33">
         <f t="shared" si="4"/>
         <v>44615</v>
       </c>
-      <c r="D88" s="33" t="s">
+      <c r="D88" s="32" t="s">
         <v>1120</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A89" s="43" t="s">
+      <c r="A89" s="42" t="s">
         <v>78</v>
       </c>
-      <c r="B89" s="36" t="s">
+      <c r="B89" s="35" t="s">
         <v>1119</v>
       </c>
-      <c r="C89" s="34">
+      <c r="C89" s="33">
         <f t="shared" si="4"/>
         <v>44615</v>
       </c>
-      <c r="D89" s="33" t="s">
+      <c r="D89" s="32" t="s">
         <v>1120</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A90" s="44" t="s">
+      <c r="A90" s="43" t="s">
         <v>1124</v>
       </c>
-      <c r="C90" s="34"/>
+      <c r="C90" s="33"/>
     </row>
     <row r="91" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B91" s="35" t="s">
+      <c r="B91" s="34" t="s">
         <v>1119</v>
       </c>
-      <c r="C91" s="34">
+      <c r="C91" s="33">
         <f>DATE(2022,2,6)+18</f>
         <v>44616</v>
       </c>
-      <c r="D91" s="33" t="s">
+      <c r="D91" s="32" t="s">
         <v>1120</v>
       </c>
     </row>
@@ -4785,29 +4829,29 @@
       <c r="A92" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B92" s="35" t="s">
+      <c r="B92" s="34" t="s">
         <v>1119</v>
       </c>
-      <c r="C92" s="34">
+      <c r="C92" s="33">
         <f t="shared" ref="C92:C96" si="5">DATE(2022,2,6)+18</f>
         <v>44616</v>
       </c>
-      <c r="D92" s="33" t="s">
+      <c r="D92" s="32" t="s">
         <v>1120</v>
       </c>
     </row>
     <row r="93" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A93" s="43" t="s">
+      <c r="A93" s="42" t="s">
         <v>81</v>
       </c>
-      <c r="B93" s="36" t="s">
+      <c r="B93" s="35" t="s">
         <v>1119</v>
       </c>
-      <c r="C93" s="34">
+      <c r="C93" s="33">
         <f t="shared" si="5"/>
         <v>44616</v>
       </c>
-      <c r="D93" s="33" t="s">
+      <c r="D93" s="32" t="s">
         <v>1120</v>
       </c>
     </row>
@@ -4815,14 +4859,14 @@
       <c r="A94" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B94" s="35" t="s">
+      <c r="B94" s="34" t="s">
         <v>1119</v>
       </c>
-      <c r="C94" s="34">
+      <c r="C94" s="33">
         <f t="shared" si="5"/>
         <v>44616</v>
       </c>
-      <c r="D94" s="33" t="s">
+      <c r="D94" s="32" t="s">
         <v>1120</v>
       </c>
     </row>
@@ -4830,34 +4874,34 @@
       <c r="A95" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B95" s="35" t="s">
+      <c r="B95" s="34" t="s">
         <v>1119</v>
       </c>
-      <c r="C95" s="34">
+      <c r="C95" s="33">
         <f t="shared" si="5"/>
         <v>44616</v>
       </c>
-      <c r="D95" s="33" t="s">
+      <c r="D95" s="32" t="s">
         <v>1120</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A96" s="42" t="s">
+      <c r="A96" s="41" t="s">
         <v>84</v>
       </c>
-      <c r="B96" s="36" t="s">
+      <c r="B96" s="35" t="s">
         <v>1119</v>
       </c>
-      <c r="C96" s="34">
+      <c r="C96" s="33">
         <f t="shared" si="5"/>
         <v>44616</v>
       </c>
-      <c r="D96" s="33" t="s">
+      <c r="D96" s="32" t="s">
         <v>1120</v>
       </c>
     </row>
     <row r="97" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A97" s="44" t="s">
+      <c r="A97" s="43" t="s">
         <v>1125</v>
       </c>
     </row>
@@ -4865,14 +4909,14 @@
       <c r="A98" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B98" s="36" t="s">
+      <c r="B98" s="35" t="s">
         <v>1119</v>
       </c>
-      <c r="C98" s="34">
+      <c r="C98" s="33">
         <f>DATE(2022,2,6)+25</f>
         <v>44623</v>
       </c>
-      <c r="D98" s="33" t="s">
+      <c r="D98" s="32" t="s">
         <v>1120</v>
       </c>
     </row>
@@ -4880,14 +4924,14 @@
       <c r="A99" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B99" s="36" t="s">
+      <c r="B99" s="35" t="s">
         <v>1119</v>
       </c>
-      <c r="C99" s="34">
-        <f t="shared" ref="C99:C102" si="6">DATE(2022,2,6)+25</f>
+      <c r="C99" s="33">
+        <f t="shared" ref="C99:C101" si="6">DATE(2022,2,6)+25</f>
         <v>44623</v>
       </c>
-      <c r="D99" s="33" t="s">
+      <c r="D99" s="32" t="s">
         <v>1120</v>
       </c>
     </row>
@@ -4895,14 +4939,14 @@
       <c r="A100" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B100" s="36" t="s">
+      <c r="B100" s="35" t="s">
         <v>1119</v>
       </c>
-      <c r="C100" s="34">
+      <c r="C100" s="33">
         <f t="shared" si="6"/>
         <v>44623</v>
       </c>
-      <c r="D100" s="33" t="s">
+      <c r="D100" s="32" t="s">
         <v>1120</v>
       </c>
     </row>
@@ -4910,34 +4954,34 @@
       <c r="A101" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B101" s="36" t="s">
+      <c r="B101" s="35" t="s">
         <v>1119</v>
       </c>
-      <c r="C101" s="34">
+      <c r="C101" s="33">
         <f t="shared" si="6"/>
         <v>44623</v>
       </c>
-      <c r="D101" s="33" t="s">
+      <c r="D101" s="32" t="s">
         <v>1120</v>
       </c>
     </row>
     <row r="102" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A102" s="42" t="s">
+      <c r="A102" s="41" t="s">
         <v>89</v>
       </c>
-      <c r="B102" s="36" t="s">
+      <c r="B102" s="35" t="s">
         <v>1119</v>
       </c>
-      <c r="C102" s="34">
+      <c r="C102" s="33">
         <f>DATE(2022,2,6)+29</f>
         <v>44627</v>
       </c>
-      <c r="D102" s="33" t="s">
+      <c r="D102" s="32" t="s">
         <v>1120</v>
       </c>
     </row>
     <row r="103" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A103" s="44" t="s">
+      <c r="A103" s="43" t="s">
         <v>1126</v>
       </c>
     </row>
@@ -4945,39 +4989,109 @@
       <c r="A104" s="2" t="s">
         <v>90</v>
       </c>
+      <c r="B104" s="35" t="s">
+        <v>1119</v>
+      </c>
+      <c r="C104" s="33">
+        <f>DATE(2022,2,6)+29</f>
+        <v>44627</v>
+      </c>
+      <c r="D104" s="32" t="s">
+        <v>1120</v>
+      </c>
     </row>
     <row r="105" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
         <v>91</v>
       </c>
+      <c r="B105" s="35" t="s">
+        <v>1119</v>
+      </c>
+      <c r="C105" s="33">
+        <f t="shared" ref="C105:C110" si="7">DATE(2022,2,6)+29</f>
+        <v>44627</v>
+      </c>
+      <c r="D105" s="32" t="s">
+        <v>1120</v>
+      </c>
     </row>
     <row r="106" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>92</v>
       </c>
+      <c r="B106" s="35" t="s">
+        <v>1119</v>
+      </c>
+      <c r="C106" s="33">
+        <f t="shared" si="7"/>
+        <v>44627</v>
+      </c>
+      <c r="D106" s="32" t="s">
+        <v>1120</v>
+      </c>
     </row>
     <row r="107" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>93</v>
       </c>
+      <c r="B107" s="35" t="s">
+        <v>1119</v>
+      </c>
+      <c r="C107" s="33">
+        <f t="shared" si="7"/>
+        <v>44627</v>
+      </c>
+      <c r="D107" s="32" t="s">
+        <v>1120</v>
+      </c>
     </row>
     <row r="108" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A108" s="2" t="s">
+      <c r="A108" s="41" t="s">
         <v>94</v>
       </c>
+      <c r="B108" s="35" t="s">
+        <v>1119</v>
+      </c>
+      <c r="C108" s="33">
+        <f t="shared" si="7"/>
+        <v>44627</v>
+      </c>
+      <c r="D108" s="32" t="s">
+        <v>1120</v>
+      </c>
     </row>
     <row r="109" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A109" s="2" t="s">
+      <c r="A109" s="41" t="s">
         <v>95</v>
       </c>
+      <c r="B109" s="35" t="s">
+        <v>1119</v>
+      </c>
+      <c r="C109" s="33">
+        <f t="shared" si="7"/>
+        <v>44627</v>
+      </c>
+      <c r="D109" s="32" t="s">
+        <v>1120</v>
+      </c>
     </row>
     <row r="110" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A110" s="2" t="s">
+      <c r="A110" s="41" t="s">
         <v>96</v>
       </c>
+      <c r="B110" s="35" t="s">
+        <v>1119</v>
+      </c>
+      <c r="C110" s="33">
+        <f t="shared" si="7"/>
+        <v>44627</v>
+      </c>
+      <c r="D110" s="32" t="s">
+        <v>1120</v>
+      </c>
     </row>
     <row r="111" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A111" s="44" t="s">
+      <c r="A111" s="43" t="s">
         <v>1127</v>
       </c>
     </row>
@@ -5001,20 +5115,20 @@
         <v>100</v>
       </c>
     </row>
-    <row r="116" spans="1:4" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A116" s="27"/>
-    </row>
-    <row r="117" spans="1:4" s="39" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A117" s="40" t="s">
+    <row r="116" spans="1:4" s="59" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A116" s="58"/>
+    </row>
+    <row r="117" spans="1:4" s="38" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A117" s="39" t="s">
         <v>1128</v>
       </c>
-      <c r="B117" s="31" t="s">
+      <c r="B117" s="30" t="s">
         <v>1116</v>
       </c>
-      <c r="C117" s="31" t="s">
+      <c r="C117" s="30" t="s">
         <v>1117</v>
       </c>
-      <c r="D117" s="31" t="s">
+      <c r="D117" s="30" t="s">
         <v>1118</v>
       </c>
     </row>
@@ -5088,2190 +5202,2280 @@
         <v>114</v>
       </c>
     </row>
-    <row r="132" spans="1:4" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A132" s="27"/>
-    </row>
-    <row r="133" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A133" s="2" t="s">
+    <row r="132" spans="1:4" s="59" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A132" s="58"/>
+    </row>
+    <row r="133" spans="1:4" s="38" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A133" s="39" t="s">
+        <v>1131</v>
+      </c>
+      <c r="B133" s="30" t="s">
+        <v>1116</v>
+      </c>
+      <c r="C133" s="30" t="s">
+        <v>1117</v>
+      </c>
+      <c r="D133" s="30" t="s">
+        <v>1118</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" s="38" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A134" s="43" t="s">
+        <v>1132</v>
+      </c>
+      <c r="B134" s="30"/>
+      <c r="C134" s="30"/>
+      <c r="D134" s="30"/>
+    </row>
+    <row r="135" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A135" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="B133" s="35" t="s">
+      <c r="B135" s="34" t="s">
         <v>1119</v>
       </c>
-      <c r="C133" s="34">
+      <c r="C135" s="33">
         <f>DATE(2022,2,6)+25</f>
         <v>44623</v>
       </c>
-      <c r="D133" s="33" t="s">
+      <c r="D135" s="32" t="s">
         <v>1120</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A134" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="135" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A135" s="2" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="136" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="137" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="138" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="139" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="140" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="141" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="142" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="143" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="144" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="145" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="146" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="147" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="148" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="149" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="150" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="151" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="152" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="153" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="154" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A154" s="2"/>
+      <c r="A154" s="2" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="155" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="156" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A156" s="2" t="s">
-        <v>137</v>
+      <c r="A156" s="43" t="s">
+        <v>1133</v>
       </c>
     </row>
     <row r="157" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="158" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="159" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="160" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="161" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="162" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="163" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="164" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="165" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="166" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="167" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="168" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="169" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="170" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="171" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="172" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="173" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A173" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="174" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A174" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="175" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="176" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A176" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="177" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A177" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="178" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A178" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="179" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="180" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="181" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="182" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="183" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="184" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="185" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A185" s="2"/>
+      <c r="A185" s="2" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="186" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A186" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="187" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A187" s="2" t="s">
-        <v>167</v>
+      <c r="A187" s="43" t="s">
+        <v>1134</v>
       </c>
     </row>
     <row r="188" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A188" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="189" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A189" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="190" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A190" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="191" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A191" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="192" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A192" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="193" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A193" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="194" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A194" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="195" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A195" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="196" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A196" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="197" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A197" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="198" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A198" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="199" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A199" s="2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="200" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A200" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="201" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A201" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="202" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A202" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="203" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A203" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="204" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A204" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="205" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A205" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="206" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="207" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="208" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A208" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="209" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A209" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="210" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A210" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="211" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A211" s="2"/>
+      <c r="A211" s="2" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="212" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A212" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="213" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A213" s="2" t="s">
-        <v>191</v>
+      <c r="A213" s="43" t="s">
+        <v>1135</v>
       </c>
     </row>
     <row r="214" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A214" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="215" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A215" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="216" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A216" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="217" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A217" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="218" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A218" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="219" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A219" s="2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="220" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A220" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="221" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A221" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="222" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A222" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="223" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A223" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="224" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A224" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="225" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A225" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="226" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A226" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="227" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A227" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="228" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A228" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="229" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A229" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="230" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A230" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="231" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A231" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="232" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A232" s="2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="233" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A233" s="2" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="234" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A234" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="235" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A235" s="2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="236" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A236" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="237" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A237" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="238" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A238" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="239" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A239" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="240" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A240" s="2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="241" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A241" s="2" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="242" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A242" s="2" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="243" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A243" s="2"/>
+      <c r="A243" s="2" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="244" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A244" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="245" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A245" s="2" t="s">
-        <v>222</v>
+      <c r="A245" s="43" t="s">
+        <v>1136</v>
       </c>
     </row>
     <row r="246" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A246" s="2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="247" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A247" s="2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="248" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A248" s="2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="249" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A249" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="250" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A250" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="251" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A251" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="252" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A252" s="2" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="253" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A253" s="2" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="254" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A254" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="255" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A255" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="256" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A256" s="2" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="257" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A257" s="2" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="258" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A258" s="2" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="257" spans="1:1" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A257" s="27"/>
-    </row>
-    <row r="258" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A258" s="2" t="s">
+    <row r="259" spans="1:4" s="59" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A259" s="58"/>
+    </row>
+    <row r="260" spans="1:4" s="38" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A260" s="39" t="s">
+        <v>1137</v>
+      </c>
+      <c r="B260" s="30" t="s">
+        <v>1116</v>
+      </c>
+      <c r="C260" s="30" t="s">
+        <v>1117</v>
+      </c>
+      <c r="D260" s="30" t="s">
+        <v>1118</v>
+      </c>
+    </row>
+    <row r="261" spans="1:4" s="38" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A261" s="43" t="s">
+        <v>1139</v>
+      </c>
+      <c r="B261" s="30"/>
+      <c r="C261" s="30"/>
+      <c r="D261" s="30"/>
+    </row>
+    <row r="262" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A262" s="2" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="259" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A259" s="2" t="s">
+    <row r="263" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A263" s="2" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="260" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A260" s="2" t="s">
+    <row r="264" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A264" s="2" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="261" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A261" s="2" t="s">
+    <row r="265" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A265" s="2" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="262" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A262" s="2"/>
-    </row>
-    <row r="263" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A263" s="2" t="s">
+    <row r="266" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A266" s="43" t="s">
+        <v>1140</v>
+      </c>
+    </row>
+    <row r="267" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A267" s="2" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="264" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A264" s="2" t="s">
+    <row r="268" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A268" s="2" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="265" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A265" s="2" t="s">
+    <row r="269" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A269" s="2" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="266" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A266" s="2" t="s">
+    <row r="270" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A270" s="2" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="267" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A267" s="2" t="s">
+    <row r="271" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A271" s="2" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="268" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A268" s="2"/>
-    </row>
-    <row r="269" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A269" s="2" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="270" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A270" s="2" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="271" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A271" s="2" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="272" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A272" s="2" t="s">
-        <v>246</v>
+    <row r="272" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A272" s="43" t="s">
+        <v>1141</v>
       </c>
     </row>
     <row r="273" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A273" s="2" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="274" spans="1:1" s="30" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A274" s="29"/>
+        <v>243</v>
+      </c>
+    </row>
+    <row r="274" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A274" s="2" t="s">
+        <v>244</v>
+      </c>
     </row>
     <row r="275" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A275" s="2" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="276" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A276" s="2" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="277" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A277" s="2" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="278" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A278" s="2" t="s">
-        <v>251</v>
+        <v>247</v>
+      </c>
+    </row>
+    <row r="278" spans="1:1" s="45" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A278" s="43" t="s">
+        <v>1142</v>
       </c>
     </row>
     <row r="279" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A279" s="2" t="s">
-        <v>252</v>
+        <v>304</v>
       </c>
     </row>
     <row r="280" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A280" s="2" t="s">
-        <v>253</v>
+        <v>305</v>
       </c>
     </row>
     <row r="281" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A281" s="3" t="s">
-        <v>254</v>
+      <c r="A281" s="2" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="282" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A282" s="3" t="s">
-        <v>255</v>
+      <c r="A282" s="2" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="283" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A283" s="3" t="s">
-        <v>256</v>
+      <c r="A283" s="2" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="284" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A284" s="3" t="s">
-        <v>257</v>
+      <c r="A284" s="2" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="285" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A285" s="3" t="s">
-        <v>258</v>
+      <c r="A285" s="2" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="286" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A286" s="3" t="s">
-        <v>259</v>
+      <c r="A286" s="2" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="287" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A287" s="3" t="s">
-        <v>260</v>
+      <c r="A287" s="2" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="288" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A288" s="2" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="289" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="289" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A289" s="2" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="290" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="290" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A290" s="2" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="291" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="291" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A291" s="2" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="292" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="292" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A292" s="2" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="293" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="293" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A293" s="2" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="294" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="294" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A294" s="2" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="295" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="295" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A295" s="2" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="296" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A296" s="2" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="297" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A297" s="2" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="298" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="296" spans="1:4" s="59" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A296" s="58"/>
+    </row>
+    <row r="297" spans="1:4" s="38" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A297" s="39" t="s">
+        <v>1138</v>
+      </c>
+      <c r="B297" s="30" t="s">
+        <v>1116</v>
+      </c>
+      <c r="C297" s="30" t="s">
+        <v>1117</v>
+      </c>
+      <c r="D297" s="30" t="s">
+        <v>1118</v>
+      </c>
+    </row>
+    <row r="298" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A298" s="2" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="299" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="299" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A299" s="2" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="300" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="300" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A300" s="2" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="301" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="301" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A301" s="2" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="302" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="302" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A302" s="2" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="303" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="303" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A303" s="2" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="304" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="304" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A304" s="2" t="s">
-        <v>277</v>
+        <v>327</v>
       </c>
     </row>
     <row r="305" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A305" s="2" t="s">
-        <v>278</v>
+        <v>328</v>
       </c>
     </row>
     <row r="306" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A306" s="2" t="s">
-        <v>279</v>
+      <c r="A306" s="3" t="s">
+        <v>329</v>
       </c>
     </row>
     <row r="307" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A307" s="2" t="s">
-        <v>280</v>
+        <v>330</v>
       </c>
     </row>
     <row r="308" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A308" s="2" t="s">
-        <v>281</v>
+        <v>331</v>
       </c>
     </row>
     <row r="309" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A309" s="2" t="s">
-        <v>282</v>
+        <v>332</v>
       </c>
     </row>
     <row r="310" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A310" s="2" t="s">
-        <v>283</v>
+        <v>333</v>
       </c>
     </row>
     <row r="311" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A311" s="2" t="s">
-        <v>284</v>
+        <v>334</v>
       </c>
     </row>
     <row r="312" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A312" s="2" t="s">
-        <v>285</v>
+        <v>335</v>
       </c>
     </row>
     <row r="313" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A313" s="2" t="s">
-        <v>286</v>
+        <v>336</v>
       </c>
     </row>
     <row r="314" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A314" s="2" t="s">
-        <v>287</v>
+        <v>337</v>
       </c>
     </row>
     <row r="315" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A315" s="2" t="s">
-        <v>288</v>
+        <v>338</v>
       </c>
     </row>
     <row r="316" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A316" s="2" t="s">
-        <v>289</v>
+        <v>339</v>
       </c>
     </row>
     <row r="317" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A317" s="2" t="s">
-        <v>290</v>
+        <v>340</v>
       </c>
     </row>
     <row r="318" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A318" s="2" t="s">
-        <v>291</v>
+        <v>341</v>
       </c>
     </row>
     <row r="319" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A319" s="2" t="s">
-        <v>292</v>
+        <v>342</v>
       </c>
     </row>
     <row r="320" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A320" s="2" t="s">
-        <v>293</v>
+        <v>343</v>
       </c>
     </row>
     <row r="321" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A321" s="2" t="s">
-        <v>294</v>
+        <v>344</v>
       </c>
     </row>
     <row r="322" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A322" s="2" t="s">
-        <v>295</v>
+        <v>345</v>
       </c>
     </row>
     <row r="323" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A323" s="2" t="s">
-        <v>296</v>
+        <v>346</v>
       </c>
     </row>
     <row r="324" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A324" s="2" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="325" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A325" s="2" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="326" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A326" s="2" t="s">
-        <v>299</v>
-      </c>
+        <v>347</v>
+      </c>
+    </row>
+    <row r="325" spans="1:1" s="45" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A325" s="2"/>
+    </row>
+    <row r="326" spans="1:1" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A326" s="28"/>
     </row>
     <row r="327" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A327" s="2" t="s">
-        <v>300</v>
+        <v>248</v>
       </c>
     </row>
     <row r="328" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A328" s="2" t="s">
-        <v>301</v>
+        <v>249</v>
       </c>
     </row>
     <row r="329" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A329" s="2" t="s">
-        <v>302</v>
+        <v>250</v>
       </c>
     </row>
     <row r="330" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A330" s="2" t="s">
-        <v>303</v>
+        <v>251</v>
       </c>
     </row>
     <row r="331" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A331" s="2" t="s">
-        <v>304</v>
+        <v>252</v>
       </c>
     </row>
     <row r="332" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A332" s="2" t="s">
-        <v>305</v>
+        <v>253</v>
       </c>
     </row>
     <row r="333" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A333" s="2" t="s">
-        <v>306</v>
+      <c r="A333" s="3" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="334" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A334" s="2" t="s">
-        <v>307</v>
+      <c r="A334" s="3" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="335" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A335" s="2" t="s">
-        <v>308</v>
+      <c r="A335" s="3" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="336" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A336" s="2" t="s">
-        <v>309</v>
+      <c r="A336" s="3" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="337" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A337" s="2" t="s">
-        <v>310</v>
+      <c r="A337" s="3" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="338" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A338" s="2" t="s">
-        <v>311</v>
+      <c r="A338" s="3" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="339" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A339" s="2" t="s">
-        <v>312</v>
+      <c r="A339" s="3" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="340" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A340" s="2" t="s">
-        <v>313</v>
+        <v>261</v>
       </c>
     </row>
     <row r="341" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A341" s="2" t="s">
-        <v>314</v>
+        <v>262</v>
       </c>
     </row>
     <row r="342" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A342" s="2" t="s">
-        <v>315</v>
+        <v>263</v>
       </c>
     </row>
     <row r="343" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A343" s="2" t="s">
-        <v>316</v>
+        <v>264</v>
       </c>
     </row>
     <row r="344" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A344" s="2" t="s">
-        <v>317</v>
+        <v>265</v>
       </c>
     </row>
     <row r="345" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A345" s="2" t="s">
-        <v>318</v>
+        <v>266</v>
       </c>
     </row>
     <row r="346" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A346" s="2" t="s">
-        <v>319</v>
+        <v>267</v>
       </c>
     </row>
     <row r="347" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A347" s="2" t="s">
-        <v>320</v>
+        <v>268</v>
       </c>
     </row>
     <row r="348" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A348" s="2" t="s">
-        <v>321</v>
+        <v>269</v>
       </c>
     </row>
     <row r="349" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A349" s="2" t="s">
-        <v>322</v>
+        <v>270</v>
       </c>
     </row>
     <row r="350" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A350" s="2" t="s">
-        <v>323</v>
+        <v>271</v>
       </c>
     </row>
     <row r="351" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A351" s="2" t="s">
-        <v>324</v>
+        <v>272</v>
       </c>
     </row>
     <row r="352" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A352" s="2" t="s">
-        <v>325</v>
+        <v>273</v>
       </c>
     </row>
     <row r="353" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A353" s="2" t="s">
-        <v>326</v>
+        <v>274</v>
       </c>
     </row>
     <row r="354" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A354" s="2" t="s">
-        <v>327</v>
+        <v>275</v>
       </c>
     </row>
     <row r="355" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A355" s="2" t="s">
-        <v>328</v>
+        <v>276</v>
       </c>
     </row>
     <row r="356" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A356" s="3" t="s">
-        <v>329</v>
+      <c r="A356" s="2" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="357" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A357" s="2" t="s">
-        <v>330</v>
+        <v>278</v>
       </c>
     </row>
     <row r="358" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A358" s="2" t="s">
-        <v>331</v>
+        <v>279</v>
       </c>
     </row>
     <row r="359" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A359" s="2" t="s">
-        <v>332</v>
+        <v>280</v>
       </c>
     </row>
     <row r="360" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A360" s="2" t="s">
-        <v>333</v>
+        <v>281</v>
       </c>
     </row>
     <row r="361" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A361" s="2" t="s">
-        <v>334</v>
+        <v>282</v>
       </c>
     </row>
     <row r="362" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A362" s="2" t="s">
-        <v>335</v>
+        <v>283</v>
       </c>
     </row>
     <row r="363" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A363" s="2" t="s">
-        <v>336</v>
+        <v>284</v>
       </c>
     </row>
     <row r="364" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A364" s="2" t="s">
-        <v>337</v>
+        <v>285</v>
       </c>
     </row>
     <row r="365" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A365" s="2" t="s">
-        <v>338</v>
+        <v>286</v>
       </c>
     </row>
     <row r="366" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A366" s="2" t="s">
-        <v>339</v>
+        <v>287</v>
       </c>
     </row>
     <row r="367" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A367" s="2" t="s">
-        <v>340</v>
+        <v>288</v>
       </c>
     </row>
     <row r="368" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A368" s="2" t="s">
-        <v>341</v>
+        <v>289</v>
       </c>
     </row>
     <row r="369" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A369" s="2" t="s">
-        <v>342</v>
+        <v>290</v>
       </c>
     </row>
     <row r="370" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A370" s="2" t="s">
-        <v>343</v>
+        <v>291</v>
       </c>
     </row>
     <row r="371" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A371" s="2" t="s">
-        <v>344</v>
+        <v>292</v>
       </c>
     </row>
     <row r="372" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A372" s="2" t="s">
-        <v>345</v>
+        <v>293</v>
       </c>
     </row>
     <row r="373" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A373" s="2" t="s">
-        <v>346</v>
+        <v>294</v>
       </c>
     </row>
     <row r="374" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A374" s="2" t="s">
-        <v>347</v>
+        <v>295</v>
       </c>
     </row>
     <row r="375" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A375" s="2" t="s">
-        <v>348</v>
+        <v>296</v>
       </c>
     </row>
     <row r="376" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A376" s="2" t="s">
-        <v>349</v>
+        <v>297</v>
       </c>
     </row>
     <row r="377" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A377" s="2" t="s">
-        <v>350</v>
+        <v>298</v>
       </c>
     </row>
     <row r="378" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A378" s="2" t="s">
-        <v>351</v>
+        <v>299</v>
       </c>
     </row>
     <row r="379" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A379" s="2" t="s">
-        <v>352</v>
+        <v>300</v>
       </c>
     </row>
     <row r="380" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A380" s="2" t="s">
-        <v>353</v>
+        <v>301</v>
       </c>
     </row>
     <row r="381" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A381" s="2" t="s">
-        <v>354</v>
+        <v>302</v>
       </c>
     </row>
     <row r="382" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A382" s="2" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="383" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A383" s="2" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="384" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A384" s="2" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="385" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A385" s="2" t="s">
-        <v>358</v>
-      </c>
+        <v>303</v>
+      </c>
+    </row>
+    <row r="383" spans="1:1" s="45" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A383" s="2"/>
+    </row>
+    <row r="384" spans="1:1" s="45" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A384" s="2"/>
+    </row>
+    <row r="385" spans="1:1" s="45" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A385" s="2"/>
     </row>
     <row r="386" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A386" s="2" t="s">
-        <v>359</v>
+        <v>348</v>
       </c>
     </row>
     <row r="387" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A387" s="2" t="s">
-        <v>360</v>
+        <v>349</v>
       </c>
     </row>
     <row r="388" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A388" s="2" t="s">
-        <v>361</v>
+        <v>350</v>
       </c>
     </row>
     <row r="389" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A389" s="2" t="s">
-        <v>362</v>
+        <v>351</v>
       </c>
     </row>
     <row r="390" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A390" s="2" t="s">
-        <v>363</v>
+        <v>352</v>
       </c>
     </row>
     <row r="391" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A391" s="2" t="s">
-        <v>364</v>
+        <v>353</v>
       </c>
     </row>
     <row r="392" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A392" s="2" t="s">
-        <v>365</v>
+        <v>354</v>
       </c>
     </row>
     <row r="393" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A393" s="2" t="s">
-        <v>366</v>
+        <v>355</v>
       </c>
     </row>
     <row r="394" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A394" s="2" t="s">
-        <v>367</v>
+        <v>356</v>
       </c>
     </row>
     <row r="395" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A395" s="2" t="s">
-        <v>368</v>
+        <v>357</v>
       </c>
     </row>
     <row r="396" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A396" s="2" t="s">
-        <v>369</v>
+        <v>358</v>
       </c>
     </row>
     <row r="397" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A397" s="2" t="s">
-        <v>370</v>
+        <v>359</v>
       </c>
     </row>
     <row r="398" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A398" s="2" t="s">
-        <v>371</v>
+        <v>360</v>
       </c>
     </row>
     <row r="399" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A399" s="2" t="s">
-        <v>372</v>
+        <v>361</v>
       </c>
     </row>
     <row r="400" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A400" s="2" t="s">
-        <v>373</v>
+        <v>362</v>
       </c>
     </row>
     <row r="401" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A401" s="2" t="s">
-        <v>374</v>
+        <v>363</v>
       </c>
     </row>
     <row r="402" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A402" s="2" t="s">
-        <v>375</v>
+        <v>364</v>
       </c>
     </row>
     <row r="403" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A403" s="2" t="s">
-        <v>376</v>
+        <v>365</v>
       </c>
     </row>
     <row r="404" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A404" s="2" t="s">
-        <v>377</v>
+        <v>366</v>
       </c>
     </row>
     <row r="405" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A405" s="2" t="s">
-        <v>378</v>
+        <v>367</v>
       </c>
     </row>
     <row r="406" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A406" s="2" t="s">
-        <v>379</v>
+        <v>368</v>
       </c>
     </row>
     <row r="407" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A407" s="2" t="s">
-        <v>380</v>
+        <v>369</v>
       </c>
     </row>
     <row r="408" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A408" s="2" t="s">
-        <v>381</v>
+        <v>370</v>
       </c>
     </row>
     <row r="409" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A409" s="2" t="s">
-        <v>382</v>
+        <v>371</v>
       </c>
     </row>
     <row r="410" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A410" s="2" t="s">
-        <v>383</v>
+        <v>372</v>
       </c>
     </row>
     <row r="411" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A411" s="2" t="s">
-        <v>384</v>
+        <v>373</v>
       </c>
     </row>
     <row r="412" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A412" s="2" t="s">
-        <v>385</v>
+        <v>374</v>
       </c>
     </row>
     <row r="413" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A413" s="2" t="s">
-        <v>386</v>
+        <v>375</v>
       </c>
     </row>
     <row r="414" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A414" s="2" t="s">
-        <v>387</v>
+        <v>376</v>
       </c>
     </row>
     <row r="415" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A415" s="2" t="s">
-        <v>388</v>
+        <v>377</v>
       </c>
     </row>
     <row r="416" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A416" s="2" t="s">
-        <v>389</v>
+        <v>378</v>
       </c>
     </row>
     <row r="417" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A417" s="2" t="s">
-        <v>390</v>
+        <v>379</v>
       </c>
     </row>
     <row r="418" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A418" s="2" t="s">
-        <v>391</v>
+        <v>380</v>
       </c>
     </row>
     <row r="419" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A419" s="2" t="s">
-        <v>392</v>
+        <v>381</v>
       </c>
     </row>
     <row r="420" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A420" s="2" t="s">
-        <v>393</v>
+        <v>382</v>
       </c>
     </row>
     <row r="421" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A421" s="2" t="s">
-        <v>394</v>
+        <v>383</v>
       </c>
     </row>
     <row r="422" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A422" s="2" t="s">
-        <v>395</v>
+        <v>384</v>
       </c>
     </row>
     <row r="423" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A423" s="2" t="s">
-        <v>396</v>
+        <v>385</v>
       </c>
     </row>
     <row r="424" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A424" s="2" t="s">
-        <v>397</v>
+        <v>386</v>
       </c>
     </row>
     <row r="425" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A425" s="2" t="s">
-        <v>398</v>
+        <v>387</v>
       </c>
     </row>
     <row r="426" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A426" s="2" t="s">
-        <v>399</v>
+        <v>388</v>
       </c>
     </row>
     <row r="427" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A427" s="2" t="s">
-        <v>400</v>
+        <v>389</v>
       </c>
     </row>
     <row r="428" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A428" s="2" t="s">
-        <v>401</v>
+        <v>390</v>
       </c>
     </row>
     <row r="429" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A429" s="2" t="s">
-        <v>402</v>
+        <v>391</v>
       </c>
     </row>
     <row r="430" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A430" s="2" t="s">
-        <v>403</v>
+        <v>392</v>
       </c>
     </row>
     <row r="431" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A431" s="2" t="s">
-        <v>404</v>
+        <v>393</v>
       </c>
     </row>
     <row r="432" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A432" s="2" t="s">
-        <v>405</v>
+        <v>394</v>
       </c>
     </row>
     <row r="433" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A433" s="2" t="s">
-        <v>406</v>
+        <v>395</v>
       </c>
     </row>
     <row r="434" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A434" s="2" t="s">
-        <v>407</v>
+        <v>396</v>
       </c>
     </row>
     <row r="435" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A435" s="2" t="s">
-        <v>408</v>
+        <v>397</v>
       </c>
     </row>
     <row r="436" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A436" s="2" t="s">
-        <v>409</v>
+        <v>398</v>
       </c>
     </row>
     <row r="437" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A437" s="2" t="s">
-        <v>410</v>
+        <v>399</v>
       </c>
     </row>
     <row r="438" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A438" s="2" t="s">
-        <v>411</v>
+        <v>400</v>
       </c>
     </row>
     <row r="439" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A439" s="2" t="s">
-        <v>412</v>
+        <v>401</v>
       </c>
     </row>
     <row r="440" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A440" s="2" t="s">
-        <v>413</v>
+        <v>402</v>
       </c>
     </row>
     <row r="441" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A441" s="2" t="s">
-        <v>414</v>
+        <v>403</v>
       </c>
     </row>
     <row r="442" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A442" s="2" t="s">
-        <v>415</v>
+        <v>404</v>
       </c>
     </row>
     <row r="443" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A443" s="2" t="s">
-        <v>416</v>
+        <v>405</v>
       </c>
     </row>
     <row r="444" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A444" s="2" t="s">
-        <v>417</v>
+        <v>406</v>
       </c>
     </row>
     <row r="445" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A445" s="2" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
     </row>
     <row r="446" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A446" s="2" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
     </row>
     <row r="447" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A447" s="2" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
     </row>
     <row r="448" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A448" s="2" t="s">
-        <v>421</v>
+        <v>410</v>
       </c>
     </row>
     <row r="449" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A449" s="2" t="s">
-        <v>422</v>
+        <v>411</v>
       </c>
     </row>
     <row r="450" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A450" s="2" t="s">
-        <v>423</v>
+        <v>412</v>
       </c>
     </row>
     <row r="451" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A451" s="2" t="s">
-        <v>424</v>
+        <v>413</v>
       </c>
     </row>
     <row r="452" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A452" s="2" t="s">
-        <v>425</v>
+        <v>414</v>
       </c>
     </row>
     <row r="453" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A453" s="2" t="s">
-        <v>426</v>
+        <v>415</v>
       </c>
     </row>
     <row r="454" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A454" s="2" t="s">
-        <v>427</v>
+        <v>416</v>
       </c>
     </row>
     <row r="455" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A455" s="2" t="s">
-        <v>428</v>
+        <v>417</v>
       </c>
     </row>
     <row r="456" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A456" s="2" t="s">
-        <v>429</v>
+        <v>418</v>
       </c>
     </row>
     <row r="457" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A457" s="2" t="s">
-        <v>430</v>
+        <v>419</v>
       </c>
     </row>
     <row r="458" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A458" s="2" t="s">
-        <v>431</v>
+        <v>420</v>
       </c>
     </row>
     <row r="459" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A459" s="2" t="s">
-        <v>432</v>
+        <v>421</v>
       </c>
     </row>
     <row r="460" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A460" s="2" t="s">
-        <v>433</v>
+        <v>422</v>
       </c>
     </row>
     <row r="461" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A461" s="2" t="s">
-        <v>434</v>
+        <v>423</v>
       </c>
     </row>
     <row r="462" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A462" s="2" t="s">
-        <v>435</v>
+        <v>424</v>
       </c>
     </row>
     <row r="463" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A463" s="2" t="s">
-        <v>436</v>
+        <v>425</v>
       </c>
     </row>
     <row r="464" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A464" s="2" t="s">
-        <v>437</v>
+        <v>426</v>
       </c>
     </row>
     <row r="465" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A465" s="2" t="s">
-        <v>438</v>
+        <v>427</v>
       </c>
     </row>
     <row r="466" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A466" s="2" t="s">
-        <v>439</v>
+        <v>428</v>
       </c>
     </row>
     <row r="467" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A467" s="2" t="s">
-        <v>440</v>
+        <v>429</v>
       </c>
     </row>
     <row r="468" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A468" s="2" t="s">
-        <v>441</v>
+        <v>430</v>
       </c>
     </row>
     <row r="469" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A469" s="2" t="s">
-        <v>442</v>
+        <v>431</v>
       </c>
     </row>
     <row r="470" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A470" s="2" t="s">
-        <v>443</v>
+        <v>432</v>
       </c>
     </row>
     <row r="471" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A471" s="2" t="s">
-        <v>444</v>
+        <v>433</v>
       </c>
     </row>
     <row r="472" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A472" s="2" t="s">
-        <v>445</v>
+        <v>434</v>
       </c>
     </row>
     <row r="473" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A473" s="2" t="s">
-        <v>446</v>
+        <v>435</v>
       </c>
     </row>
     <row r="474" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A474" s="2" t="s">
-        <v>447</v>
+        <v>436</v>
       </c>
     </row>
     <row r="475" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A475" s="2" t="s">
-        <v>448</v>
+        <v>437</v>
       </c>
     </row>
     <row r="476" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A476" s="2" t="s">
-        <v>449</v>
+        <v>438</v>
       </c>
     </row>
     <row r="477" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A477" s="2" t="s">
-        <v>450</v>
+        <v>439</v>
       </c>
     </row>
     <row r="478" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A478" s="2" t="s">
-        <v>451</v>
+        <v>440</v>
       </c>
     </row>
     <row r="479" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A479" s="2" t="s">
-        <v>452</v>
+        <v>441</v>
       </c>
     </row>
     <row r="480" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A480" s="2" t="s">
-        <v>453</v>
+        <v>442</v>
       </c>
     </row>
     <row r="481" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A481" s="2" t="s">
-        <v>454</v>
+        <v>443</v>
       </c>
     </row>
     <row r="482" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A482" s="2" t="s">
-        <v>455</v>
+        <v>444</v>
       </c>
     </row>
     <row r="483" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A483" s="2" t="s">
-        <v>456</v>
+        <v>445</v>
       </c>
     </row>
     <row r="484" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A484" s="2" t="s">
-        <v>457</v>
+        <v>446</v>
       </c>
     </row>
     <row r="485" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A485" s="2" t="s">
-        <v>458</v>
+        <v>447</v>
       </c>
     </row>
     <row r="486" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A486" s="2" t="s">
-        <v>459</v>
+        <v>448</v>
       </c>
     </row>
     <row r="487" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A487" s="2" t="s">
-        <v>460</v>
+        <v>449</v>
       </c>
     </row>
     <row r="488" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A488" s="2" t="s">
-        <v>461</v>
+        <v>450</v>
       </c>
     </row>
     <row r="489" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A489" s="2" t="s">
-        <v>462</v>
+        <v>451</v>
       </c>
     </row>
     <row r="490" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A490" s="2" t="s">
-        <v>463</v>
+        <v>452</v>
       </c>
     </row>
     <row r="491" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A491" s="2" t="s">
-        <v>464</v>
+        <v>453</v>
       </c>
     </row>
     <row r="492" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A492" s="2" t="s">
-        <v>465</v>
+        <v>454</v>
       </c>
     </row>
     <row r="493" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A493" s="2" t="s">
-        <v>466</v>
+        <v>455</v>
       </c>
     </row>
     <row r="494" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A494" s="2" t="s">
-        <v>467</v>
+        <v>456</v>
       </c>
     </row>
     <row r="495" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A495" s="2" t="s">
-        <v>468</v>
+        <v>457</v>
       </c>
     </row>
     <row r="496" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A496" s="2" t="s">
-        <v>469</v>
+        <v>458</v>
       </c>
     </row>
     <row r="497" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A497" s="2" t="s">
-        <v>470</v>
+        <v>459</v>
       </c>
     </row>
     <row r="498" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A498" s="2" t="s">
-        <v>471</v>
+        <v>460</v>
       </c>
     </row>
     <row r="499" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A499" s="2" t="s">
-        <v>472</v>
+        <v>461</v>
       </c>
     </row>
     <row r="500" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A500" s="2" t="s">
-        <v>473</v>
+        <v>462</v>
       </c>
     </row>
     <row r="501" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A501" s="2" t="s">
-        <v>474</v>
+        <v>463</v>
       </c>
     </row>
     <row r="502" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A502" s="2" t="s">
-        <v>475</v>
+        <v>464</v>
       </c>
     </row>
     <row r="503" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A503" s="2" t="s">
-        <v>476</v>
+        <v>465</v>
       </c>
     </row>
     <row r="504" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A504" s="2" t="s">
-        <v>477</v>
+        <v>466</v>
       </c>
     </row>
     <row r="505" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A505" s="2" t="s">
-        <v>478</v>
+        <v>467</v>
       </c>
     </row>
     <row r="506" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A506" s="2" t="s">
-        <v>479</v>
+        <v>468</v>
       </c>
     </row>
     <row r="507" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A507" s="2" t="s">
-        <v>480</v>
+        <v>469</v>
       </c>
     </row>
     <row r="508" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A508" s="2" t="s">
-        <v>481</v>
+        <v>470</v>
       </c>
     </row>
     <row r="509" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A509" s="2" t="s">
-        <v>482</v>
+        <v>471</v>
       </c>
     </row>
     <row r="510" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A510" s="2" t="s">
-        <v>483</v>
+        <v>472</v>
       </c>
     </row>
     <row r="511" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A511" s="2" t="s">
-        <v>484</v>
+        <v>473</v>
       </c>
     </row>
     <row r="512" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A512" s="2" t="s">
-        <v>485</v>
+        <v>474</v>
       </c>
     </row>
     <row r="513" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A513" s="2" t="s">
-        <v>486</v>
+        <v>475</v>
       </c>
     </row>
     <row r="514" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A514" s="2" t="s">
-        <v>487</v>
+        <v>476</v>
       </c>
     </row>
     <row r="515" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A515" s="2" t="s">
-        <v>488</v>
+        <v>477</v>
       </c>
     </row>
     <row r="516" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A516" s="2" t="s">
-        <v>489</v>
+        <v>478</v>
       </c>
     </row>
     <row r="517" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A517" s="2" t="s">
-        <v>490</v>
+        <v>479</v>
       </c>
     </row>
     <row r="518" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A518" s="2" t="s">
-        <v>491</v>
+        <v>480</v>
       </c>
     </row>
     <row r="519" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A519" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
     </row>
     <row r="520" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A520" s="2" t="s">
-        <v>493</v>
+        <v>482</v>
       </c>
     </row>
     <row r="521" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A521" s="2" t="s">
-        <v>494</v>
+        <v>483</v>
       </c>
     </row>
     <row r="522" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A522" s="2" t="s">
-        <v>495</v>
+        <v>484</v>
       </c>
     </row>
     <row r="523" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A523" s="2" t="s">
-        <v>496</v>
+        <v>485</v>
       </c>
     </row>
     <row r="524" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A524" s="2" t="s">
-        <v>497</v>
+        <v>486</v>
       </c>
     </row>
     <row r="525" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A525" s="2" t="s">
-        <v>498</v>
+        <v>487</v>
       </c>
     </row>
     <row r="526" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A526" s="2" t="s">
-        <v>499</v>
+        <v>488</v>
       </c>
     </row>
     <row r="527" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A527" s="2" t="s">
-        <v>500</v>
+        <v>489</v>
       </c>
     </row>
     <row r="528" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A528" s="2" t="s">
-        <v>501</v>
+        <v>490</v>
       </c>
     </row>
     <row r="529" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A529" s="2" t="s">
-        <v>502</v>
+        <v>491</v>
       </c>
     </row>
     <row r="530" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A530" s="2" t="s">
-        <v>503</v>
+        <v>492</v>
       </c>
     </row>
     <row r="531" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A531" s="2" t="s">
-        <v>504</v>
+        <v>493</v>
       </c>
     </row>
     <row r="532" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A532" s="2" t="s">
-        <v>505</v>
+        <v>494</v>
       </c>
     </row>
     <row r="533" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A533" s="2" t="s">
-        <v>506</v>
+        <v>495</v>
       </c>
     </row>
     <row r="534" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A534" s="2" t="s">
-        <v>507</v>
+        <v>496</v>
       </c>
     </row>
     <row r="535" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A535" s="2" t="s">
-        <v>508</v>
+        <v>497</v>
       </c>
     </row>
     <row r="536" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A536" s="2" t="s">
-        <v>509</v>
+        <v>498</v>
       </c>
     </row>
     <row r="537" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A537" s="2" t="s">
-        <v>510</v>
+        <v>499</v>
       </c>
     </row>
     <row r="538" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A538" s="2" t="s">
-        <v>511</v>
+        <v>500</v>
       </c>
     </row>
     <row r="539" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A539" s="2" t="s">
-        <v>512</v>
+        <v>501</v>
       </c>
     </row>
     <row r="540" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A540" s="2" t="s">
-        <v>513</v>
+        <v>502</v>
       </c>
     </row>
     <row r="541" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A541" s="2" t="s">
-        <v>514</v>
+        <v>503</v>
       </c>
     </row>
     <row r="542" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A542" s="2" t="s">
-        <v>515</v>
+        <v>504</v>
       </c>
     </row>
     <row r="543" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A543" s="2" t="s">
-        <v>516</v>
+        <v>505</v>
       </c>
     </row>
     <row r="544" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A544" s="2" t="s">
-        <v>517</v>
+        <v>506</v>
       </c>
     </row>
     <row r="545" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A545" s="2" t="s">
-        <v>518</v>
+        <v>507</v>
       </c>
     </row>
     <row r="546" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A546" s="2" t="s">
-        <v>519</v>
+        <v>508</v>
       </c>
     </row>
     <row r="547" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A547" s="2" t="s">
-        <v>520</v>
+        <v>509</v>
       </c>
     </row>
     <row r="548" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A548" s="2" t="s">
-        <v>521</v>
+        <v>510</v>
       </c>
     </row>
     <row r="549" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A549" s="2" t="s">
-        <v>522</v>
+        <v>511</v>
       </c>
     </row>
     <row r="550" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A550" s="2" t="s">
-        <v>523</v>
+        <v>512</v>
       </c>
     </row>
     <row r="551" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A551" s="2" t="s">
-        <v>524</v>
+        <v>513</v>
       </c>
     </row>
     <row r="552" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A552" s="2" t="s">
-        <v>525</v>
+        <v>514</v>
       </c>
     </row>
     <row r="553" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A553" s="2" t="s">
-        <v>526</v>
+        <v>515</v>
       </c>
     </row>
     <row r="554" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A554" s="2" t="s">
-        <v>527</v>
+        <v>516</v>
       </c>
     </row>
     <row r="555" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A555" s="2" t="s">
-        <v>528</v>
+        <v>517</v>
       </c>
     </row>
     <row r="556" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A556" s="2" t="s">
-        <v>529</v>
+        <v>518</v>
       </c>
     </row>
     <row r="557" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A557" s="2" t="s">
-        <v>530</v>
+        <v>519</v>
       </c>
     </row>
     <row r="558" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A558" s="2" t="s">
-        <v>531</v>
+        <v>520</v>
       </c>
     </row>
     <row r="559" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A559" s="2" t="s">
-        <v>532</v>
+        <v>521</v>
       </c>
     </row>
     <row r="560" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A560" s="2" t="s">
-        <v>533</v>
+        <v>522</v>
       </c>
     </row>
     <row r="561" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A561" s="2" t="s">
-        <v>534</v>
+        <v>523</v>
       </c>
     </row>
     <row r="562" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A562" s="2" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="563" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A563" s="2" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="564" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A564" s="2" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="565" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A565" s="2" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="566" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A566" s="2" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="567" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A567" s="2" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="568" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A568" s="2" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="569" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A569" s="2" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="570" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A570" s="2" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="571" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A571" s="2" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="572" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A572" s="2" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="573" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A573" s="2" t="s">
         <v>535</v>
       </c>
     </row>
-    <row r="563" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A563" s="3" t="s">
+    <row r="574" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A574" s="3" t="s">
         <v>536</v>
       </c>
     </row>
-    <row r="564" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A564" s="3" t="s">
+    <row r="575" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A575" s="3" t="s">
         <v>537</v>
       </c>
     </row>
-    <row r="565" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A565" s="3" t="s">
+    <row r="576" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A576" s="3" t="s">
         <v>538</v>
       </c>
     </row>
-    <row r="566" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A566" s="3" t="s">
+    <row r="577" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A577" s="3" t="s">
         <v>539</v>
       </c>
     </row>
-    <row r="567" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A567" s="3" t="s">
+    <row r="578" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A578" s="3" t="s">
         <v>540</v>
       </c>
     </row>
-    <row r="568" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A568" s="3" t="s">
+    <row r="579" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A579" s="3" t="s">
         <v>541</v>
       </c>
     </row>
-    <row r="569" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A569" s="3" t="s">
+    <row r="580" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A580" s="3" t="s">
         <v>542</v>
       </c>
     </row>
-    <row r="570" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A570" s="3" t="s">
+    <row r="581" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A581" s="3" t="s">
         <v>543</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated FJP xlsx and completed Recursion and Backtracking Level1
</commit_message>
<xml_diff>
--- a/Level_1/First Job Program With Web Development.xlsx
+++ b/Level_1/First Job Program With Web Development.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\Nados\LearnDSA\Level_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24CFEA99-9ACB-4C4C-81D3-A1AA7536ABE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABB61C06-5040-4A05-A913-6819DC11B7DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4812" yWindow="348" windowWidth="17184" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DSA" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1317" uniqueCount="1143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1333" uniqueCount="1145">
   <si>
     <t>Print Z</t>
   </si>
@@ -3483,6 +3483,12 @@
   </si>
   <si>
     <t>5.4 Graphs</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Hard</t>
   </si>
 </sst>
 </file>
@@ -3609,7 +3615,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="20">
+  <fills count="22">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3724,6 +3730,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -3789,7 +3807,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -3858,18 +3876,18 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3878,14 +3896,18 @@
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4106,8 +4128,8 @@
   </sheetPr>
   <dimension ref="A1:D581"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
-      <selection activeCell="A300" sqref="A300"/>
+    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
+      <selection activeCell="F113" sqref="F113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4667,8 +4689,8 @@
         <v>71</v>
       </c>
     </row>
-    <row r="80" spans="1:1" s="59" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A80" s="58"/>
+    <row r="80" spans="1:1" s="47" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A80" s="46"/>
     </row>
     <row r="81" spans="1:4" s="38" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="39" t="s">
@@ -5099,24 +5121,64 @@
       <c r="A112" s="2" t="s">
         <v>97</v>
       </c>
+      <c r="B112" s="35" t="s">
+        <v>1119</v>
+      </c>
+      <c r="C112" s="33">
+        <f>DATE(2022,2,6)+32</f>
+        <v>44630</v>
+      </c>
+      <c r="D112" s="32" t="s">
+        <v>1120</v>
+      </c>
     </row>
     <row r="113" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A113" s="2" t="s">
+      <c r="A113" s="41" t="s">
         <v>98</v>
       </c>
+      <c r="B113" s="51" t="s">
+        <v>1119</v>
+      </c>
+      <c r="C113" s="33">
+        <f t="shared" ref="C113:C115" si="8">DATE(2022,2,6)+32</f>
+        <v>44630</v>
+      </c>
+      <c r="D113" s="32" t="s">
+        <v>1120</v>
+      </c>
     </row>
     <row r="114" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A114" s="2" t="s">
+      <c r="A114" s="41" t="s">
         <v>99</v>
       </c>
+      <c r="B114" s="51" t="s">
+        <v>1119</v>
+      </c>
+      <c r="C114" s="33">
+        <f t="shared" si="8"/>
+        <v>44630</v>
+      </c>
+      <c r="D114" s="32" t="s">
+        <v>1120</v>
+      </c>
     </row>
     <row r="115" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A115" s="2" t="s">
+      <c r="A115" s="41" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="116" spans="1:4" s="59" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A116" s="58"/>
+      <c r="B115" s="51" t="s">
+        <v>1119</v>
+      </c>
+      <c r="C115" s="33">
+        <f t="shared" si="8"/>
+        <v>44630</v>
+      </c>
+      <c r="D115" s="32" t="s">
+        <v>1120</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" s="47" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A116" s="46"/>
     </row>
     <row r="117" spans="1:4" s="38" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A117" s="39" t="s">
@@ -5202,8 +5264,8 @@
         <v>114</v>
       </c>
     </row>
-    <row r="132" spans="1:4" s="59" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A132" s="58"/>
+    <row r="132" spans="1:4" s="47" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A132" s="46"/>
     </row>
     <row r="133" spans="1:4" s="38" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A133" s="39" t="s">
@@ -5228,7 +5290,7 @@
       <c r="D134" s="30"/>
     </row>
     <row r="135" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A135" s="2" t="s">
+      <c r="A135" s="41" t="s">
         <v>115</v>
       </c>
       <c r="B135" s="34" t="s">
@@ -5243,29 +5305,73 @@
       </c>
     </row>
     <row r="136" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A136" s="2" t="s">
+      <c r="A136" s="48" t="s">
         <v>116</v>
+      </c>
+      <c r="B136" s="35" t="s">
+        <v>1119</v>
+      </c>
+      <c r="C136" s="33">
+        <f>DATE(2022,2,6)+30</f>
+        <v>44628</v>
+      </c>
+      <c r="D136" s="32" t="s">
+        <v>1120</v>
       </c>
     </row>
     <row r="137" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
         <v>117</v>
       </c>
+      <c r="B137" s="49" t="s">
+        <v>1143</v>
+      </c>
+      <c r="C137" s="33">
+        <f t="shared" ref="C137:C140" si="9">DATE(2022,2,6)+30</f>
+        <v>44628</v>
+      </c>
+      <c r="D137" s="32" t="s">
+        <v>1120</v>
+      </c>
     </row>
     <row r="138" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A138" s="2" t="s">
+      <c r="A138" s="41" t="s">
         <v>118</v>
       </c>
+      <c r="B138" s="35" t="s">
+        <v>1119</v>
+      </c>
+      <c r="C138" s="33">
+        <f t="shared" si="9"/>
+        <v>44628</v>
+      </c>
+      <c r="D138" s="32" t="s">
+        <v>1120</v>
+      </c>
     </row>
     <row r="139" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A139" s="2" t="s">
+      <c r="A139" s="41" t="s">
         <v>119</v>
+      </c>
+      <c r="B139" s="50" t="s">
+        <v>1144</v>
+      </c>
+      <c r="C139" s="33">
+        <f t="shared" si="9"/>
+        <v>44628</v>
+      </c>
+      <c r="D139" s="32" t="s">
+        <v>1120</v>
       </c>
     </row>
     <row r="140" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
         <v>120</v>
       </c>
+      <c r="C140" s="33">
+        <f t="shared" si="9"/>
+        <v>44628</v>
+      </c>
     </row>
     <row r="141" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
@@ -5857,8 +5963,8 @@
         <v>233</v>
       </c>
     </row>
-    <row r="259" spans="1:4" s="59" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A259" s="58"/>
+    <row r="259" spans="1:4" s="47" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A259" s="46"/>
     </row>
     <row r="260" spans="1:4" s="38" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A260" s="39" t="s">
@@ -6052,8 +6158,8 @@
         <v>320</v>
       </c>
     </row>
-    <row r="296" spans="1:4" s="59" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A296" s="58"/>
+    <row r="296" spans="1:4" s="47" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A296" s="46"/>
     </row>
     <row r="297" spans="1:4" s="38" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A297" s="39" t="s">
@@ -7505,7 +7611,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="60" t="s">
         <v>544</v>
       </c>
       <c r="B1" s="4" t="s">
@@ -7517,7 +7623,7 @@
       <c r="D1" s="2"/>
     </row>
     <row r="2" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A2" s="47"/>
+      <c r="A2" s="53"/>
       <c r="B2" s="6" t="s">
         <v>547</v>
       </c>
@@ -7527,7 +7633,7 @@
       <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A3" s="47"/>
+      <c r="A3" s="53"/>
       <c r="B3" s="6" t="s">
         <v>547</v>
       </c>
@@ -7537,7 +7643,7 @@
       <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A4" s="47"/>
+      <c r="A4" s="53"/>
       <c r="B4" s="6" t="s">
         <v>547</v>
       </c>
@@ -7547,29 +7653,29 @@
       <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A5" s="47"/>
+      <c r="A5" s="53"/>
       <c r="B5" s="6" t="s">
         <v>551</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>552</v>
       </c>
-      <c r="D5" s="48" t="s">
+      <c r="D5" s="52" t="s">
         <v>553</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A6" s="47"/>
+      <c r="A6" s="53"/>
       <c r="B6" s="6" t="s">
         <v>551</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>554</v>
       </c>
-      <c r="D6" s="47"/>
+      <c r="D6" s="53"/>
     </row>
     <row r="7" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A7" s="47"/>
+      <c r="A7" s="53"/>
       <c r="B7" s="9" t="s">
         <v>555</v>
       </c>
@@ -7579,7 +7685,7 @@
       <c r="D7" s="10"/>
     </row>
     <row r="8" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A8" s="47"/>
+      <c r="A8" s="53"/>
       <c r="B8" s="2" t="s">
         <v>557</v>
       </c>
@@ -7589,39 +7695,39 @@
       <c r="D8" s="10"/>
     </row>
     <row r="9" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A9" s="47"/>
+      <c r="A9" s="53"/>
       <c r="B9" s="6" t="s">
         <v>559</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>560</v>
       </c>
-      <c r="D9" s="48" t="s">
+      <c r="D9" s="52" t="s">
         <v>561</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A10" s="47"/>
+      <c r="A10" s="53"/>
       <c r="B10" s="6" t="s">
         <v>559</v>
       </c>
       <c r="C10" s="12" t="s">
         <v>562</v>
       </c>
-      <c r="D10" s="47"/>
+      <c r="D10" s="53"/>
     </row>
     <row r="11" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A11" s="47"/>
+      <c r="A11" s="53"/>
       <c r="B11" s="6" t="s">
         <v>559</v>
       </c>
       <c r="C11" s="12" t="s">
         <v>563</v>
       </c>
-      <c r="D11" s="47"/>
+      <c r="D11" s="53"/>
     </row>
     <row r="12" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A12" s="47"/>
+      <c r="A12" s="53"/>
       <c r="B12" s="9" t="s">
         <v>564</v>
       </c>
@@ -7631,39 +7737,39 @@
       <c r="D12" s="10"/>
     </row>
     <row r="13" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A13" s="47"/>
+      <c r="A13" s="53"/>
       <c r="B13" s="6" t="s">
         <v>566</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>567</v>
       </c>
-      <c r="D13" s="48" t="s">
+      <c r="D13" s="52" t="s">
         <v>568</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A14" s="47"/>
+      <c r="A14" s="53"/>
       <c r="B14" s="6" t="s">
         <v>566</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>569</v>
       </c>
-      <c r="D14" s="47"/>
+      <c r="D14" s="53"/>
     </row>
     <row r="15" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A15" s="47"/>
+      <c r="A15" s="53"/>
       <c r="B15" s="6" t="s">
         <v>566</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>569</v>
       </c>
-      <c r="D15" s="47"/>
+      <c r="D15" s="53"/>
     </row>
     <row r="16" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A16" s="47"/>
+      <c r="A16" s="53"/>
       <c r="B16" s="9" t="s">
         <v>570</v>
       </c>
@@ -7673,7 +7779,7 @@
       <c r="D16" s="2"/>
     </row>
     <row r="17" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A17" s="47"/>
+      <c r="A17" s="53"/>
       <c r="B17" s="6" t="s">
         <v>566</v>
       </c>
@@ -7683,7 +7789,7 @@
       <c r="D17" s="10"/>
     </row>
     <row r="18" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A18" s="47"/>
+      <c r="A18" s="53"/>
       <c r="B18" s="6" t="s">
         <v>566</v>
       </c>
@@ -7693,7 +7799,7 @@
       <c r="D18" s="10"/>
     </row>
     <row r="19" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A19" s="47"/>
+      <c r="A19" s="53"/>
       <c r="B19" s="9" t="s">
         <v>574</v>
       </c>
@@ -7703,7 +7809,7 @@
       <c r="D19" s="10"/>
     </row>
     <row r="20" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A20" s="47"/>
+      <c r="A20" s="53"/>
       <c r="B20" s="2" t="s">
         <v>557</v>
       </c>
@@ -7713,7 +7819,7 @@
       <c r="D20" s="10"/>
     </row>
     <row r="21" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A21" s="46" t="s">
+      <c r="A21" s="57" t="s">
         <v>577</v>
       </c>
       <c r="B21" s="6" t="s">
@@ -7725,7 +7831,7 @@
       <c r="D21" s="2"/>
     </row>
     <row r="22" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A22" s="47"/>
+      <c r="A22" s="53"/>
       <c r="B22" s="6" t="s">
         <v>578</v>
       </c>
@@ -7735,7 +7841,7 @@
       <c r="D22" s="2"/>
     </row>
     <row r="23" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A23" s="47"/>
+      <c r="A23" s="53"/>
       <c r="B23" s="6" t="s">
         <v>578</v>
       </c>
@@ -7745,7 +7851,7 @@
       <c r="D23" s="2"/>
     </row>
     <row r="24" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A24" s="47"/>
+      <c r="A24" s="53"/>
       <c r="B24" s="10" t="s">
         <v>582</v>
       </c>
@@ -7755,37 +7861,37 @@
       <c r="D24" s="2"/>
     </row>
     <row r="25" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A25" s="47"/>
+      <c r="A25" s="53"/>
       <c r="B25" s="13" t="s">
         <v>584</v>
       </c>
       <c r="C25" s="7"/>
-      <c r="D25" s="49" t="s">
+      <c r="D25" s="54" t="s">
         <v>585</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A26" s="47"/>
+      <c r="A26" s="53"/>
       <c r="B26" s="6" t="s">
         <v>584</v>
       </c>
       <c r="C26" s="7" t="s">
         <v>586</v>
       </c>
-      <c r="D26" s="50"/>
+      <c r="D26" s="55"/>
     </row>
     <row r="27" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A27" s="47"/>
+      <c r="A27" s="53"/>
       <c r="B27" s="6" t="s">
         <v>584</v>
       </c>
       <c r="C27" s="7" t="s">
         <v>587</v>
       </c>
-      <c r="D27" s="51"/>
+      <c r="D27" s="56"/>
     </row>
     <row r="28" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A28" s="47"/>
+      <c r="A28" s="53"/>
       <c r="B28" s="2" t="s">
         <v>582</v>
       </c>
@@ -7795,39 +7901,39 @@
       <c r="D28" s="2"/>
     </row>
     <row r="29" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A29" s="47"/>
+      <c r="A29" s="53"/>
       <c r="B29" s="6" t="s">
         <v>589</v>
       </c>
       <c r="C29" s="7" t="s">
         <v>590</v>
       </c>
-      <c r="D29" s="48" t="s">
+      <c r="D29" s="52" t="s">
         <v>591</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A30" s="47"/>
+      <c r="A30" s="53"/>
       <c r="B30" s="6" t="s">
         <v>589</v>
       </c>
       <c r="C30" s="7" t="s">
         <v>592</v>
       </c>
-      <c r="D30" s="47"/>
+      <c r="D30" s="53"/>
     </row>
     <row r="31" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A31" s="47"/>
+      <c r="A31" s="53"/>
       <c r="B31" s="6" t="s">
         <v>589</v>
       </c>
       <c r="C31" s="7" t="s">
         <v>593</v>
       </c>
-      <c r="D31" s="47"/>
+      <c r="D31" s="53"/>
     </row>
     <row r="32" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A32" s="47"/>
+      <c r="A32" s="53"/>
       <c r="B32" s="6" t="s">
         <v>594</v>
       </c>
@@ -7837,7 +7943,7 @@
       <c r="D32" s="2"/>
     </row>
     <row r="33" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A33" s="47"/>
+      <c r="A33" s="53"/>
       <c r="B33" s="2" t="s">
         <v>596</v>
       </c>
@@ -7847,39 +7953,39 @@
       <c r="D33" s="2"/>
     </row>
     <row r="34" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A34" s="47"/>
+      <c r="A34" s="53"/>
       <c r="B34" s="6" t="s">
         <v>598</v>
       </c>
       <c r="C34" s="7" t="s">
         <v>599</v>
       </c>
-      <c r="D34" s="49" t="s">
+      <c r="D34" s="54" t="s">
         <v>600</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A35" s="47"/>
+      <c r="A35" s="53"/>
       <c r="B35" s="6" t="s">
         <v>598</v>
       </c>
       <c r="C35" s="7" t="s">
         <v>601</v>
       </c>
-      <c r="D35" s="50"/>
+      <c r="D35" s="55"/>
     </row>
     <row r="36" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A36" s="47"/>
+      <c r="A36" s="53"/>
       <c r="B36" s="6" t="s">
         <v>598</v>
       </c>
       <c r="C36" s="7" t="s">
         <v>602</v>
       </c>
-      <c r="D36" s="51"/>
+      <c r="D36" s="56"/>
     </row>
     <row r="37" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A37" s="47"/>
+      <c r="A37" s="53"/>
       <c r="B37" s="6" t="s">
         <v>598</v>
       </c>
@@ -7889,7 +7995,7 @@
       <c r="D37" s="2"/>
     </row>
     <row r="38" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A38" s="47"/>
+      <c r="A38" s="53"/>
       <c r="B38" s="2" t="s">
         <v>582</v>
       </c>
@@ -7899,7 +8005,7 @@
       <c r="D38" s="2"/>
     </row>
     <row r="39" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A39" s="47"/>
+      <c r="A39" s="53"/>
       <c r="B39" s="9" t="s">
         <v>605</v>
       </c>
@@ -7909,7 +8015,7 @@
       <c r="D39" s="2"/>
     </row>
     <row r="40" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A40" s="54" t="s">
+      <c r="A40" s="58" t="s">
         <v>607</v>
       </c>
       <c r="B40" s="6" t="s">
@@ -7921,7 +8027,7 @@
       <c r="D40" s="2"/>
     </row>
     <row r="41" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A41" s="47"/>
+      <c r="A41" s="53"/>
       <c r="B41" s="6" t="s">
         <v>608</v>
       </c>
@@ -7931,7 +8037,7 @@
       <c r="D41" s="2"/>
     </row>
     <row r="42" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A42" s="47"/>
+      <c r="A42" s="53"/>
       <c r="B42" s="6" t="s">
         <v>608</v>
       </c>
@@ -7941,51 +8047,51 @@
       <c r="D42" s="2"/>
     </row>
     <row r="43" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A43" s="47"/>
+      <c r="A43" s="53"/>
       <c r="B43" s="6" t="s">
         <v>612</v>
       </c>
       <c r="C43" s="7"/>
-      <c r="D43" s="48" t="s">
+      <c r="D43" s="52" t="s">
         <v>613</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A44" s="47"/>
+      <c r="A44" s="53"/>
       <c r="B44" s="6" t="s">
         <v>612</v>
       </c>
       <c r="C44" s="7"/>
-      <c r="D44" s="47"/>
+      <c r="D44" s="53"/>
     </row>
     <row r="45" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A45" s="47"/>
+      <c r="A45" s="53"/>
       <c r="B45" s="6" t="s">
         <v>612</v>
       </c>
       <c r="C45" s="7"/>
-      <c r="D45" s="47"/>
+      <c r="D45" s="53"/>
     </row>
     <row r="46" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A46" s="47"/>
+      <c r="A46" s="53"/>
       <c r="B46" s="6" t="s">
         <v>612</v>
       </c>
       <c r="C46" s="7"/>
-      <c r="D46" s="47"/>
+      <c r="D46" s="53"/>
     </row>
     <row r="47" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A47" s="47"/>
+      <c r="A47" s="53"/>
       <c r="B47" s="6" t="s">
         <v>614</v>
       </c>
       <c r="C47" s="7" t="s">
         <v>615</v>
       </c>
-      <c r="D47" s="47"/>
+      <c r="D47" s="53"/>
     </row>
     <row r="48" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A48" s="47"/>
+      <c r="A48" s="53"/>
       <c r="B48" s="6" t="s">
         <v>614</v>
       </c>
@@ -7995,7 +8101,7 @@
       <c r="D48" s="2"/>
     </row>
     <row r="49" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A49" s="47"/>
+      <c r="A49" s="53"/>
       <c r="B49" s="6" t="s">
         <v>614</v>
       </c>
@@ -8005,7 +8111,7 @@
       <c r="D49" s="2"/>
     </row>
     <row r="50" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A50" s="47"/>
+      <c r="A50" s="53"/>
       <c r="B50" s="2" t="s">
         <v>618</v>
       </c>
@@ -8013,57 +8119,57 @@
       <c r="D50" s="2"/>
     </row>
     <row r="51" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A51" s="47"/>
+      <c r="A51" s="53"/>
       <c r="B51" s="6" t="s">
         <v>619</v>
       </c>
       <c r="C51" s="7"/>
-      <c r="D51" s="49" t="s">
+      <c r="D51" s="54" t="s">
         <v>620</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A52" s="47"/>
+      <c r="A52" s="53"/>
       <c r="B52" s="6" t="s">
         <v>619</v>
       </c>
       <c r="C52" s="7"/>
-      <c r="D52" s="50"/>
+      <c r="D52" s="55"/>
     </row>
     <row r="53" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A53" s="47"/>
+      <c r="A53" s="53"/>
       <c r="B53" s="6" t="s">
         <v>619</v>
       </c>
       <c r="C53" s="7"/>
-      <c r="D53" s="50"/>
+      <c r="D53" s="55"/>
     </row>
     <row r="54" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A54" s="47"/>
+      <c r="A54" s="53"/>
       <c r="B54" s="6" t="s">
         <v>619</v>
       </c>
       <c r="C54" s="7"/>
-      <c r="D54" s="50"/>
+      <c r="D54" s="55"/>
     </row>
     <row r="55" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A55" s="47"/>
+      <c r="A55" s="53"/>
       <c r="B55" s="6" t="s">
         <v>619</v>
       </c>
       <c r="C55" s="7"/>
-      <c r="D55" s="50"/>
+      <c r="D55" s="55"/>
     </row>
     <row r="56" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A56" s="47"/>
+      <c r="A56" s="53"/>
       <c r="B56" s="6" t="s">
         <v>619</v>
       </c>
       <c r="C56" s="7"/>
-      <c r="D56" s="51"/>
+      <c r="D56" s="56"/>
     </row>
     <row r="57" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A57" s="47"/>
+      <c r="A57" s="53"/>
       <c r="B57" s="6" t="s">
         <v>621</v>
       </c>
@@ -8073,7 +8179,7 @@
       <c r="D57" s="2"/>
     </row>
     <row r="58" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A58" s="47"/>
+      <c r="A58" s="53"/>
       <c r="B58" s="6" t="s">
         <v>621</v>
       </c>
@@ -8083,7 +8189,7 @@
       <c r="D58" s="2"/>
     </row>
     <row r="59" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A59" s="47"/>
+      <c r="A59" s="53"/>
       <c r="B59" s="6" t="s">
         <v>621</v>
       </c>
@@ -8095,33 +8201,33 @@
       </c>
     </row>
     <row r="60" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A60" s="47"/>
+      <c r="A60" s="53"/>
       <c r="B60" s="6" t="s">
         <v>626</v>
       </c>
       <c r="C60" s="7"/>
-      <c r="D60" s="48" t="s">
+      <c r="D60" s="52" t="s">
         <v>627</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A61" s="47"/>
+      <c r="A61" s="53"/>
       <c r="B61" s="6" t="s">
         <v>626</v>
       </c>
       <c r="C61" s="7"/>
-      <c r="D61" s="47"/>
+      <c r="D61" s="53"/>
     </row>
     <row r="62" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A62" s="47"/>
+      <c r="A62" s="53"/>
       <c r="B62" s="6" t="s">
         <v>626</v>
       </c>
       <c r="C62" s="7"/>
-      <c r="D62" s="47"/>
+      <c r="D62" s="53"/>
     </row>
     <row r="63" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A63" s="47"/>
+      <c r="A63" s="53"/>
       <c r="B63" s="6" t="s">
         <v>626</v>
       </c>
@@ -8129,7 +8235,7 @@
       <c r="D63" s="8"/>
     </row>
     <row r="64" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A64" s="55" t="s">
+      <c r="A64" s="59" t="s">
         <v>628</v>
       </c>
       <c r="B64" s="9" t="s">
@@ -8139,7 +8245,7 @@
       <c r="D64" s="8"/>
     </row>
     <row r="65" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A65" s="47"/>
+      <c r="A65" s="53"/>
       <c r="B65" s="9" t="s">
         <v>629</v>
       </c>
@@ -8147,7 +8253,7 @@
       <c r="D65" s="2"/>
     </row>
     <row r="66" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A66" s="47"/>
+      <c r="A66" s="53"/>
       <c r="B66" s="9" t="s">
         <v>629</v>
       </c>
@@ -8155,7 +8261,7 @@
       <c r="D66" s="2"/>
     </row>
     <row r="67" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A67" s="47"/>
+      <c r="A67" s="53"/>
       <c r="B67" s="9" t="s">
         <v>629</v>
       </c>
@@ -8163,7 +8269,7 @@
       <c r="D67" s="2"/>
     </row>
     <row r="68" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A68" s="47"/>
+      <c r="A68" s="53"/>
       <c r="B68" s="9" t="s">
         <v>630</v>
       </c>
@@ -8171,7 +8277,7 @@
       <c r="D68" s="2"/>
     </row>
     <row r="69" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A69" s="47"/>
+      <c r="A69" s="53"/>
       <c r="B69" s="9" t="s">
         <v>630</v>
       </c>
@@ -8179,7 +8285,7 @@
       <c r="D69" s="2"/>
     </row>
     <row r="70" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A70" s="47"/>
+      <c r="A70" s="53"/>
       <c r="B70" s="9" t="s">
         <v>630</v>
       </c>
@@ -8187,7 +8293,7 @@
       <c r="D70" s="2"/>
     </row>
     <row r="71" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A71" s="47"/>
+      <c r="A71" s="53"/>
       <c r="B71" s="9" t="s">
         <v>630</v>
       </c>
@@ -8195,7 +8301,7 @@
       <c r="D71" s="2"/>
     </row>
     <row r="72" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A72" s="47"/>
+      <c r="A72" s="53"/>
       <c r="B72" s="9" t="s">
         <v>631</v>
       </c>
@@ -8203,7 +8309,7 @@
       <c r="D72" s="2"/>
     </row>
     <row r="73" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A73" s="47"/>
+      <c r="A73" s="53"/>
       <c r="B73" s="9" t="s">
         <v>631</v>
       </c>
@@ -8211,7 +8317,7 @@
       <c r="D73" s="2"/>
     </row>
     <row r="74" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A74" s="47"/>
+      <c r="A74" s="53"/>
       <c r="B74" s="9" t="s">
         <v>631</v>
       </c>
@@ -8219,7 +8325,7 @@
       <c r="D74" s="2"/>
     </row>
     <row r="75" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A75" s="52" t="s">
+      <c r="A75" s="61" t="s">
         <v>632</v>
       </c>
       <c r="B75" s="6" t="s">
@@ -8228,32 +8334,32 @@
       <c r="C75" s="7" t="s">
         <v>634</v>
       </c>
-      <c r="D75" s="48" t="s">
+      <c r="D75" s="52" t="s">
         <v>635</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A76" s="47"/>
+      <c r="A76" s="53"/>
       <c r="B76" s="6" t="s">
         <v>633</v>
       </c>
       <c r="C76" s="7" t="s">
         <v>636</v>
       </c>
-      <c r="D76" s="47"/>
+      <c r="D76" s="53"/>
     </row>
     <row r="77" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A77" s="47"/>
+      <c r="A77" s="53"/>
       <c r="B77" s="6" t="s">
         <v>633</v>
       </c>
       <c r="C77" s="7" t="s">
         <v>637</v>
       </c>
-      <c r="D77" s="47"/>
+      <c r="D77" s="53"/>
     </row>
     <row r="78" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A78" s="47"/>
+      <c r="A78" s="53"/>
       <c r="B78" s="6" t="s">
         <v>633</v>
       </c>
@@ -8263,7 +8369,7 @@
       <c r="D78" s="2"/>
     </row>
     <row r="79" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A79" s="47"/>
+      <c r="A79" s="53"/>
       <c r="B79" s="6" t="s">
         <v>633</v>
       </c>
@@ -8273,7 +8379,7 @@
       <c r="D79" s="2"/>
     </row>
     <row r="80" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A80" s="47"/>
+      <c r="A80" s="53"/>
       <c r="B80" s="6" t="s">
         <v>633</v>
       </c>
@@ -8283,7 +8389,7 @@
       <c r="D80" s="2"/>
     </row>
     <row r="81" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A81" s="47"/>
+      <c r="A81" s="53"/>
       <c r="B81" s="6" t="s">
         <v>633</v>
       </c>
@@ -8293,7 +8399,7 @@
       <c r="D81" s="2"/>
     </row>
     <row r="82" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A82" s="47"/>
+      <c r="A82" s="53"/>
       <c r="B82" s="6" t="s">
         <v>633</v>
       </c>
@@ -8303,7 +8409,7 @@
       <c r="D82" s="2"/>
     </row>
     <row r="83" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A83" s="47"/>
+      <c r="A83" s="53"/>
       <c r="B83" s="6" t="s">
         <v>633</v>
       </c>
@@ -8313,7 +8419,7 @@
       <c r="D83" s="2"/>
     </row>
     <row r="84" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A84" s="47"/>
+      <c r="A84" s="53"/>
       <c r="B84" s="6" t="s">
         <v>633</v>
       </c>
@@ -8323,7 +8429,7 @@
       <c r="D84" s="2"/>
     </row>
     <row r="85" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A85" s="47"/>
+      <c r="A85" s="53"/>
       <c r="B85" s="6" t="s">
         <v>633</v>
       </c>
@@ -8333,7 +8439,7 @@
       <c r="D85" s="2"/>
     </row>
     <row r="86" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A86" s="47"/>
+      <c r="A86" s="53"/>
       <c r="B86" s="6" t="s">
         <v>633</v>
       </c>
@@ -8343,7 +8449,7 @@
       <c r="D86" s="2"/>
     </row>
     <row r="87" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A87" s="47"/>
+      <c r="A87" s="53"/>
       <c r="B87" s="6" t="s">
         <v>647</v>
       </c>
@@ -8353,7 +8459,7 @@
       <c r="D87" s="2"/>
     </row>
     <row r="88" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A88" s="47"/>
+      <c r="A88" s="53"/>
       <c r="B88" s="6" t="s">
         <v>647</v>
       </c>
@@ -8363,7 +8469,7 @@
       <c r="D88" s="2"/>
     </row>
     <row r="89" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A89" s="47"/>
+      <c r="A89" s="53"/>
       <c r="B89" s="6" t="s">
         <v>647</v>
       </c>
@@ -8373,7 +8479,7 @@
       <c r="D89" s="2"/>
     </row>
     <row r="90" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A90" s="47"/>
+      <c r="A90" s="53"/>
       <c r="B90" s="6" t="s">
         <v>647</v>
       </c>
@@ -8383,7 +8489,7 @@
       <c r="D90" s="2"/>
     </row>
     <row r="91" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A91" s="47"/>
+      <c r="A91" s="53"/>
       <c r="B91" s="6" t="s">
         <v>647</v>
       </c>
@@ -8393,7 +8499,7 @@
       <c r="D91" s="10"/>
     </row>
     <row r="92" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A92" s="47"/>
+      <c r="A92" s="53"/>
       <c r="B92" s="14" t="s">
         <v>647</v>
       </c>
@@ -8403,7 +8509,7 @@
       <c r="D92" s="10"/>
     </row>
     <row r="93" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A93" s="47"/>
+      <c r="A93" s="53"/>
       <c r="B93" s="6" t="s">
         <v>647</v>
       </c>
@@ -8413,7 +8519,7 @@
       <c r="D93" s="2"/>
     </row>
     <row r="94" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A94" s="47"/>
+      <c r="A94" s="53"/>
       <c r="B94" s="6" t="s">
         <v>647</v>
       </c>
@@ -8423,7 +8529,7 @@
       <c r="D94" s="2"/>
     </row>
     <row r="95" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A95" s="47"/>
+      <c r="A95" s="53"/>
       <c r="B95" s="6" t="s">
         <v>647</v>
       </c>
@@ -8433,7 +8539,7 @@
       <c r="D95" s="2"/>
     </row>
     <row r="96" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A96" s="47"/>
+      <c r="A96" s="53"/>
       <c r="B96" s="6" t="s">
         <v>657</v>
       </c>
@@ -8443,7 +8549,7 @@
       <c r="D96" s="2"/>
     </row>
     <row r="97" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A97" s="47"/>
+      <c r="A97" s="53"/>
       <c r="B97" s="6" t="s">
         <v>657</v>
       </c>
@@ -8453,7 +8559,7 @@
       <c r="D97" s="2"/>
     </row>
     <row r="98" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A98" s="47"/>
+      <c r="A98" s="53"/>
       <c r="B98" s="14" t="s">
         <v>657</v>
       </c>
@@ -8463,7 +8569,7 @@
       <c r="D98" s="2"/>
     </row>
     <row r="99" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A99" s="47"/>
+      <c r="A99" s="53"/>
       <c r="B99" s="16" t="s">
         <v>661</v>
       </c>
@@ -8471,7 +8577,7 @@
       <c r="D99" s="2"/>
     </row>
     <row r="100" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A100" s="47"/>
+      <c r="A100" s="53"/>
       <c r="B100" s="9" t="s">
         <v>661</v>
       </c>
@@ -8479,7 +8585,7 @@
       <c r="D100" s="2"/>
     </row>
     <row r="101" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A101" s="47"/>
+      <c r="A101" s="53"/>
       <c r="B101" s="9" t="s">
         <v>661</v>
       </c>
@@ -8487,7 +8593,7 @@
       <c r="D101" s="2"/>
     </row>
     <row r="102" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A102" s="47"/>
+      <c r="A102" s="53"/>
       <c r="B102" s="9" t="s">
         <v>661</v>
       </c>
@@ -8495,7 +8601,7 @@
       <c r="D102" s="2"/>
     </row>
     <row r="103" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A103" s="46" t="s">
+      <c r="A103" s="57" t="s">
         <v>662</v>
       </c>
       <c r="B103" s="6" t="s">
@@ -8507,7 +8613,7 @@
       <c r="D103" s="2"/>
     </row>
     <row r="104" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A104" s="47"/>
+      <c r="A104" s="53"/>
       <c r="B104" s="6" t="s">
         <v>663</v>
       </c>
@@ -8517,7 +8623,7 @@
       <c r="D104" s="2"/>
     </row>
     <row r="105" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A105" s="47"/>
+      <c r="A105" s="53"/>
       <c r="B105" s="6" t="s">
         <v>663</v>
       </c>
@@ -11213,22 +11319,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="D29:D31"/>
-    <mergeCell ref="D34:D36"/>
-    <mergeCell ref="A21:A39"/>
-    <mergeCell ref="A40:A63"/>
-    <mergeCell ref="A64:A74"/>
-    <mergeCell ref="A1:A20"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="D9:D11"/>
-    <mergeCell ref="D13:D15"/>
-    <mergeCell ref="D25:D27"/>
     <mergeCell ref="A103:A105"/>
     <mergeCell ref="D43:D47"/>
     <mergeCell ref="D51:D56"/>
     <mergeCell ref="D60:D62"/>
     <mergeCell ref="D75:D77"/>
     <mergeCell ref="A75:A102"/>
+    <mergeCell ref="A1:A20"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="D13:D15"/>
+    <mergeCell ref="D25:D27"/>
+    <mergeCell ref="D29:D31"/>
+    <mergeCell ref="D34:D36"/>
+    <mergeCell ref="A21:A39"/>
+    <mergeCell ref="A40:A63"/>
+    <mergeCell ref="A64:A74"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -14153,7 +14259,7 @@
       <c r="A2" s="2" t="s">
         <v>1086</v>
       </c>
-      <c r="B2" s="56" t="s">
+      <c r="B2" s="62" t="s">
         <v>1087</v>
       </c>
     </row>
@@ -14161,31 +14267,31 @@
       <c r="A3" s="2" t="s">
         <v>1088</v>
       </c>
-      <c r="B3" s="47"/>
+      <c r="B3" s="53"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>1089</v>
       </c>
-      <c r="B4" s="47"/>
+      <c r="B4" s="53"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>1090</v>
       </c>
-      <c r="B5" s="47"/>
+      <c r="B5" s="53"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>1091</v>
       </c>
-      <c r="B6" s="47"/>
+      <c r="B6" s="53"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>1092</v>
       </c>
-      <c r="B7" s="56" t="s">
+      <c r="B7" s="62" t="s">
         <v>1093</v>
       </c>
     </row>
@@ -14193,19 +14299,19 @@
       <c r="A8" s="2" t="s">
         <v>1094</v>
       </c>
-      <c r="B8" s="47"/>
+      <c r="B8" s="53"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>1095</v>
       </c>
-      <c r="B9" s="47"/>
+      <c r="B9" s="53"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>1096</v>
       </c>
-      <c r="B10" s="56" t="s">
+      <c r="B10" s="62" t="s">
         <v>1097</v>
       </c>
     </row>
@@ -14213,25 +14319,25 @@
       <c r="A11" s="2" t="s">
         <v>1098</v>
       </c>
-      <c r="B11" s="47"/>
+      <c r="B11" s="53"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>1099</v>
       </c>
-      <c r="B12" s="47"/>
+      <c r="B12" s="53"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>1100</v>
       </c>
-      <c r="B13" s="47"/>
+      <c r="B13" s="53"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>1101</v>
       </c>
-      <c r="B14" s="56" t="s">
+      <c r="B14" s="62" t="s">
         <v>1102</v>
       </c>
     </row>
@@ -14239,61 +14345,61 @@
       <c r="A15" s="2" t="s">
         <v>1103</v>
       </c>
-      <c r="B15" s="47"/>
+      <c r="B15" s="53"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>1104</v>
       </c>
-      <c r="B16" s="47"/>
+      <c r="B16" s="53"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>1105</v>
       </c>
-      <c r="B17" s="47"/>
+      <c r="B17" s="53"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>1106</v>
       </c>
-      <c r="B18" s="47"/>
+      <c r="B18" s="53"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>1107</v>
       </c>
-      <c r="B19" s="47"/>
+      <c r="B19" s="53"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>1108</v>
       </c>
-      <c r="B20" s="47"/>
+      <c r="B20" s="53"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>1109</v>
       </c>
-      <c r="B21" s="47"/>
+      <c r="B21" s="53"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>1110</v>
       </c>
-      <c r="B22" s="47"/>
+      <c r="B22" s="53"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>1111</v>
       </c>
-      <c r="B23" s="47"/>
+      <c r="B23" s="53"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>1112</v>
       </c>
-      <c r="B24" s="57" t="s">
+      <c r="B24" s="63" t="s">
         <v>1113</v>
       </c>
     </row>
@@ -14301,7 +14407,7 @@
       <c r="A25" s="2" t="s">
         <v>1114</v>
       </c>
-      <c r="B25" s="47"/>
+      <c r="B25" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
updated FJP on 27 March 2022 till Celebrity Problem
</commit_message>
<xml_diff>
--- a/Level_1/First Job Program With Web Development.xlsx
+++ b/Level_1/First Job Program With Web Development.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\Nados\LearnDSA\Level_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1A21B6A-2930-4ACE-A38C-75269635F9FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8520FE7D-AFAC-4D84-B71A-BB9FDDF4FDB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4812" yWindow="348" windowWidth="17184" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DSA" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1333" uniqueCount="1145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1345" uniqueCount="1145">
   <si>
     <t>Print Z</t>
   </si>
@@ -4128,8 +4128,8 @@
   </sheetPr>
   <dimension ref="A1:D581"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A131" workbookViewId="0">
-      <selection activeCell="C141" sqref="C141"/>
+    <sheetView tabSelected="1" topLeftCell="A125" workbookViewId="0">
+      <selection activeCell="G142" sqref="G142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5327,7 +5327,7 @@
         <v>1143</v>
       </c>
       <c r="C137" s="33">
-        <f t="shared" ref="C137:C140" si="9">DATE(2022,2,6)+30</f>
+        <f t="shared" ref="C137:C139" si="9">DATE(2022,2,6)+30</f>
         <v>44628</v>
       </c>
       <c r="D137" s="32" t="s">
@@ -5353,7 +5353,7 @@
       <c r="A139" s="41" t="s">
         <v>119</v>
       </c>
-      <c r="B139" s="50" t="s">
+      <c r="B139" s="48" t="s">
         <v>1144</v>
       </c>
       <c r="C139" s="33">
@@ -5365,110 +5365,166 @@
       </c>
     </row>
     <row r="140" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A140" s="2" t="s">
+      <c r="A140" s="48" t="s">
         <v>120</v>
       </c>
+      <c r="B140" s="50" t="s">
+        <v>1144</v>
+      </c>
       <c r="C140" s="33">
-        <f>DATE(2022,2,6)+32</f>
-        <v>44630</v>
+        <f>DATE(2022,2,6)+38</f>
+        <v>44636</v>
+      </c>
+      <c r="D140" s="32" t="s">
+        <v>1120</v>
       </c>
     </row>
     <row r="141" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A141" s="2" t="s">
+      <c r="A141" s="41" t="s">
         <v>121</v>
       </c>
+      <c r="B141" s="49" t="s">
+        <v>1143</v>
+      </c>
+      <c r="C141" s="33">
+        <f>DATE(2022,2,6)+49</f>
+        <v>44647</v>
+      </c>
+      <c r="D141" s="32" t="s">
+        <v>1120</v>
+      </c>
     </row>
     <row r="142" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A142" s="2" t="s">
+      <c r="A142" s="41" t="s">
         <v>122</v>
       </c>
+      <c r="B142" s="49" t="s">
+        <v>1143</v>
+      </c>
+      <c r="C142" s="33">
+        <f t="shared" ref="C142:C145" si="10">DATE(2022,2,6)+49</f>
+        <v>44647</v>
+      </c>
+      <c r="D142" s="32" t="s">
+        <v>1120</v>
+      </c>
     </row>
     <row r="143" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A143" s="2" t="s">
+      <c r="A143" s="48" t="s">
         <v>123</v>
       </c>
+      <c r="B143" s="49" t="s">
+        <v>1143</v>
+      </c>
+      <c r="C143" s="33">
+        <f t="shared" si="10"/>
+        <v>44647</v>
+      </c>
+      <c r="D143" s="32" t="s">
+        <v>1120</v>
+      </c>
     </row>
     <row r="144" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A144" s="2" t="s">
+      <c r="A144" s="48" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="145" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B144" s="49" t="s">
+        <v>1143</v>
+      </c>
+      <c r="C144" s="33">
+        <f t="shared" si="10"/>
+        <v>44647</v>
+      </c>
+      <c r="D144" s="32" t="s">
+        <v>1120</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="146" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B145" s="51" t="s">
+        <v>1119</v>
+      </c>
+      <c r="C145" s="33">
+        <f t="shared" si="10"/>
+        <v>44647</v>
+      </c>
+      <c r="D145" s="32" t="s">
+        <v>1120</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="147" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="148" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="149" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="150" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="151" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="152" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="153" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="154" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="155" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="156" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A156" s="43" t="s">
         <v>1133</v>
       </c>
     </row>
-    <row r="157" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="158" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="159" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="160" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
         <v>139</v>
       </c>

</xml_diff>